<commit_message>
ascii import and resample functions, e_map import
</commit_message>
<xml_diff>
--- a/output/xyz_age_eros.xlsx
+++ b/output/xyz_age_eros.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G180"/>
+  <dimension ref="A1:H180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -394,10 +394,15 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>E_map</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>E_exp_Z</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>E_inv_exp_Z</t>
         </is>
@@ -420,9 +425,12 @@
         <v>19.44814549592458</v>
       </c>
       <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="n">
         <v>1.71577234424401</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>24.54370929475012</v>
       </c>
     </row>
@@ -443,9 +451,12 @@
         <v>19.42737511200367</v>
       </c>
       <c r="F3" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3" t="n">
         <v>2.527187593999784</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>16.6633524686021</v>
       </c>
     </row>
@@ -466,9 +477,12 @@
         <v>18.25158525384342</v>
       </c>
       <c r="F4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" t="n">
         <v>1.513732700682522</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>27.81958638675733</v>
       </c>
     </row>
@@ -489,9 +503,12 @@
         <v>17.57794269205465</v>
       </c>
       <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
         <v>1.205371905865509</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>34.93645191843017</v>
       </c>
     </row>
@@ -515,6 +532,9 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
         <v>42.11141763309691</v>
       </c>
     </row>
@@ -535,9 +555,12 @@
         <v>22.10552016041226</v>
       </c>
       <c r="F7" t="n">
+        <v>10</v>
+      </c>
+      <c r="G7" t="n">
         <v>7.38905609893065</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>5.699160632870456</v>
       </c>
     </row>
@@ -558,9 +581,12 @@
         <v>19.94098590451998</v>
       </c>
       <c r="F8" t="n">
+        <v>10</v>
+      </c>
+      <c r="G8" t="n">
         <v>3.276540548249262</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>12.85240240826505</v>
       </c>
     </row>
@@ -581,9 +607,12 @@
         <v>17.91726158854982</v>
       </c>
       <c r="F9" t="n">
+        <v>10</v>
+      </c>
+      <c r="G9" t="n">
         <v>2.475904843525316</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>17.00849600226824</v>
       </c>
     </row>
@@ -604,9 +633,12 @@
         <v>16.4031851167013</v>
       </c>
       <c r="F10" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" t="n">
         <v>1.53806313144631</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>27.37951178473256</v>
       </c>
     </row>
@@ -627,9 +659,12 @@
         <v>15.8761488006341</v>
       </c>
       <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="n">
         <v>1.276007117771601</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>33.00249430163026</v>
       </c>
     </row>
@@ -650,9 +685,12 @@
         <v>16.3905221979472</v>
       </c>
       <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
         <v>1.136056031253367</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>37.06808156868549</v>
       </c>
     </row>
@@ -673,9 +711,12 @@
         <v>14.624167806468</v>
       </c>
       <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
         <v>1.763319615489954</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>23.88189711222369</v>
       </c>
     </row>
@@ -696,9 +737,12 @@
         <v>12.41957142851253</v>
       </c>
       <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
         <v>1.598791916034733</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>26.33952374336501</v>
       </c>
     </row>
@@ -719,9 +763,12 @@
         <v>10.95027980424291</v>
       </c>
       <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
         <v>1.650600155135878</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>25.51279151529602</v>
       </c>
     </row>
@@ -742,9 +789,12 @@
         <v>21.55571220228536</v>
       </c>
       <c r="F16" t="n">
+        <v>10</v>
+      </c>
+      <c r="G16" t="n">
         <v>11.05838613157211</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>3.808097956795633</v>
       </c>
     </row>
@@ -765,9 +815,12 @@
         <v>18.79606229671177</v>
       </c>
       <c r="F17" t="n">
+        <v>10</v>
+      </c>
+      <c r="G17" t="n">
         <v>4.326212651421302</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>9.734014720534354</v>
       </c>
     </row>
@@ -788,9 +841,12 @@
         <v>16.04933185726385</v>
       </c>
       <c r="F18" t="n">
+        <v>10</v>
+      </c>
+      <c r="G18" t="n">
         <v>2.338847564732744</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>18.00519976936116</v>
       </c>
     </row>
@@ -811,9 +867,12 @@
         <v>13.66571114707362</v>
       </c>
       <c r="F19" t="n">
+        <v>10</v>
+      </c>
+      <c r="G19" t="n">
         <v>1.858165995243492</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>22.66289327266409</v>
       </c>
     </row>
@@ -834,9 +893,12 @@
         <v>12.30121737342334</v>
       </c>
       <c r="F20" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" t="n">
         <v>1.338529674884737</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>31.46095183636717</v>
       </c>
     </row>
@@ -857,9 +919,12 @@
         <v>12.55771968397517</v>
       </c>
       <c r="F21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" t="n">
         <v>1.183605064314989</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>35.57894343538389</v>
       </c>
     </row>
@@ -880,9 +945,12 @@
         <v>11.59767603496123</v>
       </c>
       <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
         <v>1.213637280943926</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>34.6985201380301</v>
       </c>
     </row>
@@ -903,9 +971,12 @@
         <v>9.994557213448665</v>
       </c>
       <c r="F23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" t="n">
         <v>1.50000279342122</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>28.07422613997191</v>
       </c>
     </row>
@@ -926,9 +997,12 @@
         <v>8.8474161306303</v>
       </c>
       <c r="F24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" t="n">
         <v>1.631907262573603</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>25.80503108165902</v>
       </c>
     </row>
@@ -949,9 +1023,12 @@
         <v>8.505378346574808</v>
       </c>
       <c r="F25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" t="n">
         <v>2.270603279516831</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>18.54635638598123</v>
       </c>
     </row>
@@ -972,9 +1049,12 @@
         <v>9.194695305776342</v>
       </c>
       <c r="F26" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" t="n">
         <v>2.021565957079946</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>20.8310876455027</v>
       </c>
     </row>
@@ -995,9 +1075,12 @@
         <v>24.13843773696987</v>
       </c>
       <c r="F27" t="n">
+        <v>10</v>
+      </c>
+      <c r="G27" t="n">
         <v>17.40037969153265</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>2.42014360488864</v>
       </c>
     </row>
@@ -1018,9 +1101,12 @@
         <v>21.15022437317182</v>
       </c>
       <c r="F28" t="n">
+        <v>10</v>
+      </c>
+      <c r="G28" t="n">
         <v>9.070354874271228</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>4.642753036328187</v>
       </c>
     </row>
@@ -1041,9 +1127,12 @@
         <v>17.69736439597586</v>
       </c>
       <c r="F29" t="n">
+        <v>10</v>
+      </c>
+      <c r="G29" t="n">
         <v>4.238423330031359</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>9.935632746902924</v>
       </c>
     </row>
@@ -1064,9 +1153,12 @@
         <v>14.18733893389331</v>
       </c>
       <c r="F30" t="n">
+        <v>10</v>
+      </c>
+      <c r="G30" t="n">
         <v>2.755688790255169</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>15.28163041560201</v>
       </c>
     </row>
@@ -1087,9 +1179,12 @@
         <v>10.69072522154512</v>
       </c>
       <c r="F31" t="n">
+        <v>10</v>
+      </c>
+      <c r="G31" t="n">
         <v>1.743350185569119</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>24.15545538795442</v>
       </c>
     </row>
@@ -1110,9 +1205,12 @@
         <v>7.291418967993124</v>
       </c>
       <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
         <v>1.385055649403185</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>30.40413405139538</v>
       </c>
     </row>
@@ -1133,9 +1231,12 @@
         <v>7.020650996724029</v>
       </c>
       <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
         <v>1.545086238592975</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>27.25505967320339</v>
       </c>
     </row>
@@ -1156,9 +1257,12 @@
         <v>7.802485445938721</v>
       </c>
       <c r="F34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" t="n">
         <v>1.335484102423399</v>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>31.53269855978113</v>
       </c>
     </row>
@@ -1179,9 +1283,12 @@
         <v>7.421020149846687</v>
       </c>
       <c r="F35" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" t="n">
         <v>1.385055649403185</v>
       </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
         <v>30.40413405139538</v>
       </c>
     </row>
@@ -1202,9 +1309,12 @@
         <v>6.675092241598335</v>
       </c>
       <c r="F36" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" t="n">
         <v>1.503423550876351</v>
       </c>
-      <c r="G36" t="n">
+      <c r="H36" t="n">
         <v>28.01034851991644</v>
       </c>
     </row>
@@ -1225,9 +1335,12 @@
         <v>6.582101307937918</v>
       </c>
       <c r="F37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" t="n">
         <v>2.072860184000009</v>
       </c>
-      <c r="G37" t="n">
+      <c r="H37" t="n">
         <v>20.31560930068823</v>
       </c>
     </row>
@@ -1248,9 +1361,12 @@
         <v>8.175952479585597</v>
       </c>
       <c r="F38" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" t="n">
         <v>2.699769197680611</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>15.59815471236397</v>
       </c>
     </row>
@@ -1271,9 +1387,12 @@
         <v>10.96771296044583</v>
       </c>
       <c r="F39" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" t="n">
         <v>2.812766630296358</v>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>14.97152916260955</v>
       </c>
     </row>
@@ -1294,9 +1413,12 @@
         <v>13.60412706113798</v>
       </c>
       <c r="F40" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" t="n">
         <v>4.486796407757537</v>
       </c>
-      <c r="G40" t="n">
+      <c r="H40" t="n">
         <v>9.385631485370613</v>
       </c>
     </row>
@@ -1317,9 +1439,12 @@
         <v>15.28603010453255</v>
       </c>
       <c r="F41" t="n">
+        <v>1</v>
+      </c>
+      <c r="G41" t="n">
         <v>3.56466690612579</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>11.81356315809746</v>
       </c>
     </row>
@@ -1340,9 +1465,12 @@
         <v>20.69491044048138</v>
       </c>
       <c r="F42" t="n">
+        <v>10</v>
+      </c>
+      <c r="G42" t="n">
         <v>7.857774445006733</v>
       </c>
-      <c r="G42" t="n">
+      <c r="H42" t="n">
         <v>5.359204177699049</v>
       </c>
     </row>
@@ -1363,9 +1491,12 @@
         <v>16.67367378043709</v>
       </c>
       <c r="F43" t="n">
+        <v>10</v>
+      </c>
+      <c r="G43" t="n">
         <v>3.994689409680294</v>
       </c>
-      <c r="G43" t="n">
+      <c r="H43" t="n">
         <v>10.5418502702735</v>
       </c>
     </row>
@@ -1386,9 +1517,12 @@
         <v>12.81644328551365</v>
       </c>
       <c r="F44" t="n">
+        <v>10</v>
+      </c>
+      <c r="G44" t="n">
         <v>2.749418738833005</v>
       </c>
-      <c r="G44" t="n">
+      <c r="H44" t="n">
         <v>15.31648018481578</v>
       </c>
     </row>
@@ -1409,9 +1543,12 @@
         <v>9.097262961972582</v>
       </c>
       <c r="F45" t="n">
+        <v>10</v>
+      </c>
+      <c r="G45" t="n">
         <v>1.88373668613625</v>
       </c>
-      <c r="G45" t="n">
+      <c r="H45" t="n">
         <v>22.35525694383116</v>
       </c>
     </row>
@@ -1432,9 +1569,12 @@
         <v>5.649583491377424</v>
       </c>
       <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
         <v>1.510288486696439</v>
       </c>
-      <c r="G46" t="n">
+      <c r="H46" t="n">
         <v>27.88302897363019</v>
       </c>
     </row>
@@ -1455,9 +1595,12 @@
         <v>5.133228375596552</v>
       </c>
       <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
         <v>2.159618666600905</v>
       </c>
-      <c r="G47" t="n">
+      <c r="H47" t="n">
         <v>19.49946918146316</v>
       </c>
     </row>
@@ -1478,9 +1621,12 @@
         <v>6.075271503049112</v>
       </c>
       <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
         <v>1.755304540160127</v>
       </c>
-      <c r="G48" t="n">
+      <c r="H48" t="n">
         <v>23.99094668168255</v>
       </c>
     </row>
@@ -1501,9 +1647,12 @@
         <v>6.125135081063</v>
       </c>
       <c r="F49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" t="n">
         <v>1.433198821018947</v>
       </c>
-      <c r="G49" t="n">
+      <c r="H49" t="n">
         <v>29.38281626770903</v>
       </c>
     </row>
@@ -1524,9 +1673,12 @@
         <v>5.377752904058379</v>
       </c>
       <c r="F50" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" t="n">
         <v>1.658137129079801</v>
       </c>
-      <c r="G50" t="n">
+      <c r="H50" t="n">
         <v>25.39682448125809</v>
       </c>
     </row>
@@ -1547,9 +1699,12 @@
         <v>4.708031331374997</v>
       </c>
       <c r="F51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" t="n">
         <v>1.892338208604575</v>
       </c>
-      <c r="G51" t="n">
+      <c r="H51" t="n">
         <v>22.25364231489581</v>
       </c>
     </row>
@@ -1570,9 +1725,12 @@
         <v>7.636796552959012</v>
       </c>
       <c r="F52" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" t="n">
         <v>2.164543678531826</v>
       </c>
-      <c r="G52" t="n">
+      <c r="H52" t="n">
         <v>19.45510180772161</v>
       </c>
     </row>
@@ -1593,9 +1751,12 @@
         <v>12.52545734618108</v>
       </c>
       <c r="F53" t="n">
+        <v>1</v>
+      </c>
+      <c r="G53" t="n">
         <v>2.464650750021215</v>
       </c>
-      <c r="G53" t="n">
+      <c r="H53" t="n">
         <v>17.08616023293946</v>
       </c>
     </row>
@@ -1616,9 +1777,12 @@
         <v>16.44334941989044</v>
       </c>
       <c r="F54" t="n">
+        <v>1</v>
+      </c>
+      <c r="G54" t="n">
         <v>3.382715588569269</v>
       </c>
-      <c r="G54" t="n">
+      <c r="H54" t="n">
         <v>12.44899741952828</v>
       </c>
     </row>
@@ -1639,9 +1803,12 @@
         <v>18.79155910963738</v>
       </c>
       <c r="F55" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" t="n">
         <v>4.914819975131787</v>
       </c>
-      <c r="G55" t="n">
+      <c r="H55" t="n">
         <v>8.568252315684813</v>
       </c>
     </row>
@@ -1662,9 +1829,12 @@
         <v>19.33787702659292</v>
       </c>
       <c r="F56" t="n">
+        <v>2</v>
+      </c>
+      <c r="G56" t="n">
         <v>5.830471954825193</v>
       </c>
-      <c r="G56" t="n">
+      <c r="H56" t="n">
         <v>7.222643031195142</v>
       </c>
     </row>
@@ -1685,9 +1855,12 @@
         <v>17.90233860765787</v>
       </c>
       <c r="F57" t="n">
+        <v>2</v>
+      </c>
+      <c r="G57" t="n">
         <v>6.900976133077612</v>
       </c>
-      <c r="G57" t="n">
+      <c r="H57" t="n">
         <v>6.102240729575828</v>
       </c>
     </row>
@@ -1708,9 +1881,12 @@
         <v>19.49239248924531</v>
       </c>
       <c r="F58" t="n">
+        <v>10</v>
+      </c>
+      <c r="G58" t="n">
         <v>9.132551350533355</v>
       </c>
-      <c r="G58" t="n">
+      <c r="H58" t="n">
         <v>4.611133955533417</v>
       </c>
     </row>
@@ -1731,9 +1907,12 @@
         <v>15.53049095553061</v>
       </c>
       <c r="F59" t="n">
+        <v>10</v>
+      </c>
+      <c r="G59" t="n">
         <v>4.209557902844931</v>
       </c>
-      <c r="G59" t="n">
+      <c r="H59" t="n">
         <v>10.00376253397937</v>
       </c>
     </row>
@@ -1754,9 +1933,12 @@
         <v>11.90433764759585</v>
       </c>
       <c r="F60" t="n">
+        <v>10</v>
+      </c>
+      <c r="G60" t="n">
         <v>2.793610518686659</v>
       </c>
-      <c r="G60" t="n">
+      <c r="H60" t="n">
         <v>15.07419067597672</v>
       </c>
     </row>
@@ -1777,9 +1959,12 @@
         <v>8.922388874810878</v>
       </c>
       <c r="F61" t="n">
+        <v>10</v>
+      </c>
+      <c r="G61" t="n">
         <v>2.035428069511566</v>
       </c>
-      <c r="G61" t="n">
+      <c r="H61" t="n">
         <v>20.68921926737614</v>
       </c>
     </row>
@@ -1800,9 +1985,12 @@
         <v>7.01757063787479</v>
       </c>
       <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
         <v>1.692481677039882</v>
       </c>
-      <c r="G62" t="n">
+      <c r="H62" t="n">
         <v>24.88146146831497</v>
       </c>
     </row>
@@ -1823,9 +2011,12 @@
         <v>6.504981448738963</v>
       </c>
       <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
         <v>1.704087220363075</v>
       </c>
-      <c r="G63" t="n">
+      <c r="H63" t="n">
         <v>24.71200835842464</v>
       </c>
     </row>
@@ -1846,9 +2037,12 @@
         <v>6.785937840478056</v>
       </c>
       <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="n">
         <v>1.971541038015586</v>
       </c>
-      <c r="G64" t="n">
+      <c r="H64" t="n">
         <v>21.35964548599165</v>
       </c>
     </row>
@@ -1869,9 +2063,12 @@
         <v>6.998733141509192</v>
       </c>
       <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
         <v>1.980543492902473</v>
       </c>
-      <c r="G65" t="n">
+      <c r="H65" t="n">
         <v>21.26255635587326</v>
       </c>
     </row>
@@ -1892,9 +2089,12 @@
         <v>6.672968561304103</v>
       </c>
       <c r="F66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G66" t="n">
         <v>1.64684452500568</v>
       </c>
-      <c r="G66" t="n">
+      <c r="H66" t="n">
         <v>25.57097345479633</v>
       </c>
     </row>
@@ -1915,9 +2115,12 @@
         <v>5.815647967554202</v>
       </c>
       <c r="F67" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" t="n">
         <v>1.866650756768601</v>
       </c>
-      <c r="G67" t="n">
+      <c r="H67" t="n">
         <v>22.5598802991926</v>
       </c>
     </row>
@@ -1938,9 +2141,12 @@
         <v>10.14661884912806</v>
       </c>
       <c r="F68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G68" t="n">
         <v>2.149802235056419</v>
       </c>
-      <c r="G68" t="n">
+      <c r="H68" t="n">
         <v>19.58850769917064</v>
       </c>
     </row>
@@ -1961,9 +2167,12 @@
         <v>16.44103904919074</v>
       </c>
       <c r="F69" t="n">
+        <v>1</v>
+      </c>
+      <c r="G69" t="n">
         <v>2.61503014826508</v>
       </c>
-      <c r="G69" t="n">
+      <c r="H69" t="n">
         <v>16.10360693586473</v>
       </c>
     </row>
@@ -1984,9 +2193,12 @@
         <v>21.08616442699801</v>
       </c>
       <c r="F70" t="n">
+        <v>1</v>
+      </c>
+      <c r="G70" t="n">
         <v>2.991192034732157</v>
       </c>
-      <c r="G70" t="n">
+      <c r="H70" t="n">
         <v>14.07847344607807</v>
       </c>
     </row>
@@ -2007,9 +2219,12 @@
         <v>23.80449943392495</v>
       </c>
       <c r="F71" t="n">
+        <v>2</v>
+      </c>
+      <c r="G71" t="n">
         <v>3.646798496007988</v>
       </c>
-      <c r="G71" t="n">
+      <c r="H71" t="n">
         <v>11.54750329067939</v>
       </c>
     </row>
@@ -2030,9 +2245,12 @@
         <v>24.49337602795674</v>
       </c>
       <c r="F72" t="n">
+        <v>2</v>
+      </c>
+      <c r="G72" t="n">
         <v>4.815086387087103</v>
       </c>
-      <c r="G72" t="n">
+      <c r="H72" t="n">
         <v>8.74572421920187</v>
       </c>
     </row>
@@ -2053,9 +2271,12 @@
         <v>22.73808948321865</v>
       </c>
       <c r="F73" t="n">
+        <v>2</v>
+      </c>
+      <c r="G73" t="n">
         <v>7.33873355108866</v>
       </c>
-      <c r="G73" t="n">
+      <c r="H73" t="n">
         <v>5.738240438890156</v>
       </c>
     </row>
@@ -2076,9 +2297,12 @@
         <v>17.97032751749764</v>
       </c>
       <c r="F74" t="n">
+        <v>2</v>
+      </c>
+      <c r="G74" t="n">
         <v>12.08575316908585</v>
       </c>
-      <c r="G74" t="n">
+      <c r="H74" t="n">
         <v>3.484385047744787</v>
       </c>
     </row>
@@ -2099,9 +2323,12 @@
         <v>10.97987202189546</v>
       </c>
       <c r="F75" t="n">
+        <v>2</v>
+      </c>
+      <c r="G75" t="n">
         <v>15.92123509167183</v>
       </c>
-      <c r="G75" t="n">
+      <c r="H75" t="n">
         <v>2.644984348929361</v>
       </c>
     </row>
@@ -2122,9 +2349,12 @@
         <v>4.512007942290957</v>
       </c>
       <c r="F76" t="n">
+        <v>2</v>
+      </c>
+      <c r="G76" t="n">
         <v>25.10920781651108</v>
       </c>
-      <c r="G76" t="n">
+      <c r="H76" t="n">
         <v>1.677130475036559</v>
       </c>
     </row>
@@ -2145,9 +2375,12 @@
         <v>2.012861414000298</v>
       </c>
       <c r="F77" t="n">
+        <v>100</v>
+      </c>
+      <c r="G77" t="n">
         <v>31.60460890164972</v>
       </c>
-      <c r="G77" t="n">
+      <c r="H77" t="n">
         <v>1.332445459589242</v>
       </c>
     </row>
@@ -2168,9 +2401,12 @@
         <v>1.904036269713067</v>
       </c>
       <c r="F78" t="n">
+        <v>100</v>
+      </c>
+      <c r="G78" t="n">
         <v>17.28187586265758</v>
       </c>
-      <c r="G78" t="n">
+      <c r="H78" t="n">
         <v>2.436738810518286</v>
       </c>
     </row>
@@ -2191,9 +2427,12 @@
         <v>14.1763351992318</v>
       </c>
       <c r="F79" t="n">
+        <v>10</v>
+      </c>
+      <c r="G79" t="n">
         <v>5.532867134488765</v>
       </c>
-      <c r="G79" t="n">
+      <c r="H79" t="n">
         <v>7.61113842235577</v>
       </c>
     </row>
@@ -2214,9 +2453,12 @@
         <v>10.97126686657625</v>
       </c>
       <c r="F80" t="n">
+        <v>10</v>
+      </c>
+      <c r="G80" t="n">
         <v>3.067089080017121</v>
       </c>
-      <c r="G80" t="n">
+      <c r="H80" t="n">
         <v>13.73009277997946</v>
       </c>
     </row>
@@ -2237,9 +2479,12 @@
         <v>8.755218740226773</v>
       </c>
       <c r="F81" t="n">
+        <v>10</v>
+      </c>
+      <c r="G81" t="n">
         <v>2.275781391937766</v>
       </c>
-      <c r="G81" t="n">
+      <c r="H81" t="n">
         <v>18.50415764109934</v>
       </c>
     </row>
@@ -2260,9 +2505,12 @@
         <v>8.22459639425445</v>
       </c>
       <c r="F82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" t="n">
         <v>1.858165995243492</v>
       </c>
-      <c r="G82" t="n">
+      <c r="H82" t="n">
         <v>22.66289327266409</v>
       </c>
     </row>
@@ -2283,9 +2531,12 @@
         <v>8.422217270074508</v>
       </c>
       <c r="F83" t="n">
+        <v>0</v>
+      </c>
+      <c r="G83" t="n">
         <v>2.05874314328703</v>
       </c>
-      <c r="G83" t="n">
+      <c r="H83" t="n">
         <v>20.45491579190447</v>
       </c>
     </row>
@@ -2306,9 +2557,12 @@
         <v>8.777114273167584</v>
       </c>
       <c r="F84" t="n">
+        <v>0</v>
+      </c>
+      <c r="G84" t="n">
         <v>2.730694052733707</v>
       </c>
-      <c r="G84" t="n">
+      <c r="H84" t="n">
         <v>15.42150706738421</v>
       </c>
     </row>
@@ -2329,9 +2583,12 @@
         <v>9.773076693857931</v>
       </c>
       <c r="F85" t="n">
+        <v>0</v>
+      </c>
+      <c r="G85" t="n">
         <v>3.508277880485534</v>
       </c>
-      <c r="G85" t="n">
+      <c r="H85" t="n">
         <v>12.00344415912368</v>
       </c>
     </row>
@@ -2352,9 +2609,12 @@
         <v>11.00558208442262</v>
       </c>
       <c r="F86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" t="n">
         <v>2.436738810518287</v>
       </c>
-      <c r="G86" t="n">
+      <c r="H86" t="n">
         <v>17.28187586265757</v>
       </c>
     </row>
@@ -2375,9 +2635,12 @@
         <v>13.02950802563445</v>
       </c>
       <c r="F87" t="n">
+        <v>1</v>
+      </c>
+      <c r="G87" t="n">
         <v>1.940353473771524</v>
       </c>
-      <c r="G87" t="n">
+      <c r="H87" t="n">
         <v>21.7029619614841</v>
       </c>
     </row>
@@ -2398,9 +2661,12 @@
         <v>17.36078575479908</v>
       </c>
       <c r="F88" t="n">
+        <v>1</v>
+      </c>
+      <c r="G88" t="n">
         <v>2.21441577552405</v>
       </c>
-      <c r="G88" t="n">
+      <c r="H88" t="n">
         <v>19.01694257174043</v>
       </c>
     </row>
@@ -2421,9 +2687,12 @@
         <v>22.93971051046045</v>
       </c>
       <c r="F89" t="n">
+        <v>1</v>
+      </c>
+      <c r="G89" t="n">
         <v>2.579532550278769</v>
       </c>
-      <c r="G89" t="n">
+      <c r="H89" t="n">
         <v>16.32521273226265</v>
       </c>
     </row>
@@ -2444,9 +2713,12 @@
         <v>27.39580915602916</v>
       </c>
       <c r="F90" t="n">
+        <v>1</v>
+      </c>
+      <c r="G90" t="n">
         <v>3.195460494856385</v>
       </c>
-      <c r="G90" t="n">
+      <c r="H90" t="n">
         <v>13.17851298768428</v>
       </c>
     </row>
@@ -2467,9 +2739,12 @@
         <v>29.90419185177807</v>
       </c>
       <c r="F91" t="n">
+        <v>2</v>
+      </c>
+      <c r="G91" t="n">
         <v>4.003799301767846</v>
       </c>
-      <c r="G91" t="n">
+      <c r="H91" t="n">
         <v>10.51786427319245</v>
       </c>
     </row>
@@ -2490,9 +2765,12 @@
         <v>30.68864594160431</v>
       </c>
       <c r="F92" t="n">
+        <v>2</v>
+      </c>
+      <c r="G92" t="n">
         <v>4.621649649853573</v>
       </c>
-      <c r="G92" t="n">
+      <c r="H92" t="n">
         <v>9.111771948016681</v>
       </c>
     </row>
@@ -2513,9 +2791,12 @@
         <v>29.32793229773935</v>
       </c>
       <c r="F93" t="n">
+        <v>2</v>
+      </c>
+      <c r="G93" t="n">
         <v>5.120527203525829</v>
       </c>
-      <c r="G93" t="n">
+      <c r="H93" t="n">
         <v>8.224039431740612</v>
       </c>
     </row>
@@ -2536,9 +2817,12 @@
         <v>23.16395330621176</v>
       </c>
       <c r="F94" t="n">
+        <v>2</v>
+      </c>
+      <c r="G94" t="n">
         <v>7.157131980958146</v>
       </c>
-      <c r="G94" t="n">
+      <c r="H94" t="n">
         <v>5.883839748258957</v>
       </c>
     </row>
@@ -2559,9 +2843,12 @@
         <v>13.10008568673119</v>
       </c>
       <c r="F95" t="n">
+        <v>2</v>
+      </c>
+      <c r="G95" t="n">
         <v>9.756213148143731</v>
       </c>
-      <c r="G95" t="n">
+      <c r="H95" t="n">
         <v>4.316369168411337</v>
       </c>
     </row>
@@ -2582,9 +2869,12 @@
         <v>2.192695962383084</v>
       </c>
       <c r="F96" t="n">
+        <v>2</v>
+      </c>
+      <c r="G96" t="n">
         <v>15.95754347981189</v>
       </c>
-      <c r="G96" t="n">
+      <c r="H96" t="n">
         <v>2.638966184636918</v>
       </c>
     </row>
@@ -2605,9 +2895,12 @@
         <v>1.436530755349501</v>
       </c>
       <c r="F97" t="n">
+        <v>100</v>
+      </c>
+      <c r="G97" t="n">
         <v>30.47347070108647</v>
       </c>
-      <c r="G97" t="n">
+      <c r="H97" t="n">
         <v>1.381904215839632</v>
       </c>
     </row>
@@ -2628,9 +2921,12 @@
         <v>1.960170768556473</v>
       </c>
       <c r="F98" t="n">
+        <v>100</v>
+      </c>
+      <c r="G98" t="n">
         <v>14.01448049539119</v>
       </c>
-      <c r="G98" t="n">
+      <c r="H98" t="n">
         <v>3.00485042217196</v>
       </c>
     </row>
@@ -2651,9 +2947,12 @@
         <v>12.7929463620569</v>
       </c>
       <c r="F99" t="n">
+        <v>10</v>
+      </c>
+      <c r="G99" t="n">
         <v>5.52027813620713</v>
       </c>
-      <c r="G99" t="n">
+      <c r="H99" t="n">
         <v>7.628495629031982</v>
       </c>
     </row>
@@ -2674,9 +2973,12 @@
         <v>9.753047116847963</v>
       </c>
       <c r="F100" t="n">
+        <v>10</v>
+      </c>
+      <c r="G100" t="n">
         <v>3.390429873915228</v>
       </c>
-      <c r="G100" t="n">
+      <c r="H100" t="n">
         <v>12.42067206789537</v>
       </c>
     </row>
@@ -2697,9 +2999,12 @@
         <v>7.655024687559967</v>
       </c>
       <c r="F101" t="n">
+        <v>10</v>
+      </c>
+      <c r="G101" t="n">
         <v>2.90391325460475</v>
       </c>
-      <c r="G101" t="n">
+      <c r="H101" t="n">
         <v>14.50161004855108</v>
       </c>
     </row>
@@ -2720,9 +3025,12 @@
         <v>7.509367148038177</v>
       </c>
       <c r="F102" t="n">
+        <v>0</v>
+      </c>
+      <c r="G102" t="n">
         <v>2.189337723731022</v>
       </c>
-      <c r="G102" t="n">
+      <c r="H102" t="n">
         <v>19.23477459719259</v>
       </c>
     </row>
@@ -2743,9 +3051,12 @@
         <v>8.939150100287534</v>
       </c>
       <c r="F103" t="n">
+        <v>0</v>
+      </c>
+      <c r="G103" t="n">
         <v>2.464650750021215</v>
       </c>
-      <c r="G103" t="n">
+      <c r="H103" t="n">
         <v>17.08616023293946</v>
       </c>
     </row>
@@ -2766,9 +3077,12 @@
         <v>10.86397895833826</v>
       </c>
       <c r="F104" t="n">
+        <v>0</v>
+      </c>
+      <c r="G104" t="n">
         <v>3.224709357887811</v>
       </c>
-      <c r="G104" t="n">
+      <c r="H104" t="n">
         <v>13.05898081329102</v>
       </c>
     </row>
@@ -2789,9 +3103,12 @@
         <v>13.4046951585318</v>
       </c>
       <c r="F105" t="n">
+        <v>0</v>
+      </c>
+      <c r="G105" t="n">
         <v>3.344406650532939</v>
       </c>
-      <c r="G105" t="n">
+      <c r="H105" t="n">
         <v>12.59159606873355</v>
       </c>
     </row>
@@ -2812,9 +3129,12 @@
         <v>16.31826787753617</v>
       </c>
       <c r="F106" t="n">
+        <v>0</v>
+      </c>
+      <c r="G106" t="n">
         <v>2.250008380271464</v>
       </c>
-      <c r="G106" t="n">
+      <c r="H106" t="n">
         <v>18.71611590531772</v>
       </c>
     </row>
@@ -2835,9 +3155,12 @@
         <v>19.97724970423302</v>
       </c>
       <c r="F107" t="n">
+        <v>1</v>
+      </c>
+      <c r="G107" t="n">
         <v>2.130303029348465</v>
       </c>
-      <c r="G107" t="n">
+      <c r="H107" t="n">
         <v>19.76780629466425</v>
       </c>
     </row>
@@ -2858,9 +3181,12 @@
         <v>24.91812758738087</v>
       </c>
       <c r="F108" t="n">
+        <v>1</v>
+      </c>
+      <c r="G108" t="n">
         <v>2.36563819631443</v>
       </c>
-      <c r="G108" t="n">
+      <c r="H108" t="n">
         <v>17.80129256397061</v>
       </c>
     </row>
@@ -2881,9 +3207,12 @@
         <v>30.52522839508805</v>
       </c>
       <c r="F109" t="n">
+        <v>1</v>
+      </c>
+      <c r="G109" t="n">
         <v>2.984386139981755</v>
       </c>
-      <c r="G109" t="n">
+      <c r="H109" t="n">
         <v>14.11057941495277</v>
       </c>
     </row>
@@ -2904,9 +3233,12 @@
         <v>34.53071896447337</v>
       </c>
       <c r="F110" t="n">
+        <v>2</v>
+      </c>
+      <c r="G110" t="n">
         <v>3.398161751694496</v>
       </c>
-      <c r="G110" t="n">
+      <c r="H110" t="n">
         <v>12.39241116527135</v>
       </c>
     </row>
@@ -2927,9 +3259,12 @@
         <v>35.84717448716342</v>
       </c>
       <c r="F111" t="n">
+        <v>2</v>
+      </c>
+      <c r="G111" t="n">
         <v>4.022081458667099</v>
       </c>
-      <c r="G111" t="n">
+      <c r="H111" t="n">
         <v>10.47005588172559</v>
       </c>
     </row>
@@ -2950,9 +3285,12 @@
         <v>36.00825769121968</v>
       </c>
       <c r="F112" t="n">
+        <v>2</v>
+      </c>
+      <c r="G112" t="n">
         <v>6.074503319580139</v>
       </c>
-      <c r="G112" t="n">
+      <c r="H112" t="n">
         <v>6.932487384994562</v>
       </c>
     </row>
@@ -2973,9 +3311,12 @@
         <v>35.99102534042315</v>
       </c>
       <c r="F113" t="n">
+        <v>2</v>
+      </c>
+      <c r="G113" t="n">
         <v>8.020530411659378</v>
       </c>
-      <c r="G113" t="n">
+      <c r="H113" t="n">
         <v>5.250452959056161</v>
       </c>
     </row>
@@ -2996,9 +3337,12 @@
         <v>28.66408455332091</v>
       </c>
       <c r="F114" t="n">
+        <v>2</v>
+      </c>
+      <c r="G114" t="n">
         <v>7.38905609893065</v>
       </c>
-      <c r="G114" t="n">
+      <c r="H114" t="n">
         <v>5.699160632870456</v>
       </c>
     </row>
@@ -3019,9 +3363,12 @@
         <v>17.06133534216584</v>
       </c>
       <c r="F115" t="n">
+        <v>2</v>
+      </c>
+      <c r="G115" t="n">
         <v>9.008581981902688</v>
       </c>
-      <c r="G115" t="n">
+      <c r="H115" t="n">
         <v>4.674588932830317</v>
       </c>
     </row>
@@ -3042,9 +3389,12 @@
         <v>7.683849957718948</v>
       </c>
       <c r="F116" t="n">
+        <v>2</v>
+      </c>
+      <c r="G116" t="n">
         <v>15.24685994048192</v>
       </c>
-      <c r="G116" t="n">
+      <c r="H116" t="n">
         <v>2.761973140534133</v>
       </c>
     </row>
@@ -3065,9 +3415,12 @@
         <v>3.959362848831567</v>
       </c>
       <c r="F117" t="n">
+        <v>100</v>
+      </c>
+      <c r="G117" t="n">
         <v>29.71938553256001</v>
       </c>
-      <c r="G117" t="n">
+      <c r="H117" t="n">
         <v>1.416967978256496</v>
       </c>
     </row>
@@ -3088,9 +3441,12 @@
         <v>3.417494179306651</v>
       </c>
       <c r="F118" t="n">
+        <v>100</v>
+      </c>
+      <c r="G118" t="n">
         <v>20.45491579190448</v>
       </c>
-      <c r="G118" t="n">
+      <c r="H118" t="n">
         <v>2.058743143287029</v>
       </c>
     </row>
@@ -3111,9 +3467,12 @@
         <v>5.999892176066218</v>
       </c>
       <c r="F119" t="n">
+        <v>10</v>
+      </c>
+      <c r="G119" t="n">
         <v>4.209557902844931</v>
       </c>
-      <c r="G119" t="n">
+      <c r="H119" t="n">
         <v>10.00376253397937</v>
       </c>
     </row>
@@ -3134,9 +3493,12 @@
         <v>4.86002637255668</v>
       </c>
       <c r="F120" t="n">
+        <v>0</v>
+      </c>
+      <c r="G120" t="n">
         <v>2.651016237649828</v>
       </c>
-      <c r="G120" t="n">
+      <c r="H120" t="n">
         <v>15.88500931643837</v>
       </c>
     </row>
@@ -3157,9 +3519,12 @@
         <v>8.505739795459482</v>
       </c>
       <c r="F121" t="n">
+        <v>0</v>
+      </c>
+      <c r="G121" t="n">
         <v>3.730822436068817</v>
       </c>
-      <c r="G121" t="n">
+      <c r="H121" t="n">
         <v>11.28743550643752</v>
       </c>
     </row>
@@ -3180,9 +3545,12 @@
         <v>12.94471001665543</v>
       </c>
       <c r="F122" t="n">
+        <v>2</v>
+      </c>
+      <c r="G122" t="n">
         <v>4.590174291905306</v>
       </c>
-      <c r="G122" t="n">
+      <c r="H122" t="n">
         <v>9.17425242596118</v>
       </c>
     </row>
@@ -3203,9 +3571,12 @@
         <v>17.2431032100854</v>
       </c>
       <c r="F123" t="n">
+        <v>2</v>
+      </c>
+      <c r="G123" t="n">
         <v>3.067089080017121</v>
       </c>
-      <c r="G123" t="n">
+      <c r="H123" t="n">
         <v>13.73009277997946</v>
       </c>
     </row>
@@ -3226,9 +3597,12 @@
         <v>21.36482490156886</v>
       </c>
       <c r="F124" t="n">
+        <v>2</v>
+      </c>
+      <c r="G124" t="n">
         <v>2.626970904497728</v>
       </c>
-      <c r="G124" t="n">
+      <c r="H124" t="n">
         <v>16.03040884883669</v>
       </c>
     </row>
@@ -3249,9 +3623,12 @@
         <v>25.67525631530482</v>
       </c>
       <c r="F125" t="n">
+        <v>2</v>
+      </c>
+      <c r="G125" t="n">
         <v>2.78725418350556</v>
       </c>
-      <c r="G125" t="n">
+      <c r="H125" t="n">
         <v>15.10856737871424</v>
       </c>
     </row>
@@ -3272,9 +3649,12 @@
         <v>30.88140662293259</v>
       </c>
       <c r="F126" t="n">
+        <v>2</v>
+      </c>
+      <c r="G126" t="n">
         <v>3.173698078726824</v>
       </c>
-      <c r="G126" t="n">
+      <c r="H126" t="n">
         <v>13.26887958100618</v>
       </c>
     </row>
@@ -3295,9 +3675,12 @@
         <v>37.2461832256778</v>
       </c>
       <c r="F127" t="n">
+        <v>2</v>
+      </c>
+      <c r="G127" t="n">
         <v>2.991192034732157</v>
       </c>
-      <c r="G127" t="n">
+      <c r="H127" t="n">
         <v>14.07847344607807</v>
       </c>
     </row>
@@ -3318,9 +3701,12 @@
         <v>41.34277113170809</v>
       </c>
       <c r="F128" t="n">
+        <v>2</v>
+      </c>
+      <c r="G128" t="n">
         <v>4.257776827668183</v>
       </c>
-      <c r="G128" t="n">
+      <c r="H128" t="n">
         <v>9.89047085780672</v>
       </c>
     </row>
@@ -3341,9 +3727,12 @@
         <v>39.7802013399217</v>
       </c>
       <c r="F129" t="n">
+        <v>2</v>
+      </c>
+      <c r="G129" t="n">
         <v>4.685249336272087</v>
       </c>
-      <c r="G129" t="n">
+      <c r="H129" t="n">
         <v>8.988084648362323</v>
       </c>
     </row>
@@ -3364,9 +3753,12 @@
         <v>37.99112343390719</v>
       </c>
       <c r="F130" t="n">
+        <v>2</v>
+      </c>
+      <c r="G130" t="n">
         <v>5.132204569516401</v>
       </c>
-      <c r="G130" t="n">
+      <c r="H130" t="n">
         <v>8.205327177179338</v>
       </c>
     </row>
@@ -3387,9 +3779,12 @@
         <v>35.34115437313403</v>
       </c>
       <c r="F131" t="n">
+        <v>2</v>
+      </c>
+      <c r="G131" t="n">
         <v>6.59363495933794</v>
       </c>
-      <c r="G131" t="n">
+      <c r="H131" t="n">
         <v>6.386677135266413</v>
       </c>
     </row>
@@ -3410,9 +3805,12 @@
         <v>28.93210910164752</v>
       </c>
       <c r="F132" t="n">
+        <v>2</v>
+      </c>
+      <c r="G132" t="n">
         <v>10.51786427319245</v>
       </c>
-      <c r="G132" t="n">
+      <c r="H132" t="n">
         <v>4.003799301767844</v>
       </c>
     </row>
@@ -3433,9 +3831,12 @@
         <v>19.87785786813677</v>
       </c>
       <c r="F133" t="n">
+        <v>2</v>
+      </c>
+      <c r="G133" t="n">
         <v>15.03989219095908</v>
       </c>
-      <c r="G133" t="n">
+      <c r="H133" t="n">
         <v>2.799981349494734</v>
       </c>
     </row>
@@ -3456,9 +3857,12 @@
         <v>12.04145820799784</v>
       </c>
       <c r="F134" t="n">
+        <v>2</v>
+      </c>
+      <c r="G134" t="n">
         <v>21.8517816909397</v>
       </c>
-      <c r="G134" t="n">
+      <c r="H134" t="n">
         <v>1.927138858913155</v>
       </c>
     </row>
@@ -3479,9 +3883,12 @@
         <v>7.470996160813598</v>
       </c>
       <c r="F135" t="n">
+        <v>100</v>
+      </c>
+      <c r="G135" t="n">
         <v>30.47347070108647</v>
       </c>
-      <c r="G135" t="n">
+      <c r="H135" t="n">
         <v>1.381904215839632</v>
       </c>
     </row>
@@ -3502,9 +3909,12 @@
         <v>5.536354146749171</v>
       </c>
       <c r="F136" t="n">
+        <v>10</v>
+      </c>
+      <c r="G136" t="n">
         <v>4.277218697287138</v>
       </c>
-      <c r="G136" t="n">
+      <c r="H136" t="n">
         <v>9.845514249670336</v>
       </c>
     </row>
@@ -3525,9 +3935,12 @@
         <v>5.478989216472653</v>
       </c>
       <c r="F137" t="n">
+        <v>100</v>
+      </c>
+      <c r="G137" t="n">
         <v>3.359677887303711</v>
       </c>
-      <c r="G137" t="n">
+      <c r="H137" t="n">
         <v>12.53436163991696</v>
       </c>
     </row>
@@ -3548,9 +3961,12 @@
         <v>9.988757167458838</v>
       </c>
       <c r="F138" t="n">
+        <v>100</v>
+      </c>
+      <c r="G138" t="n">
         <v>4.497028550210074</v>
       </c>
-      <c r="G138" t="n">
+      <c r="H138" t="n">
         <v>9.364276246618385</v>
       </c>
     </row>
@@ -3571,9 +3987,12 @@
         <v>15.69188865078733</v>
       </c>
       <c r="F139" t="n">
+        <v>2</v>
+      </c>
+      <c r="G139" t="n">
         <v>5.951236950777927</v>
       </c>
-      <c r="G139" t="n">
+      <c r="H139" t="n">
         <v>7.076078129873864</v>
       </c>
     </row>
@@ -3594,9 +4013,12 @@
         <v>21.23980669633495</v>
       </c>
       <c r="F140" t="n">
+        <v>2</v>
+      </c>
+      <c r="G140" t="n">
         <v>5.085654281771596</v>
       </c>
-      <c r="G140" t="n">
+      <c r="H140" t="n">
         <v>8.280432624772779</v>
       </c>
     </row>
@@ -3617,9 +4039,12 @@
         <v>25.82497502898106</v>
       </c>
       <c r="F141" t="n">
+        <v>2</v>
+      </c>
+      <c r="G141" t="n">
         <v>3.246821564279982</v>
       </c>
-      <c r="G141" t="n">
+      <c r="H141" t="n">
         <v>12.97004371795084</v>
       </c>
     </row>
@@ -3640,9 +4065,12 @@
         <v>29.54642238996812</v>
       </c>
       <c r="F142" t="n">
+        <v>2</v>
+      </c>
+      <c r="G142" t="n">
         <v>3.137756244463604</v>
       </c>
-      <c r="G142" t="n">
+      <c r="H142" t="n">
         <v>13.42086967634919</v>
       </c>
     </row>
@@ -3663,9 +4091,12 @@
         <v>33.68431052975822</v>
       </c>
       <c r="F143" t="n">
+        <v>2</v>
+      </c>
+      <c r="G143" t="n">
         <v>3.931497911153397</v>
       </c>
-      <c r="G143" t="n">
+      <c r="H143" t="n">
         <v>10.7112908577745</v>
       </c>
     </row>
@@ -3686,9 +4117,12 @@
         <v>38.66403780272375</v>
       </c>
       <c r="F144" t="n">
+        <v>2</v>
+      </c>
+      <c r="G144" t="n">
         <v>3.67180501661647</v>
       </c>
-      <c r="G144" t="n">
+      <c r="H144" t="n">
         <v>11.46885998644398</v>
       </c>
     </row>
@@ -3709,9 +4143,12 @@
         <v>41.58878612735796</v>
       </c>
       <c r="F145" t="n">
+        <v>2</v>
+      </c>
+      <c r="G145" t="n">
         <v>4.296749342412553</v>
       </c>
-      <c r="G145" t="n">
+      <c r="H145" t="n">
         <v>9.800761989400121</v>
       </c>
     </row>
@@ -3732,9 +4169,12 @@
         <v>39.88266018812234</v>
       </c>
       <c r="F146" t="n">
+        <v>2</v>
+      </c>
+      <c r="G146" t="n">
         <v>7.173453825616434</v>
       </c>
-      <c r="G146" t="n">
+      <c r="H146" t="n">
         <v>5.870452177822188</v>
       </c>
     </row>
@@ -3755,9 +4195,12 @@
         <v>36.99725195125912</v>
       </c>
       <c r="F147" t="n">
+        <v>2</v>
+      </c>
+      <c r="G147" t="n">
         <v>5.897257849059788</v>
       </c>
-      <c r="G147" t="n">
+      <c r="H147" t="n">
         <v>7.140847273586793</v>
       </c>
     </row>
@@ -3778,9 +4221,12 @@
         <v>33.18844069140914</v>
       </c>
       <c r="F148" t="n">
+        <v>2</v>
+      </c>
+      <c r="G148" t="n">
         <v>6.59363495933794</v>
       </c>
-      <c r="G148" t="n">
+      <c r="H148" t="n">
         <v>6.386677135266413</v>
       </c>
     </row>
@@ -3801,9 +4247,12 @@
         <v>27.67774145171791</v>
       </c>
       <c r="F149" t="n">
+        <v>2</v>
+      </c>
+      <c r="G149" t="n">
         <v>11.26175307041645</v>
       </c>
-      <c r="G149" t="n">
+      <c r="H149" t="n">
         <v>3.739330579332233</v>
       </c>
     </row>
@@ -3824,9 +4273,12 @@
         <v>20.92229287090854</v>
       </c>
       <c r="F150" t="n">
+        <v>2</v>
+      </c>
+      <c r="G150" t="n">
         <v>21.16590853922112</v>
       </c>
-      <c r="G150" t="n">
+      <c r="H150" t="n">
         <v>1.989587054818038</v>
       </c>
     </row>
@@ -3847,9 +4299,12 @@
         <v>14.47350128602201</v>
       </c>
       <c r="F151" t="n">
+        <v>2</v>
+      </c>
+      <c r="G151" t="n">
         <v>40.41967327539025</v>
       </c>
-      <c r="G151" t="n">
+      <c r="H151" t="n">
         <v>1.041854478787603</v>
       </c>
     </row>
@@ -3870,9 +4325,12 @@
         <v>10.1120504007794</v>
       </c>
       <c r="F152" t="n">
+        <v>100</v>
+      </c>
+      <c r="G152" t="n">
         <v>39.06191939043615</v>
       </c>
-      <c r="G152" t="n">
+      <c r="H152" t="n">
         <v>1.078068315388706</v>
       </c>
     </row>
@@ -3893,9 +4351,12 @@
         <v>13.0168030986855</v>
       </c>
       <c r="F153" t="n">
+        <v>100</v>
+      </c>
+      <c r="G153" t="n">
         <v>6.684371632937881</v>
       </c>
-      <c r="G153" t="n">
+      <c r="H153" t="n">
         <v>6.299981500966952</v>
       </c>
     </row>
@@ -3916,9 +4377,12 @@
         <v>29.67311080212772</v>
       </c>
       <c r="F154" t="n">
+        <v>100</v>
+      </c>
+      <c r="G154" t="n">
         <v>4.199979845769421</v>
       </c>
-      <c r="G154" t="n">
+      <c r="H154" t="n">
         <v>10.02657612167238</v>
       </c>
     </row>
@@ -3939,9 +4403,12 @@
         <v>31.2677769974876</v>
       </c>
       <c r="F155" t="n">
+        <v>2</v>
+      </c>
+      <c r="G155" t="n">
         <v>4.84810399337989</v>
       </c>
-      <c r="G155" t="n">
+      <c r="H155" t="n">
         <v>8.686162196726857</v>
       </c>
     </row>
@@ -3962,9 +4429,12 @@
         <v>33.20055188917861</v>
       </c>
       <c r="F156" t="n">
+        <v>2</v>
+      </c>
+      <c r="G156" t="n">
         <v>5.3836753872296</v>
       </c>
-      <c r="G156" t="n">
+      <c r="H156" t="n">
         <v>7.822057350074953</v>
       </c>
     </row>
@@ -3985,9 +4455,12 @@
         <v>35.63312131396236</v>
       </c>
       <c r="F157" t="n">
+        <v>2</v>
+      </c>
+      <c r="G157" t="n">
         <v>5.764442404603849</v>
       </c>
-      <c r="G157" t="n">
+      <c r="H157" t="n">
         <v>7.305375728876059</v>
       </c>
     </row>
@@ -4008,9 +4481,12 @@
         <v>37.87267135145505</v>
       </c>
       <c r="F158" t="n">
+        <v>2</v>
+      </c>
+      <c r="G158" t="n">
         <v>4.05889659372358</v>
       </c>
-      <c r="G158" t="n">
+      <c r="H158" t="n">
         <v>10.37509004250449</v>
       </c>
     </row>
@@ -4031,9 +4507,12 @@
         <v>36.87946759049073</v>
       </c>
       <c r="F159" t="n">
+        <v>2</v>
+      </c>
+      <c r="G159" t="n">
         <v>6.91671381413957</v>
       </c>
-      <c r="G159" t="n">
+      <c r="H159" t="n">
         <v>6.088356228793241</v>
       </c>
     </row>
@@ -4054,9 +4533,12 @@
         <v>34.11127007117564</v>
       </c>
       <c r="F160" t="n">
+        <v>2</v>
+      </c>
+      <c r="G160" t="n">
         <v>8.205327177179342</v>
       </c>
-      <c r="G160" t="n">
+      <c r="H160" t="n">
         <v>5.132204569516397</v>
       </c>
     </row>
@@ -4077,9 +4559,12 @@
         <v>30.65014036216303</v>
       </c>
       <c r="F161" t="n">
+        <v>2</v>
+      </c>
+      <c r="G161" t="n">
         <v>8.186657498833034</v>
       </c>
-      <c r="G161" t="n">
+      <c r="H161" t="n">
         <v>5.143908565748557</v>
       </c>
     </row>
@@ -4100,9 +4585,12 @@
         <v>26.24997810749442</v>
       </c>
       <c r="F162" t="n">
+        <v>2</v>
+      </c>
+      <c r="G162" t="n">
         <v>11.52122911934112</v>
       </c>
-      <c r="G162" t="n">
+      <c r="H162" t="n">
         <v>3.65511502261533</v>
       </c>
     </row>
@@ -4123,9 +4611,12 @@
         <v>21.20356438526349</v>
       </c>
       <c r="F163" t="n">
+        <v>2</v>
+      </c>
+      <c r="G163" t="n">
         <v>20.13134200466594</v>
       </c>
-      <c r="G163" t="n">
+      <c r="H163" t="n">
         <v>2.091833600727489</v>
       </c>
     </row>
@@ -4146,9 +4637,12 @@
         <v>16.35320221663123</v>
       </c>
       <c r="F164" t="n">
+        <v>100</v>
+      </c>
+      <c r="G164" t="n">
         <v>42.11141763309691</v>
       </c>
-      <c r="G164" t="n">
+      <c r="H164" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4169,9 +4663,12 @@
         <v>12.70606592010315</v>
       </c>
       <c r="F165" t="n">
+        <v>100</v>
+      </c>
+      <c r="G165" t="n">
         <v>42.0156010245766</v>
       </c>
-      <c r="G165" t="n">
+      <c r="H165" t="n">
         <v>1.002280500723154</v>
       </c>
     </row>
@@ -4192,9 +4689,12 @@
         <v>30.51006534913649</v>
       </c>
       <c r="F166" t="n">
+        <v>100</v>
+      </c>
+      <c r="G166" t="n">
         <v>7.839895557518359</v>
       </c>
-      <c r="G166" t="n">
+      <c r="H166" t="n">
         <v>5.371425846701823</v>
       </c>
     </row>
@@ -4215,9 +4715,12 @@
         <v>30.52040004004413</v>
       </c>
       <c r="F167" t="n">
+        <v>100</v>
+      </c>
+      <c r="G167" t="n">
         <v>9.19517431525299</v>
       </c>
-      <c r="G167" t="n">
+      <c r="H167" t="n">
         <v>4.579730213840789</v>
       </c>
     </row>
@@ -4238,9 +4741,12 @@
         <v>30.12492803930272</v>
       </c>
       <c r="F168" t="n">
+        <v>100</v>
+      </c>
+      <c r="G168" t="n">
         <v>7.059977845292225</v>
       </c>
-      <c r="G168" t="n">
+      <c r="H168" t="n">
         <v>5.964808750947836</v>
       </c>
     </row>
@@ -4261,9 +4767,12 @@
         <v>30.53252949293379</v>
       </c>
       <c r="F169" t="n">
+        <v>2</v>
+      </c>
+      <c r="G169" t="n">
         <v>5.408258337249224</v>
       </c>
-      <c r="G169" t="n">
+      <c r="H169" t="n">
         <v>7.786502605294522</v>
       </c>
     </row>
@@ -4284,9 +4793,12 @@
         <v>31.23207946028282</v>
       </c>
       <c r="F170" t="n">
+        <v>2</v>
+      </c>
+      <c r="G170" t="n">
         <v>6.401241957091944</v>
       </c>
-      <c r="G170" t="n">
+      <c r="H170" t="n">
         <v>6.578632383430159</v>
       </c>
     </row>
@@ -4307,9 +4819,12 @@
         <v>30.07873966791313</v>
       </c>
       <c r="F171" t="n">
+        <v>2</v>
+      </c>
+      <c r="G171" t="n">
         <v>9.958290964567235</v>
       </c>
-      <c r="G171" t="n">
+      <c r="H171" t="n">
         <v>4.228779595106657</v>
       </c>
     </row>
@@ -4330,9 +4845,12 @@
         <v>27.85709166959406</v>
       </c>
       <c r="F172" t="n">
+        <v>2</v>
+      </c>
+      <c r="G172" t="n">
         <v>13.82424161996467</v>
       </c>
-      <c r="G172" t="n">
+      <c r="H172" t="n">
         <v>3.04620092665919</v>
       </c>
     </row>
@@ -4353,9 +4871,12 @@
         <v>24.73635655574751</v>
       </c>
       <c r="F173" t="n">
+        <v>2</v>
+      </c>
+      <c r="G173" t="n">
         <v>15.10856737871425</v>
       </c>
-      <c r="G173" t="n">
+      <c r="H173" t="n">
         <v>2.787254183505558</v>
       </c>
     </row>
@@ -4376,9 +4897,12 @@
         <v>21.10404174670357</v>
       </c>
       <c r="F174" t="n">
+        <v>100</v>
+      </c>
+      <c r="G174" t="n">
         <v>27.25505967320341</v>
       </c>
-      <c r="G174" t="n">
+      <c r="H174" t="n">
         <v>1.545086238592974</v>
       </c>
     </row>
@@ -4399,9 +4923,12 @@
         <v>17.53844973352166</v>
       </c>
       <c r="F175" t="n">
+        <v>100</v>
+      </c>
+      <c r="G175" t="n">
         <v>25.28138456919253</v>
       </c>
-      <c r="G175" t="n">
+      <c r="H175" t="n">
         <v>1.6657085183702</v>
       </c>
     </row>
@@ -4422,9 +4949,12 @@
         <v>25.58016166012715</v>
       </c>
       <c r="F176" t="n">
+        <v>100</v>
+      </c>
+      <c r="G176" t="n">
         <v>7.965907260886808</v>
       </c>
-      <c r="G176" t="n">
+      <c r="H176" t="n">
         <v>5.286455924470408</v>
       </c>
     </row>
@@ -4445,9 +4975,12 @@
         <v>26.28825088550823</v>
       </c>
       <c r="F177" t="n">
+        <v>100</v>
+      </c>
+      <c r="G177" t="n">
         <v>10.4700558817256</v>
       </c>
-      <c r="G177" t="n">
+      <c r="H177" t="n">
         <v>4.022081458667096</v>
       </c>
     </row>
@@ -4468,9 +5001,12 @@
         <v>25.31530099719284</v>
       </c>
       <c r="F178" t="n">
+        <v>100</v>
+      </c>
+      <c r="G178" t="n">
         <v>16.93118479021815</v>
       </c>
-      <c r="G178" t="n">
+      <c r="H178" t="n">
         <v>2.487210325495143</v>
       </c>
     </row>
@@ -4491,9 +5027,12 @@
         <v>23.32809410726807</v>
       </c>
       <c r="F179" t="n">
+        <v>100</v>
+      </c>
+      <c r="G179" t="n">
         <v>28.26673436747747</v>
       </c>
-      <c r="G179" t="n">
+      <c r="H179" t="n">
         <v>1.489787149998783</v>
       </c>
     </row>
@@ -4514,9 +5053,12 @@
         <v>20.80937904157605</v>
       </c>
       <c r="F180" t="n">
+        <v>100</v>
+      </c>
+      <c r="G180" t="n">
         <v>27.75628815155564</v>
       </c>
-      <c r="G180" t="n">
+      <c r="H180" t="n">
         <v>1.51718476920109</v>
       </c>
     </row>

</xml_diff>

<commit_message>
multiple erosion maps and found issue with probs
</commit_message>
<xml_diff>
--- a/output/xyz_age_eros.xlsx
+++ b/output/xyz_age_eros.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H180"/>
+  <dimension ref="A1:I180"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -394,15 +394,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>E_map</t>
+          <t>E_map1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>E_map2</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>E_exp_Z</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>E_inv_exp_Z</t>
         </is>
@@ -428,9 +433,12 @@
         <v>10</v>
       </c>
       <c r="G2" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2" t="n">
         <v>1.71577234424401</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>24.54370929475012</v>
       </c>
     </row>
@@ -454,9 +462,12 @@
         <v>10</v>
       </c>
       <c r="G3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H3" t="n">
         <v>2.527187593999784</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>16.6633524686021</v>
       </c>
     </row>
@@ -480,9 +491,12 @@
         <v>10</v>
       </c>
       <c r="G4" t="n">
+        <v>10</v>
+      </c>
+      <c r="H4" t="n">
         <v>1.513732700682522</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>27.81958638675733</v>
       </c>
     </row>
@@ -506,9 +520,12 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
         <v>1.205371905865509</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>34.93645191843017</v>
       </c>
     </row>
@@ -535,6 +552,9 @@
         <v>1</v>
       </c>
       <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
         <v>42.11141763309691</v>
       </c>
     </row>
@@ -558,9 +578,12 @@
         <v>10</v>
       </c>
       <c r="G7" t="n">
+        <v>10</v>
+      </c>
+      <c r="H7" t="n">
         <v>7.38905609893065</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>5.699160632870456</v>
       </c>
     </row>
@@ -584,9 +607,12 @@
         <v>10</v>
       </c>
       <c r="G8" t="n">
+        <v>10</v>
+      </c>
+      <c r="H8" t="n">
         <v>3.276540548249262</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>12.85240240826505</v>
       </c>
     </row>
@@ -610,9 +636,12 @@
         <v>10</v>
       </c>
       <c r="G9" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" t="n">
         <v>2.475904843525316</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>17.00849600226824</v>
       </c>
     </row>
@@ -636,9 +665,12 @@
         <v>10</v>
       </c>
       <c r="G10" t="n">
+        <v>10</v>
+      </c>
+      <c r="H10" t="n">
         <v>1.53806313144631</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>27.37951178473256</v>
       </c>
     </row>
@@ -662,9 +694,12 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" t="n">
         <v>1.276007117771601</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>33.00249430163026</v>
       </c>
     </row>
@@ -688,9 +723,12 @@
         <v>1</v>
       </c>
       <c r="G12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" t="n">
         <v>1.136056031253367</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>37.06808156868549</v>
       </c>
     </row>
@@ -714,9 +752,12 @@
         <v>1</v>
       </c>
       <c r="G13" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" t="n">
         <v>1.763319615489954</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>23.88189711222369</v>
       </c>
     </row>
@@ -740,9 +781,12 @@
         <v>1</v>
       </c>
       <c r="G14" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" t="n">
         <v>1.598791916034733</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>26.33952374336501</v>
       </c>
     </row>
@@ -766,9 +810,12 @@
         <v>1</v>
       </c>
       <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="n">
         <v>1.650600155135878</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>25.51279151529602</v>
       </c>
     </row>
@@ -792,9 +839,12 @@
         <v>10</v>
       </c>
       <c r="G16" t="n">
+        <v>10</v>
+      </c>
+      <c r="H16" t="n">
         <v>11.05838613157211</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>3.808097956795633</v>
       </c>
     </row>
@@ -818,9 +868,12 @@
         <v>10</v>
       </c>
       <c r="G17" t="n">
+        <v>10</v>
+      </c>
+      <c r="H17" t="n">
         <v>4.326212651421302</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>9.734014720534354</v>
       </c>
     </row>
@@ -844,9 +897,12 @@
         <v>10</v>
       </c>
       <c r="G18" t="n">
+        <v>10</v>
+      </c>
+      <c r="H18" t="n">
         <v>2.338847564732744</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>18.00519976936116</v>
       </c>
     </row>
@@ -870,9 +926,12 @@
         <v>10</v>
       </c>
       <c r="G19" t="n">
+        <v>10</v>
+      </c>
+      <c r="H19" t="n">
         <v>1.858165995243492</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>22.66289327266409</v>
       </c>
     </row>
@@ -896,9 +955,12 @@
         <v>1</v>
       </c>
       <c r="G20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" t="n">
         <v>1.338529674884737</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>31.46095183636717</v>
       </c>
     </row>
@@ -922,9 +984,12 @@
         <v>1</v>
       </c>
       <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
         <v>1.183605064314989</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>35.57894343538389</v>
       </c>
     </row>
@@ -948,9 +1013,12 @@
         <v>1</v>
       </c>
       <c r="G22" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" t="n">
         <v>1.213637280943926</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>34.6985201380301</v>
       </c>
     </row>
@@ -974,9 +1042,12 @@
         <v>1</v>
       </c>
       <c r="G23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" t="n">
         <v>1.50000279342122</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>28.07422613997191</v>
       </c>
     </row>
@@ -1000,9 +1071,12 @@
         <v>1</v>
       </c>
       <c r="G24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" t="n">
         <v>1.631907262573603</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>25.80503108165902</v>
       </c>
     </row>
@@ -1026,9 +1100,12 @@
         <v>1</v>
       </c>
       <c r="G25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" t="n">
         <v>2.270603279516831</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>18.54635638598123</v>
       </c>
     </row>
@@ -1052,9 +1129,12 @@
         <v>1</v>
       </c>
       <c r="G26" t="n">
+        <v>1</v>
+      </c>
+      <c r="H26" t="n">
         <v>2.021565957079946</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>20.8310876455027</v>
       </c>
     </row>
@@ -1078,9 +1158,12 @@
         <v>10</v>
       </c>
       <c r="G27" t="n">
+        <v>10</v>
+      </c>
+      <c r="H27" t="n">
         <v>17.40037969153265</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>2.42014360488864</v>
       </c>
     </row>
@@ -1104,9 +1187,12 @@
         <v>10</v>
       </c>
       <c r="G28" t="n">
+        <v>10</v>
+      </c>
+      <c r="H28" t="n">
         <v>9.070354874271228</v>
       </c>
-      <c r="H28" t="n">
+      <c r="I28" t="n">
         <v>4.642753036328187</v>
       </c>
     </row>
@@ -1130,9 +1216,12 @@
         <v>10</v>
       </c>
       <c r="G29" t="n">
+        <v>10</v>
+      </c>
+      <c r="H29" t="n">
         <v>4.238423330031359</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>9.935632746902924</v>
       </c>
     </row>
@@ -1156,9 +1245,12 @@
         <v>10</v>
       </c>
       <c r="G30" t="n">
+        <v>10</v>
+      </c>
+      <c r="H30" t="n">
         <v>2.755688790255169</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>15.28163041560201</v>
       </c>
     </row>
@@ -1182,9 +1274,12 @@
         <v>10</v>
       </c>
       <c r="G31" t="n">
+        <v>10</v>
+      </c>
+      <c r="H31" t="n">
         <v>1.743350185569119</v>
       </c>
-      <c r="H31" t="n">
+      <c r="I31" t="n">
         <v>24.15545538795442</v>
       </c>
     </row>
@@ -1208,9 +1303,12 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
         <v>1.385055649403185</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>30.40413405139538</v>
       </c>
     </row>
@@ -1234,9 +1332,12 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
         <v>1.545086238592975</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>27.25505967320339</v>
       </c>
     </row>
@@ -1260,9 +1361,12 @@
         <v>1</v>
       </c>
       <c r="G34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" t="n">
         <v>1.335484102423399</v>
       </c>
-      <c r="H34" t="n">
+      <c r="I34" t="n">
         <v>31.53269855978113</v>
       </c>
     </row>
@@ -1286,9 +1390,12 @@
         <v>1</v>
       </c>
       <c r="G35" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" t="n">
         <v>1.385055649403185</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>30.40413405139538</v>
       </c>
     </row>
@@ -1312,9 +1419,12 @@
         <v>1</v>
       </c>
       <c r="G36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" t="n">
         <v>1.503423550876351</v>
       </c>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
         <v>28.01034851991644</v>
       </c>
     </row>
@@ -1338,9 +1448,12 @@
         <v>1</v>
       </c>
       <c r="G37" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" t="n">
         <v>2.072860184000009</v>
       </c>
-      <c r="H37" t="n">
+      <c r="I37" t="n">
         <v>20.31560930068823</v>
       </c>
     </row>
@@ -1364,9 +1477,12 @@
         <v>1</v>
       </c>
       <c r="G38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" t="n">
         <v>2.699769197680611</v>
       </c>
-      <c r="H38" t="n">
+      <c r="I38" t="n">
         <v>15.59815471236397</v>
       </c>
     </row>
@@ -1390,9 +1506,12 @@
         <v>1</v>
       </c>
       <c r="G39" t="n">
+        <v>1</v>
+      </c>
+      <c r="H39" t="n">
         <v>2.812766630296358</v>
       </c>
-      <c r="H39" t="n">
+      <c r="I39" t="n">
         <v>14.97152916260955</v>
       </c>
     </row>
@@ -1416,9 +1535,12 @@
         <v>1</v>
       </c>
       <c r="G40" t="n">
+        <v>1</v>
+      </c>
+      <c r="H40" t="n">
         <v>4.486796407757537</v>
       </c>
-      <c r="H40" t="n">
+      <c r="I40" t="n">
         <v>9.385631485370613</v>
       </c>
     </row>
@@ -1442,9 +1564,12 @@
         <v>1</v>
       </c>
       <c r="G41" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" t="n">
         <v>3.56466690612579</v>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>11.81356315809746</v>
       </c>
     </row>
@@ -1468,9 +1593,12 @@
         <v>10</v>
       </c>
       <c r="G42" t="n">
+        <v>10</v>
+      </c>
+      <c r="H42" t="n">
         <v>7.857774445006733</v>
       </c>
-      <c r="H42" t="n">
+      <c r="I42" t="n">
         <v>5.359204177699049</v>
       </c>
     </row>
@@ -1494,9 +1622,12 @@
         <v>10</v>
       </c>
       <c r="G43" t="n">
+        <v>10</v>
+      </c>
+      <c r="H43" t="n">
         <v>3.994689409680294</v>
       </c>
-      <c r="H43" t="n">
+      <c r="I43" t="n">
         <v>10.5418502702735</v>
       </c>
     </row>
@@ -1520,9 +1651,12 @@
         <v>10</v>
       </c>
       <c r="G44" t="n">
+        <v>10</v>
+      </c>
+      <c r="H44" t="n">
         <v>2.749418738833005</v>
       </c>
-      <c r="H44" t="n">
+      <c r="I44" t="n">
         <v>15.31648018481578</v>
       </c>
     </row>
@@ -1546,9 +1680,12 @@
         <v>10</v>
       </c>
       <c r="G45" t="n">
+        <v>10</v>
+      </c>
+      <c r="H45" t="n">
         <v>1.88373668613625</v>
       </c>
-      <c r="H45" t="n">
+      <c r="I45" t="n">
         <v>22.35525694383116</v>
       </c>
     </row>
@@ -1572,9 +1709,12 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
         <v>1.510288486696439</v>
       </c>
-      <c r="H46" t="n">
+      <c r="I46" t="n">
         <v>27.88302897363019</v>
       </c>
     </row>
@@ -1598,9 +1738,12 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
         <v>2.159618666600905</v>
       </c>
-      <c r="H47" t="n">
+      <c r="I47" t="n">
         <v>19.49946918146316</v>
       </c>
     </row>
@@ -1624,9 +1767,12 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
         <v>1.755304540160127</v>
       </c>
-      <c r="H48" t="n">
+      <c r="I48" t="n">
         <v>23.99094668168255</v>
       </c>
     </row>
@@ -1650,9 +1796,12 @@
         <v>1</v>
       </c>
       <c r="G49" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" t="n">
         <v>1.433198821018947</v>
       </c>
-      <c r="H49" t="n">
+      <c r="I49" t="n">
         <v>29.38281626770903</v>
       </c>
     </row>
@@ -1676,9 +1825,12 @@
         <v>1</v>
       </c>
       <c r="G50" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" t="n">
         <v>1.658137129079801</v>
       </c>
-      <c r="H50" t="n">
+      <c r="I50" t="n">
         <v>25.39682448125809</v>
       </c>
     </row>
@@ -1702,9 +1854,12 @@
         <v>1</v>
       </c>
       <c r="G51" t="n">
+        <v>1</v>
+      </c>
+      <c r="H51" t="n">
         <v>1.892338208604575</v>
       </c>
-      <c r="H51" t="n">
+      <c r="I51" t="n">
         <v>22.25364231489581</v>
       </c>
     </row>
@@ -1728,9 +1883,12 @@
         <v>1</v>
       </c>
       <c r="G52" t="n">
+        <v>1</v>
+      </c>
+      <c r="H52" t="n">
         <v>2.164543678531826</v>
       </c>
-      <c r="H52" t="n">
+      <c r="I52" t="n">
         <v>19.45510180772161</v>
       </c>
     </row>
@@ -1754,9 +1912,12 @@
         <v>1</v>
       </c>
       <c r="G53" t="n">
+        <v>1</v>
+      </c>
+      <c r="H53" t="n">
         <v>2.464650750021215</v>
       </c>
-      <c r="H53" t="n">
+      <c r="I53" t="n">
         <v>17.08616023293946</v>
       </c>
     </row>
@@ -1780,9 +1941,12 @@
         <v>1</v>
       </c>
       <c r="G54" t="n">
+        <v>1</v>
+      </c>
+      <c r="H54" t="n">
         <v>3.382715588569269</v>
       </c>
-      <c r="H54" t="n">
+      <c r="I54" t="n">
         <v>12.44899741952828</v>
       </c>
     </row>
@@ -1806,9 +1970,12 @@
         <v>1</v>
       </c>
       <c r="G55" t="n">
+        <v>1</v>
+      </c>
+      <c r="H55" t="n">
         <v>4.914819975131787</v>
       </c>
-      <c r="H55" t="n">
+      <c r="I55" t="n">
         <v>8.568252315684813</v>
       </c>
     </row>
@@ -1832,9 +1999,12 @@
         <v>2</v>
       </c>
       <c r="G56" t="n">
+        <v>2</v>
+      </c>
+      <c r="H56" t="n">
         <v>5.830471954825193</v>
       </c>
-      <c r="H56" t="n">
+      <c r="I56" t="n">
         <v>7.222643031195142</v>
       </c>
     </row>
@@ -1858,9 +2028,12 @@
         <v>2</v>
       </c>
       <c r="G57" t="n">
+        <v>2</v>
+      </c>
+      <c r="H57" t="n">
         <v>6.900976133077612</v>
       </c>
-      <c r="H57" t="n">
+      <c r="I57" t="n">
         <v>6.102240729575828</v>
       </c>
     </row>
@@ -1884,9 +2057,12 @@
         <v>10</v>
       </c>
       <c r="G58" t="n">
+        <v>10</v>
+      </c>
+      <c r="H58" t="n">
         <v>9.132551350533355</v>
       </c>
-      <c r="H58" t="n">
+      <c r="I58" t="n">
         <v>4.611133955533417</v>
       </c>
     </row>
@@ -1910,9 +2086,12 @@
         <v>10</v>
       </c>
       <c r="G59" t="n">
+        <v>10</v>
+      </c>
+      <c r="H59" t="n">
         <v>4.209557902844931</v>
       </c>
-      <c r="H59" t="n">
+      <c r="I59" t="n">
         <v>10.00376253397937</v>
       </c>
     </row>
@@ -1936,9 +2115,12 @@
         <v>10</v>
       </c>
       <c r="G60" t="n">
+        <v>10</v>
+      </c>
+      <c r="H60" t="n">
         <v>2.793610518686659</v>
       </c>
-      <c r="H60" t="n">
+      <c r="I60" t="n">
         <v>15.07419067597672</v>
       </c>
     </row>
@@ -1962,9 +2144,12 @@
         <v>10</v>
       </c>
       <c r="G61" t="n">
+        <v>10</v>
+      </c>
+      <c r="H61" t="n">
         <v>2.035428069511566</v>
       </c>
-      <c r="H61" t="n">
+      <c r="I61" t="n">
         <v>20.68921926737614</v>
       </c>
     </row>
@@ -1988,9 +2173,12 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" t="n">
         <v>1.692481677039882</v>
       </c>
-      <c r="H62" t="n">
+      <c r="I62" t="n">
         <v>24.88146146831497</v>
       </c>
     </row>
@@ -2014,9 +2202,12 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
+        <v>0</v>
+      </c>
+      <c r="H63" t="n">
         <v>1.704087220363075</v>
       </c>
-      <c r="H63" t="n">
+      <c r="I63" t="n">
         <v>24.71200835842464</v>
       </c>
     </row>
@@ -2040,9 +2231,12 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" t="n">
         <v>1.971541038015586</v>
       </c>
-      <c r="H64" t="n">
+      <c r="I64" t="n">
         <v>21.35964548599165</v>
       </c>
     </row>
@@ -2066,9 +2260,12 @@
         <v>0</v>
       </c>
       <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
         <v>1.980543492902473</v>
       </c>
-      <c r="H65" t="n">
+      <c r="I65" t="n">
         <v>21.26255635587326</v>
       </c>
     </row>
@@ -2092,9 +2289,12 @@
         <v>1</v>
       </c>
       <c r="G66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H66" t="n">
         <v>1.64684452500568</v>
       </c>
-      <c r="H66" t="n">
+      <c r="I66" t="n">
         <v>25.57097345479633</v>
       </c>
     </row>
@@ -2118,9 +2318,12 @@
         <v>1</v>
       </c>
       <c r="G67" t="n">
+        <v>1</v>
+      </c>
+      <c r="H67" t="n">
         <v>1.866650756768601</v>
       </c>
-      <c r="H67" t="n">
+      <c r="I67" t="n">
         <v>22.5598802991926</v>
       </c>
     </row>
@@ -2144,9 +2347,12 @@
         <v>1</v>
       </c>
       <c r="G68" t="n">
+        <v>1</v>
+      </c>
+      <c r="H68" t="n">
         <v>2.149802235056419</v>
       </c>
-      <c r="H68" t="n">
+      <c r="I68" t="n">
         <v>19.58850769917064</v>
       </c>
     </row>
@@ -2170,9 +2376,12 @@
         <v>1</v>
       </c>
       <c r="G69" t="n">
+        <v>1</v>
+      </c>
+      <c r="H69" t="n">
         <v>2.61503014826508</v>
       </c>
-      <c r="H69" t="n">
+      <c r="I69" t="n">
         <v>16.10360693586473</v>
       </c>
     </row>
@@ -2196,9 +2405,12 @@
         <v>1</v>
       </c>
       <c r="G70" t="n">
+        <v>1</v>
+      </c>
+      <c r="H70" t="n">
         <v>2.991192034732157</v>
       </c>
-      <c r="H70" t="n">
+      <c r="I70" t="n">
         <v>14.07847344607807</v>
       </c>
     </row>
@@ -2222,9 +2434,12 @@
         <v>2</v>
       </c>
       <c r="G71" t="n">
+        <v>2</v>
+      </c>
+      <c r="H71" t="n">
         <v>3.646798496007988</v>
       </c>
-      <c r="H71" t="n">
+      <c r="I71" t="n">
         <v>11.54750329067939</v>
       </c>
     </row>
@@ -2248,9 +2463,12 @@
         <v>2</v>
       </c>
       <c r="G72" t="n">
+        <v>2</v>
+      </c>
+      <c r="H72" t="n">
         <v>4.815086387087103</v>
       </c>
-      <c r="H72" t="n">
+      <c r="I72" t="n">
         <v>8.74572421920187</v>
       </c>
     </row>
@@ -2274,9 +2492,12 @@
         <v>2</v>
       </c>
       <c r="G73" t="n">
+        <v>2</v>
+      </c>
+      <c r="H73" t="n">
         <v>7.33873355108866</v>
       </c>
-      <c r="H73" t="n">
+      <c r="I73" t="n">
         <v>5.738240438890156</v>
       </c>
     </row>
@@ -2300,9 +2521,12 @@
         <v>2</v>
       </c>
       <c r="G74" t="n">
+        <v>2</v>
+      </c>
+      <c r="H74" t="n">
         <v>12.08575316908585</v>
       </c>
-      <c r="H74" t="n">
+      <c r="I74" t="n">
         <v>3.484385047744787</v>
       </c>
     </row>
@@ -2326,9 +2550,12 @@
         <v>2</v>
       </c>
       <c r="G75" t="n">
+        <v>2</v>
+      </c>
+      <c r="H75" t="n">
         <v>15.92123509167183</v>
       </c>
-      <c r="H75" t="n">
+      <c r="I75" t="n">
         <v>2.644984348929361</v>
       </c>
     </row>
@@ -2352,9 +2579,12 @@
         <v>2</v>
       </c>
       <c r="G76" t="n">
+        <v>2</v>
+      </c>
+      <c r="H76" t="n">
         <v>25.10920781651108</v>
       </c>
-      <c r="H76" t="n">
+      <c r="I76" t="n">
         <v>1.677130475036559</v>
       </c>
     </row>
@@ -2378,9 +2608,12 @@
         <v>100</v>
       </c>
       <c r="G77" t="n">
+        <v>100</v>
+      </c>
+      <c r="H77" t="n">
         <v>31.60460890164972</v>
       </c>
-      <c r="H77" t="n">
+      <c r="I77" t="n">
         <v>1.332445459589242</v>
       </c>
     </row>
@@ -2404,9 +2637,12 @@
         <v>100</v>
       </c>
       <c r="G78" t="n">
+        <v>100</v>
+      </c>
+      <c r="H78" t="n">
         <v>17.28187586265758</v>
       </c>
-      <c r="H78" t="n">
+      <c r="I78" t="n">
         <v>2.436738810518286</v>
       </c>
     </row>
@@ -2430,9 +2666,12 @@
         <v>10</v>
       </c>
       <c r="G79" t="n">
+        <v>10</v>
+      </c>
+      <c r="H79" t="n">
         <v>5.532867134488765</v>
       </c>
-      <c r="H79" t="n">
+      <c r="I79" t="n">
         <v>7.61113842235577</v>
       </c>
     </row>
@@ -2456,9 +2695,12 @@
         <v>10</v>
       </c>
       <c r="G80" t="n">
+        <v>10</v>
+      </c>
+      <c r="H80" t="n">
         <v>3.067089080017121</v>
       </c>
-      <c r="H80" t="n">
+      <c r="I80" t="n">
         <v>13.73009277997946</v>
       </c>
     </row>
@@ -2482,9 +2724,12 @@
         <v>10</v>
       </c>
       <c r="G81" t="n">
+        <v>10</v>
+      </c>
+      <c r="H81" t="n">
         <v>2.275781391937766</v>
       </c>
-      <c r="H81" t="n">
+      <c r="I81" t="n">
         <v>18.50415764109934</v>
       </c>
     </row>
@@ -2508,9 +2753,12 @@
         <v>0</v>
       </c>
       <c r="G82" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" t="n">
         <v>1.858165995243492</v>
       </c>
-      <c r="H82" t="n">
+      <c r="I82" t="n">
         <v>22.66289327266409</v>
       </c>
     </row>
@@ -2534,9 +2782,12 @@
         <v>0</v>
       </c>
       <c r="G83" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" t="n">
         <v>2.05874314328703</v>
       </c>
-      <c r="H83" t="n">
+      <c r="I83" t="n">
         <v>20.45491579190447</v>
       </c>
     </row>
@@ -2560,9 +2811,12 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" t="n">
         <v>2.730694052733707</v>
       </c>
-      <c r="H84" t="n">
+      <c r="I84" t="n">
         <v>15.42150706738421</v>
       </c>
     </row>
@@ -2586,9 +2840,12 @@
         <v>0</v>
       </c>
       <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" t="n">
         <v>3.508277880485534</v>
       </c>
-      <c r="H85" t="n">
+      <c r="I85" t="n">
         <v>12.00344415912368</v>
       </c>
     </row>
@@ -2612,9 +2869,12 @@
         <v>0</v>
       </c>
       <c r="G86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" t="n">
         <v>2.436738810518287</v>
       </c>
-      <c r="H86" t="n">
+      <c r="I86" t="n">
         <v>17.28187586265757</v>
       </c>
     </row>
@@ -2638,9 +2898,12 @@
         <v>1</v>
       </c>
       <c r="G87" t="n">
+        <v>1</v>
+      </c>
+      <c r="H87" t="n">
         <v>1.940353473771524</v>
       </c>
-      <c r="H87" t="n">
+      <c r="I87" t="n">
         <v>21.7029619614841</v>
       </c>
     </row>
@@ -2664,9 +2927,12 @@
         <v>1</v>
       </c>
       <c r="G88" t="n">
+        <v>1</v>
+      </c>
+      <c r="H88" t="n">
         <v>2.21441577552405</v>
       </c>
-      <c r="H88" t="n">
+      <c r="I88" t="n">
         <v>19.01694257174043</v>
       </c>
     </row>
@@ -2690,9 +2956,12 @@
         <v>1</v>
       </c>
       <c r="G89" t="n">
+        <v>1</v>
+      </c>
+      <c r="H89" t="n">
         <v>2.579532550278769</v>
       </c>
-      <c r="H89" t="n">
+      <c r="I89" t="n">
         <v>16.32521273226265</v>
       </c>
     </row>
@@ -2716,9 +2985,12 @@
         <v>1</v>
       </c>
       <c r="G90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H90" t="n">
         <v>3.195460494856385</v>
       </c>
-      <c r="H90" t="n">
+      <c r="I90" t="n">
         <v>13.17851298768428</v>
       </c>
     </row>
@@ -2742,9 +3014,12 @@
         <v>2</v>
       </c>
       <c r="G91" t="n">
+        <v>2</v>
+      </c>
+      <c r="H91" t="n">
         <v>4.003799301767846</v>
       </c>
-      <c r="H91" t="n">
+      <c r="I91" t="n">
         <v>10.51786427319245</v>
       </c>
     </row>
@@ -2768,9 +3043,12 @@
         <v>2</v>
       </c>
       <c r="G92" t="n">
+        <v>2</v>
+      </c>
+      <c r="H92" t="n">
         <v>4.621649649853573</v>
       </c>
-      <c r="H92" t="n">
+      <c r="I92" t="n">
         <v>9.111771948016681</v>
       </c>
     </row>
@@ -2794,9 +3072,12 @@
         <v>2</v>
       </c>
       <c r="G93" t="n">
+        <v>2</v>
+      </c>
+      <c r="H93" t="n">
         <v>5.120527203525829</v>
       </c>
-      <c r="H93" t="n">
+      <c r="I93" t="n">
         <v>8.224039431740612</v>
       </c>
     </row>
@@ -2820,9 +3101,12 @@
         <v>2</v>
       </c>
       <c r="G94" t="n">
+        <v>2</v>
+      </c>
+      <c r="H94" t="n">
         <v>7.157131980958146</v>
       </c>
-      <c r="H94" t="n">
+      <c r="I94" t="n">
         <v>5.883839748258957</v>
       </c>
     </row>
@@ -2846,9 +3130,12 @@
         <v>2</v>
       </c>
       <c r="G95" t="n">
+        <v>2</v>
+      </c>
+      <c r="H95" t="n">
         <v>9.756213148143731</v>
       </c>
-      <c r="H95" t="n">
+      <c r="I95" t="n">
         <v>4.316369168411337</v>
       </c>
     </row>
@@ -2872,9 +3159,12 @@
         <v>2</v>
       </c>
       <c r="G96" t="n">
+        <v>2</v>
+      </c>
+      <c r="H96" t="n">
         <v>15.95754347981189</v>
       </c>
-      <c r="H96" t="n">
+      <c r="I96" t="n">
         <v>2.638966184636918</v>
       </c>
     </row>
@@ -2898,9 +3188,12 @@
         <v>100</v>
       </c>
       <c r="G97" t="n">
+        <v>100</v>
+      </c>
+      <c r="H97" t="n">
         <v>30.47347070108647</v>
       </c>
-      <c r="H97" t="n">
+      <c r="I97" t="n">
         <v>1.381904215839632</v>
       </c>
     </row>
@@ -2924,9 +3217,12 @@
         <v>100</v>
       </c>
       <c r="G98" t="n">
+        <v>100</v>
+      </c>
+      <c r="H98" t="n">
         <v>14.01448049539119</v>
       </c>
-      <c r="H98" t="n">
+      <c r="I98" t="n">
         <v>3.00485042217196</v>
       </c>
     </row>
@@ -2950,9 +3246,12 @@
         <v>10</v>
       </c>
       <c r="G99" t="n">
+        <v>10</v>
+      </c>
+      <c r="H99" t="n">
         <v>5.52027813620713</v>
       </c>
-      <c r="H99" t="n">
+      <c r="I99" t="n">
         <v>7.628495629031982</v>
       </c>
     </row>
@@ -2976,9 +3275,12 @@
         <v>10</v>
       </c>
       <c r="G100" t="n">
+        <v>10</v>
+      </c>
+      <c r="H100" t="n">
         <v>3.390429873915228</v>
       </c>
-      <c r="H100" t="n">
+      <c r="I100" t="n">
         <v>12.42067206789537</v>
       </c>
     </row>
@@ -3002,9 +3304,12 @@
         <v>10</v>
       </c>
       <c r="G101" t="n">
+        <v>10</v>
+      </c>
+      <c r="H101" t="n">
         <v>2.90391325460475</v>
       </c>
-      <c r="H101" t="n">
+      <c r="I101" t="n">
         <v>14.50161004855108</v>
       </c>
     </row>
@@ -3028,9 +3333,12 @@
         <v>0</v>
       </c>
       <c r="G102" t="n">
+        <v>0</v>
+      </c>
+      <c r="H102" t="n">
         <v>2.189337723731022</v>
       </c>
-      <c r="H102" t="n">
+      <c r="I102" t="n">
         <v>19.23477459719259</v>
       </c>
     </row>
@@ -3054,9 +3362,12 @@
         <v>0</v>
       </c>
       <c r="G103" t="n">
+        <v>0</v>
+      </c>
+      <c r="H103" t="n">
         <v>2.464650750021215</v>
       </c>
-      <c r="H103" t="n">
+      <c r="I103" t="n">
         <v>17.08616023293946</v>
       </c>
     </row>
@@ -3080,9 +3391,12 @@
         <v>0</v>
       </c>
       <c r="G104" t="n">
+        <v>0</v>
+      </c>
+      <c r="H104" t="n">
         <v>3.224709357887811</v>
       </c>
-      <c r="H104" t="n">
+      <c r="I104" t="n">
         <v>13.05898081329102</v>
       </c>
     </row>
@@ -3106,9 +3420,12 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
+        <v>0</v>
+      </c>
+      <c r="H105" t="n">
         <v>3.344406650532939</v>
       </c>
-      <c r="H105" t="n">
+      <c r="I105" t="n">
         <v>12.59159606873355</v>
       </c>
     </row>
@@ -3132,9 +3449,12 @@
         <v>0</v>
       </c>
       <c r="G106" t="n">
+        <v>0</v>
+      </c>
+      <c r="H106" t="n">
         <v>2.250008380271464</v>
       </c>
-      <c r="H106" t="n">
+      <c r="I106" t="n">
         <v>18.71611590531772</v>
       </c>
     </row>
@@ -3158,9 +3478,12 @@
         <v>1</v>
       </c>
       <c r="G107" t="n">
+        <v>1</v>
+      </c>
+      <c r="H107" t="n">
         <v>2.130303029348465</v>
       </c>
-      <c r="H107" t="n">
+      <c r="I107" t="n">
         <v>19.76780629466425</v>
       </c>
     </row>
@@ -3184,9 +3507,12 @@
         <v>1</v>
       </c>
       <c r="G108" t="n">
+        <v>1</v>
+      </c>
+      <c r="H108" t="n">
         <v>2.36563819631443</v>
       </c>
-      <c r="H108" t="n">
+      <c r="I108" t="n">
         <v>17.80129256397061</v>
       </c>
     </row>
@@ -3210,9 +3536,12 @@
         <v>1</v>
       </c>
       <c r="G109" t="n">
+        <v>1</v>
+      </c>
+      <c r="H109" t="n">
         <v>2.984386139981755</v>
       </c>
-      <c r="H109" t="n">
+      <c r="I109" t="n">
         <v>14.11057941495277</v>
       </c>
     </row>
@@ -3236,9 +3565,12 @@
         <v>2</v>
       </c>
       <c r="G110" t="n">
+        <v>2</v>
+      </c>
+      <c r="H110" t="n">
         <v>3.398161751694496</v>
       </c>
-      <c r="H110" t="n">
+      <c r="I110" t="n">
         <v>12.39241116527135</v>
       </c>
     </row>
@@ -3262,9 +3594,12 @@
         <v>2</v>
       </c>
       <c r="G111" t="n">
+        <v>2</v>
+      </c>
+      <c r="H111" t="n">
         <v>4.022081458667099</v>
       </c>
-      <c r="H111" t="n">
+      <c r="I111" t="n">
         <v>10.47005588172559</v>
       </c>
     </row>
@@ -3288,9 +3623,12 @@
         <v>2</v>
       </c>
       <c r="G112" t="n">
+        <v>2</v>
+      </c>
+      <c r="H112" t="n">
         <v>6.074503319580139</v>
       </c>
-      <c r="H112" t="n">
+      <c r="I112" t="n">
         <v>6.932487384994562</v>
       </c>
     </row>
@@ -3314,9 +3652,12 @@
         <v>2</v>
       </c>
       <c r="G113" t="n">
+        <v>2</v>
+      </c>
+      <c r="H113" t="n">
         <v>8.020530411659378</v>
       </c>
-      <c r="H113" t="n">
+      <c r="I113" t="n">
         <v>5.250452959056161</v>
       </c>
     </row>
@@ -3340,9 +3681,12 @@
         <v>2</v>
       </c>
       <c r="G114" t="n">
+        <v>2</v>
+      </c>
+      <c r="H114" t="n">
         <v>7.38905609893065</v>
       </c>
-      <c r="H114" t="n">
+      <c r="I114" t="n">
         <v>5.699160632870456</v>
       </c>
     </row>
@@ -3366,9 +3710,12 @@
         <v>2</v>
       </c>
       <c r="G115" t="n">
+        <v>2</v>
+      </c>
+      <c r="H115" t="n">
         <v>9.008581981902688</v>
       </c>
-      <c r="H115" t="n">
+      <c r="I115" t="n">
         <v>4.674588932830317</v>
       </c>
     </row>
@@ -3392,9 +3739,12 @@
         <v>2</v>
       </c>
       <c r="G116" t="n">
+        <v>2</v>
+      </c>
+      <c r="H116" t="n">
         <v>15.24685994048192</v>
       </c>
-      <c r="H116" t="n">
+      <c r="I116" t="n">
         <v>2.761973140534133</v>
       </c>
     </row>
@@ -3418,9 +3768,12 @@
         <v>100</v>
       </c>
       <c r="G117" t="n">
+        <v>100</v>
+      </c>
+      <c r="H117" t="n">
         <v>29.71938553256001</v>
       </c>
-      <c r="H117" t="n">
+      <c r="I117" t="n">
         <v>1.416967978256496</v>
       </c>
     </row>
@@ -3444,9 +3797,12 @@
         <v>100</v>
       </c>
       <c r="G118" t="n">
+        <v>100</v>
+      </c>
+      <c r="H118" t="n">
         <v>20.45491579190448</v>
       </c>
-      <c r="H118" t="n">
+      <c r="I118" t="n">
         <v>2.058743143287029</v>
       </c>
     </row>
@@ -3470,9 +3826,12 @@
         <v>10</v>
       </c>
       <c r="G119" t="n">
+        <v>10</v>
+      </c>
+      <c r="H119" t="n">
         <v>4.209557902844931</v>
       </c>
-      <c r="H119" t="n">
+      <c r="I119" t="n">
         <v>10.00376253397937</v>
       </c>
     </row>
@@ -3496,9 +3855,12 @@
         <v>0</v>
       </c>
       <c r="G120" t="n">
+        <v>0</v>
+      </c>
+      <c r="H120" t="n">
         <v>2.651016237649828</v>
       </c>
-      <c r="H120" t="n">
+      <c r="I120" t="n">
         <v>15.88500931643837</v>
       </c>
     </row>
@@ -3522,9 +3884,12 @@
         <v>0</v>
       </c>
       <c r="G121" t="n">
+        <v>0</v>
+      </c>
+      <c r="H121" t="n">
         <v>3.730822436068817</v>
       </c>
-      <c r="H121" t="n">
+      <c r="I121" t="n">
         <v>11.28743550643752</v>
       </c>
     </row>
@@ -3548,9 +3913,12 @@
         <v>2</v>
       </c>
       <c r="G122" t="n">
+        <v>2</v>
+      </c>
+      <c r="H122" t="n">
         <v>4.590174291905306</v>
       </c>
-      <c r="H122" t="n">
+      <c r="I122" t="n">
         <v>9.17425242596118</v>
       </c>
     </row>
@@ -3574,9 +3942,12 @@
         <v>2</v>
       </c>
       <c r="G123" t="n">
+        <v>2</v>
+      </c>
+      <c r="H123" t="n">
         <v>3.067089080017121</v>
       </c>
-      <c r="H123" t="n">
+      <c r="I123" t="n">
         <v>13.73009277997946</v>
       </c>
     </row>
@@ -3600,9 +3971,12 @@
         <v>2</v>
       </c>
       <c r="G124" t="n">
+        <v>2</v>
+      </c>
+      <c r="H124" t="n">
         <v>2.626970904497728</v>
       </c>
-      <c r="H124" t="n">
+      <c r="I124" t="n">
         <v>16.03040884883669</v>
       </c>
     </row>
@@ -3626,9 +4000,12 @@
         <v>2</v>
       </c>
       <c r="G125" t="n">
+        <v>2</v>
+      </c>
+      <c r="H125" t="n">
         <v>2.78725418350556</v>
       </c>
-      <c r="H125" t="n">
+      <c r="I125" t="n">
         <v>15.10856737871424</v>
       </c>
     </row>
@@ -3652,9 +4029,12 @@
         <v>2</v>
       </c>
       <c r="G126" t="n">
+        <v>2</v>
+      </c>
+      <c r="H126" t="n">
         <v>3.173698078726824</v>
       </c>
-      <c r="H126" t="n">
+      <c r="I126" t="n">
         <v>13.26887958100618</v>
       </c>
     </row>
@@ -3678,9 +4058,12 @@
         <v>2</v>
       </c>
       <c r="G127" t="n">
+        <v>2</v>
+      </c>
+      <c r="H127" t="n">
         <v>2.991192034732157</v>
       </c>
-      <c r="H127" t="n">
+      <c r="I127" t="n">
         <v>14.07847344607807</v>
       </c>
     </row>
@@ -3704,9 +4087,12 @@
         <v>2</v>
       </c>
       <c r="G128" t="n">
+        <v>2</v>
+      </c>
+      <c r="H128" t="n">
         <v>4.257776827668183</v>
       </c>
-      <c r="H128" t="n">
+      <c r="I128" t="n">
         <v>9.89047085780672</v>
       </c>
     </row>
@@ -3730,9 +4116,12 @@
         <v>2</v>
       </c>
       <c r="G129" t="n">
+        <v>2</v>
+      </c>
+      <c r="H129" t="n">
         <v>4.685249336272087</v>
       </c>
-      <c r="H129" t="n">
+      <c r="I129" t="n">
         <v>8.988084648362323</v>
       </c>
     </row>
@@ -3756,9 +4145,12 @@
         <v>2</v>
       </c>
       <c r="G130" t="n">
+        <v>2</v>
+      </c>
+      <c r="H130" t="n">
         <v>5.132204569516401</v>
       </c>
-      <c r="H130" t="n">
+      <c r="I130" t="n">
         <v>8.205327177179338</v>
       </c>
     </row>
@@ -3782,9 +4174,12 @@
         <v>2</v>
       </c>
       <c r="G131" t="n">
+        <v>2</v>
+      </c>
+      <c r="H131" t="n">
         <v>6.59363495933794</v>
       </c>
-      <c r="H131" t="n">
+      <c r="I131" t="n">
         <v>6.386677135266413</v>
       </c>
     </row>
@@ -3808,9 +4203,12 @@
         <v>2</v>
       </c>
       <c r="G132" t="n">
+        <v>2</v>
+      </c>
+      <c r="H132" t="n">
         <v>10.51786427319245</v>
       </c>
-      <c r="H132" t="n">
+      <c r="I132" t="n">
         <v>4.003799301767844</v>
       </c>
     </row>
@@ -3834,9 +4232,12 @@
         <v>2</v>
       </c>
       <c r="G133" t="n">
+        <v>2</v>
+      </c>
+      <c r="H133" t="n">
         <v>15.03989219095908</v>
       </c>
-      <c r="H133" t="n">
+      <c r="I133" t="n">
         <v>2.799981349494734</v>
       </c>
     </row>
@@ -3860,9 +4261,12 @@
         <v>2</v>
       </c>
       <c r="G134" t="n">
+        <v>2</v>
+      </c>
+      <c r="H134" t="n">
         <v>21.8517816909397</v>
       </c>
-      <c r="H134" t="n">
+      <c r="I134" t="n">
         <v>1.927138858913155</v>
       </c>
     </row>
@@ -3886,9 +4290,12 @@
         <v>100</v>
       </c>
       <c r="G135" t="n">
+        <v>100</v>
+      </c>
+      <c r="H135" t="n">
         <v>30.47347070108647</v>
       </c>
-      <c r="H135" t="n">
+      <c r="I135" t="n">
         <v>1.381904215839632</v>
       </c>
     </row>
@@ -3912,9 +4319,12 @@
         <v>10</v>
       </c>
       <c r="G136" t="n">
+        <v>10</v>
+      </c>
+      <c r="H136" t="n">
         <v>4.277218697287138</v>
       </c>
-      <c r="H136" t="n">
+      <c r="I136" t="n">
         <v>9.845514249670336</v>
       </c>
     </row>
@@ -3938,9 +4348,12 @@
         <v>100</v>
       </c>
       <c r="G137" t="n">
+        <v>100</v>
+      </c>
+      <c r="H137" t="n">
         <v>3.359677887303711</v>
       </c>
-      <c r="H137" t="n">
+      <c r="I137" t="n">
         <v>12.53436163991696</v>
       </c>
     </row>
@@ -3964,9 +4377,12 @@
         <v>100</v>
       </c>
       <c r="G138" t="n">
+        <v>100</v>
+      </c>
+      <c r="H138" t="n">
         <v>4.497028550210074</v>
       </c>
-      <c r="H138" t="n">
+      <c r="I138" t="n">
         <v>9.364276246618385</v>
       </c>
     </row>
@@ -3990,9 +4406,12 @@
         <v>2</v>
       </c>
       <c r="G139" t="n">
+        <v>2</v>
+      </c>
+      <c r="H139" t="n">
         <v>5.951236950777927</v>
       </c>
-      <c r="H139" t="n">
+      <c r="I139" t="n">
         <v>7.076078129873864</v>
       </c>
     </row>
@@ -4016,9 +4435,12 @@
         <v>2</v>
       </c>
       <c r="G140" t="n">
+        <v>2</v>
+      </c>
+      <c r="H140" t="n">
         <v>5.085654281771596</v>
       </c>
-      <c r="H140" t="n">
+      <c r="I140" t="n">
         <v>8.280432624772779</v>
       </c>
     </row>
@@ -4042,9 +4464,12 @@
         <v>2</v>
       </c>
       <c r="G141" t="n">
+        <v>2</v>
+      </c>
+      <c r="H141" t="n">
         <v>3.246821564279982</v>
       </c>
-      <c r="H141" t="n">
+      <c r="I141" t="n">
         <v>12.97004371795084</v>
       </c>
     </row>
@@ -4068,9 +4493,12 @@
         <v>2</v>
       </c>
       <c r="G142" t="n">
+        <v>2</v>
+      </c>
+      <c r="H142" t="n">
         <v>3.137756244463604</v>
       </c>
-      <c r="H142" t="n">
+      <c r="I142" t="n">
         <v>13.42086967634919</v>
       </c>
     </row>
@@ -4094,9 +4522,12 @@
         <v>2</v>
       </c>
       <c r="G143" t="n">
+        <v>2</v>
+      </c>
+      <c r="H143" t="n">
         <v>3.931497911153397</v>
       </c>
-      <c r="H143" t="n">
+      <c r="I143" t="n">
         <v>10.7112908577745</v>
       </c>
     </row>
@@ -4120,9 +4551,12 @@
         <v>2</v>
       </c>
       <c r="G144" t="n">
+        <v>2</v>
+      </c>
+      <c r="H144" t="n">
         <v>3.67180501661647</v>
       </c>
-      <c r="H144" t="n">
+      <c r="I144" t="n">
         <v>11.46885998644398</v>
       </c>
     </row>
@@ -4146,9 +4580,12 @@
         <v>2</v>
       </c>
       <c r="G145" t="n">
+        <v>2</v>
+      </c>
+      <c r="H145" t="n">
         <v>4.296749342412553</v>
       </c>
-      <c r="H145" t="n">
+      <c r="I145" t="n">
         <v>9.800761989400121</v>
       </c>
     </row>
@@ -4172,9 +4609,12 @@
         <v>2</v>
       </c>
       <c r="G146" t="n">
+        <v>2</v>
+      </c>
+      <c r="H146" t="n">
         <v>7.173453825616434</v>
       </c>
-      <c r="H146" t="n">
+      <c r="I146" t="n">
         <v>5.870452177822188</v>
       </c>
     </row>
@@ -4198,9 +4638,12 @@
         <v>2</v>
       </c>
       <c r="G147" t="n">
+        <v>2</v>
+      </c>
+      <c r="H147" t="n">
         <v>5.897257849059788</v>
       </c>
-      <c r="H147" t="n">
+      <c r="I147" t="n">
         <v>7.140847273586793</v>
       </c>
     </row>
@@ -4224,9 +4667,12 @@
         <v>2</v>
       </c>
       <c r="G148" t="n">
+        <v>2</v>
+      </c>
+      <c r="H148" t="n">
         <v>6.59363495933794</v>
       </c>
-      <c r="H148" t="n">
+      <c r="I148" t="n">
         <v>6.386677135266413</v>
       </c>
     </row>
@@ -4250,9 +4696,12 @@
         <v>2</v>
       </c>
       <c r="G149" t="n">
+        <v>2</v>
+      </c>
+      <c r="H149" t="n">
         <v>11.26175307041645</v>
       </c>
-      <c r="H149" t="n">
+      <c r="I149" t="n">
         <v>3.739330579332233</v>
       </c>
     </row>
@@ -4276,9 +4725,12 @@
         <v>2</v>
       </c>
       <c r="G150" t="n">
+        <v>2</v>
+      </c>
+      <c r="H150" t="n">
         <v>21.16590853922112</v>
       </c>
-      <c r="H150" t="n">
+      <c r="I150" t="n">
         <v>1.989587054818038</v>
       </c>
     </row>
@@ -4302,9 +4754,12 @@
         <v>2</v>
       </c>
       <c r="G151" t="n">
+        <v>2</v>
+      </c>
+      <c r="H151" t="n">
         <v>40.41967327539025</v>
       </c>
-      <c r="H151" t="n">
+      <c r="I151" t="n">
         <v>1.041854478787603</v>
       </c>
     </row>
@@ -4328,9 +4783,12 @@
         <v>100</v>
       </c>
       <c r="G152" t="n">
+        <v>100</v>
+      </c>
+      <c r="H152" t="n">
         <v>39.06191939043615</v>
       </c>
-      <c r="H152" t="n">
+      <c r="I152" t="n">
         <v>1.078068315388706</v>
       </c>
     </row>
@@ -4354,9 +4812,12 @@
         <v>100</v>
       </c>
       <c r="G153" t="n">
+        <v>100</v>
+      </c>
+      <c r="H153" t="n">
         <v>6.684371632937881</v>
       </c>
-      <c r="H153" t="n">
+      <c r="I153" t="n">
         <v>6.299981500966952</v>
       </c>
     </row>
@@ -4380,9 +4841,12 @@
         <v>100</v>
       </c>
       <c r="G154" t="n">
+        <v>100</v>
+      </c>
+      <c r="H154" t="n">
         <v>4.199979845769421</v>
       </c>
-      <c r="H154" t="n">
+      <c r="I154" t="n">
         <v>10.02657612167238</v>
       </c>
     </row>
@@ -4406,9 +4870,12 @@
         <v>2</v>
       </c>
       <c r="G155" t="n">
+        <v>2</v>
+      </c>
+      <c r="H155" t="n">
         <v>4.84810399337989</v>
       </c>
-      <c r="H155" t="n">
+      <c r="I155" t="n">
         <v>8.686162196726857</v>
       </c>
     </row>
@@ -4432,9 +4899,12 @@
         <v>2</v>
       </c>
       <c r="G156" t="n">
+        <v>2</v>
+      </c>
+      <c r="H156" t="n">
         <v>5.3836753872296</v>
       </c>
-      <c r="H156" t="n">
+      <c r="I156" t="n">
         <v>7.822057350074953</v>
       </c>
     </row>
@@ -4458,9 +4928,12 @@
         <v>2</v>
       </c>
       <c r="G157" t="n">
+        <v>2</v>
+      </c>
+      <c r="H157" t="n">
         <v>5.764442404603849</v>
       </c>
-      <c r="H157" t="n">
+      <c r="I157" t="n">
         <v>7.305375728876059</v>
       </c>
     </row>
@@ -4484,9 +4957,12 @@
         <v>2</v>
       </c>
       <c r="G158" t="n">
+        <v>2</v>
+      </c>
+      <c r="H158" t="n">
         <v>4.05889659372358</v>
       </c>
-      <c r="H158" t="n">
+      <c r="I158" t="n">
         <v>10.37509004250449</v>
       </c>
     </row>
@@ -4510,9 +4986,12 @@
         <v>2</v>
       </c>
       <c r="G159" t="n">
+        <v>2</v>
+      </c>
+      <c r="H159" t="n">
         <v>6.91671381413957</v>
       </c>
-      <c r="H159" t="n">
+      <c r="I159" t="n">
         <v>6.088356228793241</v>
       </c>
     </row>
@@ -4536,9 +5015,12 @@
         <v>2</v>
       </c>
       <c r="G160" t="n">
+        <v>2</v>
+      </c>
+      <c r="H160" t="n">
         <v>8.205327177179342</v>
       </c>
-      <c r="H160" t="n">
+      <c r="I160" t="n">
         <v>5.132204569516397</v>
       </c>
     </row>
@@ -4562,9 +5044,12 @@
         <v>2</v>
       </c>
       <c r="G161" t="n">
+        <v>2</v>
+      </c>
+      <c r="H161" t="n">
         <v>8.186657498833034</v>
       </c>
-      <c r="H161" t="n">
+      <c r="I161" t="n">
         <v>5.143908565748557</v>
       </c>
     </row>
@@ -4588,9 +5073,12 @@
         <v>2</v>
       </c>
       <c r="G162" t="n">
+        <v>2</v>
+      </c>
+      <c r="H162" t="n">
         <v>11.52122911934112</v>
       </c>
-      <c r="H162" t="n">
+      <c r="I162" t="n">
         <v>3.65511502261533</v>
       </c>
     </row>
@@ -4614,9 +5102,12 @@
         <v>2</v>
       </c>
       <c r="G163" t="n">
+        <v>2</v>
+      </c>
+      <c r="H163" t="n">
         <v>20.13134200466594</v>
       </c>
-      <c r="H163" t="n">
+      <c r="I163" t="n">
         <v>2.091833600727489</v>
       </c>
     </row>
@@ -4640,9 +5131,12 @@
         <v>100</v>
       </c>
       <c r="G164" t="n">
+        <v>100</v>
+      </c>
+      <c r="H164" t="n">
         <v>42.11141763309691</v>
       </c>
-      <c r="H164" t="n">
+      <c r="I164" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4666,9 +5160,12 @@
         <v>100</v>
       </c>
       <c r="G165" t="n">
+        <v>100</v>
+      </c>
+      <c r="H165" t="n">
         <v>42.0156010245766</v>
       </c>
-      <c r="H165" t="n">
+      <c r="I165" t="n">
         <v>1.002280500723154</v>
       </c>
     </row>
@@ -4692,9 +5189,12 @@
         <v>100</v>
       </c>
       <c r="G166" t="n">
+        <v>100</v>
+      </c>
+      <c r="H166" t="n">
         <v>7.839895557518359</v>
       </c>
-      <c r="H166" t="n">
+      <c r="I166" t="n">
         <v>5.371425846701823</v>
       </c>
     </row>
@@ -4718,9 +5218,12 @@
         <v>100</v>
       </c>
       <c r="G167" t="n">
+        <v>100</v>
+      </c>
+      <c r="H167" t="n">
         <v>9.19517431525299</v>
       </c>
-      <c r="H167" t="n">
+      <c r="I167" t="n">
         <v>4.579730213840789</v>
       </c>
     </row>
@@ -4744,9 +5247,12 @@
         <v>100</v>
       </c>
       <c r="G168" t="n">
+        <v>100</v>
+      </c>
+      <c r="H168" t="n">
         <v>7.059977845292225</v>
       </c>
-      <c r="H168" t="n">
+      <c r="I168" t="n">
         <v>5.964808750947836</v>
       </c>
     </row>
@@ -4770,9 +5276,12 @@
         <v>2</v>
       </c>
       <c r="G169" t="n">
+        <v>2</v>
+      </c>
+      <c r="H169" t="n">
         <v>5.408258337249224</v>
       </c>
-      <c r="H169" t="n">
+      <c r="I169" t="n">
         <v>7.786502605294522</v>
       </c>
     </row>
@@ -4796,9 +5305,12 @@
         <v>2</v>
       </c>
       <c r="G170" t="n">
+        <v>2</v>
+      </c>
+      <c r="H170" t="n">
         <v>6.401241957091944</v>
       </c>
-      <c r="H170" t="n">
+      <c r="I170" t="n">
         <v>6.578632383430159</v>
       </c>
     </row>
@@ -4822,9 +5334,12 @@
         <v>2</v>
       </c>
       <c r="G171" t="n">
+        <v>2</v>
+      </c>
+      <c r="H171" t="n">
         <v>9.958290964567235</v>
       </c>
-      <c r="H171" t="n">
+      <c r="I171" t="n">
         <v>4.228779595106657</v>
       </c>
     </row>
@@ -4848,9 +5363,12 @@
         <v>2</v>
       </c>
       <c r="G172" t="n">
+        <v>2</v>
+      </c>
+      <c r="H172" t="n">
         <v>13.82424161996467</v>
       </c>
-      <c r="H172" t="n">
+      <c r="I172" t="n">
         <v>3.04620092665919</v>
       </c>
     </row>
@@ -4874,9 +5392,12 @@
         <v>2</v>
       </c>
       <c r="G173" t="n">
+        <v>2</v>
+      </c>
+      <c r="H173" t="n">
         <v>15.10856737871425</v>
       </c>
-      <c r="H173" t="n">
+      <c r="I173" t="n">
         <v>2.787254183505558</v>
       </c>
     </row>
@@ -4900,9 +5421,12 @@
         <v>100</v>
       </c>
       <c r="G174" t="n">
+        <v>100</v>
+      </c>
+      <c r="H174" t="n">
         <v>27.25505967320341</v>
       </c>
-      <c r="H174" t="n">
+      <c r="I174" t="n">
         <v>1.545086238592974</v>
       </c>
     </row>
@@ -4926,9 +5450,12 @@
         <v>100</v>
       </c>
       <c r="G175" t="n">
+        <v>100</v>
+      </c>
+      <c r="H175" t="n">
         <v>25.28138456919253</v>
       </c>
-      <c r="H175" t="n">
+      <c r="I175" t="n">
         <v>1.6657085183702</v>
       </c>
     </row>
@@ -4952,9 +5479,12 @@
         <v>100</v>
       </c>
       <c r="G176" t="n">
+        <v>100</v>
+      </c>
+      <c r="H176" t="n">
         <v>7.965907260886808</v>
       </c>
-      <c r="H176" t="n">
+      <c r="I176" t="n">
         <v>5.286455924470408</v>
       </c>
     </row>
@@ -4978,9 +5508,12 @@
         <v>100</v>
       </c>
       <c r="G177" t="n">
+        <v>100</v>
+      </c>
+      <c r="H177" t="n">
         <v>10.4700558817256</v>
       </c>
-      <c r="H177" t="n">
+      <c r="I177" t="n">
         <v>4.022081458667096</v>
       </c>
     </row>
@@ -5004,9 +5537,12 @@
         <v>100</v>
       </c>
       <c r="G178" t="n">
+        <v>100</v>
+      </c>
+      <c r="H178" t="n">
         <v>16.93118479021815</v>
       </c>
-      <c r="H178" t="n">
+      <c r="I178" t="n">
         <v>2.487210325495143</v>
       </c>
     </row>
@@ -5030,9 +5566,12 @@
         <v>100</v>
       </c>
       <c r="G179" t="n">
+        <v>100</v>
+      </c>
+      <c r="H179" t="n">
         <v>28.26673436747747</v>
       </c>
-      <c r="H179" t="n">
+      <c r="I179" t="n">
         <v>1.489787149998783</v>
       </c>
     </row>
@@ -5056,9 +5595,12 @@
         <v>100</v>
       </c>
       <c r="G180" t="n">
+        <v>100</v>
+      </c>
+      <c r="H180" t="n">
         <v>27.75628815155564</v>
       </c>
-      <c r="H180" t="n">
+      <c r="I180" t="n">
         <v>1.51718476920109</v>
       </c>
     </row>

</xml_diff>

<commit_message>
introduced DEM class, solved e_map extent problem
</commit_message>
<xml_diff>
--- a/output/xyz_age_eros.xlsx
+++ b/output/xyz_age_eros.xlsx
@@ -394,12 +394,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>E_map1</t>
+          <t>e_map0</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>E_map2</t>
+          <t>slope_map</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -433,7 +433,7 @@
         <v>10</v>
       </c>
       <c r="G2" t="n">
-        <v>10</v>
+        <v>24.4635181427002</v>
       </c>
       <c r="H2" t="n">
         <v>1.71577234424401</v>
@@ -462,7 +462,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="n">
-        <v>10</v>
+        <v>9.773893356323242</v>
       </c>
       <c r="H3" t="n">
         <v>2.527187593999784</v>
@@ -491,7 +491,7 @@
         <v>10</v>
       </c>
       <c r="G4" t="n">
-        <v>10</v>
+        <v>21.83255004882812</v>
       </c>
       <c r="H4" t="n">
         <v>1.513732700682522</v>
@@ -520,7 +520,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>14.68150901794434</v>
       </c>
       <c r="H5" t="n">
         <v>1.205371905865509</v>
@@ -549,7 +549,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>3.095420360565186</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
@@ -578,7 +578,7 @@
         <v>10</v>
       </c>
       <c r="G7" t="n">
-        <v>10</v>
+        <v>32.97629928588867</v>
       </c>
       <c r="H7" t="n">
         <v>7.38905609893065</v>
@@ -607,7 +607,7 @@
         <v>10</v>
       </c>
       <c r="G8" t="n">
-        <v>10</v>
+        <v>31.45109176635742</v>
       </c>
       <c r="H8" t="n">
         <v>3.276540548249262</v>
@@ -636,7 +636,7 @@
         <v>10</v>
       </c>
       <c r="G9" t="n">
-        <v>10</v>
+        <v>28.87717819213867</v>
       </c>
       <c r="H9" t="n">
         <v>2.475904843525316</v>
@@ -665,7 +665,7 @@
         <v>10</v>
       </c>
       <c r="G10" t="n">
-        <v>10</v>
+        <v>19.84463691711426</v>
       </c>
       <c r="H10" t="n">
         <v>1.53806313144631</v>
@@ -694,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>23.04996681213379</v>
       </c>
       <c r="H11" t="n">
         <v>1.276007117771601</v>
@@ -723,7 +723,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
+        <v>6.289937973022461</v>
       </c>
       <c r="H12" t="n">
         <v>1.136056031253367</v>
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="n">
-        <v>1</v>
+        <v>16.42742156982422</v>
       </c>
       <c r="H13" t="n">
         <v>1.763319615489954</v>
@@ -781,7 +781,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>1</v>
+        <v>30.03357315063477</v>
       </c>
       <c r="H14" t="n">
         <v>1.598791916034733</v>
@@ -810,7 +810,7 @@
         <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
+        <v>15.9727783203125</v>
       </c>
       <c r="H15" t="n">
         <v>1.650600155135878</v>
@@ -839,7 +839,7 @@
         <v>10</v>
       </c>
       <c r="G16" t="n">
-        <v>10</v>
+        <v>45.71837615966797</v>
       </c>
       <c r="H16" t="n">
         <v>11.05838613157211</v>
@@ -868,7 +868,7 @@
         <v>10</v>
       </c>
       <c r="G17" t="n">
-        <v>10</v>
+        <v>34.67289352416992</v>
       </c>
       <c r="H17" t="n">
         <v>4.326212651421302</v>
@@ -897,7 +897,7 @@
         <v>10</v>
       </c>
       <c r="G18" t="n">
-        <v>10</v>
+        <v>25.14361763000488</v>
       </c>
       <c r="H18" t="n">
         <v>2.338847564732744</v>
@@ -926,7 +926,7 @@
         <v>10</v>
       </c>
       <c r="G19" t="n">
-        <v>10</v>
+        <v>18.22125625610352</v>
       </c>
       <c r="H19" t="n">
         <v>1.858165995243492</v>
@@ -955,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>1</v>
+        <v>12.19136142730713</v>
       </c>
       <c r="H20" t="n">
         <v>1.338529674884737</v>
@@ -984,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>1</v>
+        <v>6.548885822296143</v>
       </c>
       <c r="H21" t="n">
         <v>1.183605064314989</v>
@@ -1013,7 +1013,7 @@
         <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>7.029293537139893</v>
       </c>
       <c r="H22" t="n">
         <v>1.213637280943926</v>
@@ -1042,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="G23" t="n">
-        <v>1</v>
+        <v>22.74278450012207</v>
       </c>
       <c r="H23" t="n">
         <v>1.50000279342122</v>
@@ -1071,7 +1071,7 @@
         <v>1</v>
       </c>
       <c r="G24" t="n">
-        <v>1</v>
+        <v>20.18801498413086</v>
       </c>
       <c r="H24" t="n">
         <v>1.631907262573603</v>
@@ -1100,7 +1100,7 @@
         <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>1</v>
+        <v>13.17729949951172</v>
       </c>
       <c r="H25" t="n">
         <v>2.270603279516831</v>
@@ -1129,7 +1129,7 @@
         <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>1</v>
+        <v>17.44259071350098</v>
       </c>
       <c r="H26" t="n">
         <v>2.021565957079946</v>
@@ -1158,7 +1158,7 @@
         <v>10</v>
       </c>
       <c r="G27" t="n">
-        <v>10</v>
+        <v>34.70832443237305</v>
       </c>
       <c r="H27" t="n">
         <v>17.40037969153265</v>
@@ -1187,7 +1187,7 @@
         <v>10</v>
       </c>
       <c r="G28" t="n">
-        <v>10</v>
+        <v>37.59332656860352</v>
       </c>
       <c r="H28" t="n">
         <v>9.070354874271228</v>
@@ -1216,7 +1216,7 @@
         <v>10</v>
       </c>
       <c r="G29" t="n">
-        <v>10</v>
+        <v>27.64423370361328</v>
       </c>
       <c r="H29" t="n">
         <v>4.238423330031359</v>
@@ -1245,7 +1245,7 @@
         <v>10</v>
       </c>
       <c r="G30" t="n">
-        <v>10</v>
+        <v>27.57571983337402</v>
       </c>
       <c r="H30" t="n">
         <v>2.755688790255169</v>
@@ -1274,7 +1274,7 @@
         <v>10</v>
       </c>
       <c r="G31" t="n">
-        <v>10</v>
+        <v>12.55493831634521</v>
       </c>
       <c r="H31" t="n">
         <v>1.743350185569119</v>
@@ -1303,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>10.44246959686279</v>
       </c>
       <c r="H32" t="n">
         <v>1.385055649403185</v>
@@ -1332,7 +1332,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>22.38632392883301</v>
       </c>
       <c r="H33" t="n">
         <v>1.545086238592975</v>
@@ -1361,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="G34" t="n">
-        <v>1</v>
+        <v>11.05756378173828</v>
       </c>
       <c r="H34" t="n">
         <v>1.335484102423399</v>
@@ -1390,7 +1390,7 @@
         <v>1</v>
       </c>
       <c r="G35" t="n">
-        <v>1</v>
+        <v>6.659310340881348</v>
       </c>
       <c r="H35" t="n">
         <v>1.385055649403185</v>
@@ -1419,7 +1419,7 @@
         <v>1</v>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>8.873861312866211</v>
       </c>
       <c r="H36" t="n">
         <v>1.503423550876351</v>
@@ -1448,7 +1448,7 @@
         <v>1</v>
       </c>
       <c r="G37" t="n">
-        <v>1</v>
+        <v>20.56237983703613</v>
       </c>
       <c r="H37" t="n">
         <v>2.072860184000009</v>
@@ -1477,7 +1477,7 @@
         <v>1</v>
       </c>
       <c r="G38" t="n">
-        <v>1</v>
+        <v>10.81160545349121</v>
       </c>
       <c r="H38" t="n">
         <v>2.699769197680611</v>
@@ -1506,7 +1506,7 @@
         <v>1</v>
       </c>
       <c r="G39" t="n">
-        <v>1</v>
+        <v>15.86988353729248</v>
       </c>
       <c r="H39" t="n">
         <v>2.812766630296358</v>
@@ -1535,7 +1535,7 @@
         <v>1</v>
       </c>
       <c r="G40" t="n">
-        <v>1</v>
+        <v>16.63455390930176</v>
       </c>
       <c r="H40" t="n">
         <v>4.486796407757537</v>
@@ -1564,7 +1564,7 @@
         <v>1</v>
       </c>
       <c r="G41" t="n">
-        <v>1</v>
+        <v>17.32051658630371</v>
       </c>
       <c r="H41" t="n">
         <v>3.56466690612579</v>
@@ -1593,7 +1593,7 @@
         <v>10</v>
       </c>
       <c r="G42" t="n">
-        <v>10</v>
+        <v>33.39544296264648</v>
       </c>
       <c r="H42" t="n">
         <v>7.857774445006733</v>
@@ -1622,7 +1622,7 @@
         <v>10</v>
       </c>
       <c r="G43" t="n">
-        <v>10</v>
+        <v>25.49657249450684</v>
       </c>
       <c r="H43" t="n">
         <v>3.994689409680294</v>
@@ -1651,7 +1651,7 @@
         <v>10</v>
       </c>
       <c r="G44" t="n">
-        <v>10</v>
+        <v>20.20866012573242</v>
       </c>
       <c r="H44" t="n">
         <v>2.749418738833005</v>
@@ -1680,7 +1680,7 @@
         <v>10</v>
       </c>
       <c r="G45" t="n">
-        <v>10</v>
+        <v>15.97757530212402</v>
       </c>
       <c r="H45" t="n">
         <v>1.88373668613625</v>
@@ -1709,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>8.469196319580078</v>
       </c>
       <c r="H46" t="n">
         <v>1.510288486696439</v>
@@ -1738,7 +1738,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>0</v>
+        <v>29.8424186706543</v>
       </c>
       <c r="H47" t="n">
         <v>2.159618666600905</v>
@@ -1767,7 +1767,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>0</v>
+        <v>25.46588706970215</v>
       </c>
       <c r="H48" t="n">
         <v>1.755304540160127</v>
@@ -1796,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="G49" t="n">
-        <v>1</v>
+        <v>10.4645938873291</v>
       </c>
       <c r="H49" t="n">
         <v>1.433198821018947</v>
@@ -1825,7 +1825,7 @@
         <v>1</v>
       </c>
       <c r="G50" t="n">
-        <v>1</v>
+        <v>9.380246162414551</v>
       </c>
       <c r="H50" t="n">
         <v>1.658137129079801</v>
@@ -1854,7 +1854,7 @@
         <v>1</v>
       </c>
       <c r="G51" t="n">
-        <v>1</v>
+        <v>8.513031959533691</v>
       </c>
       <c r="H51" t="n">
         <v>1.892338208604575</v>
@@ -1883,7 +1883,7 @@
         <v>1</v>
       </c>
       <c r="G52" t="n">
-        <v>1</v>
+        <v>6.238790035247803</v>
       </c>
       <c r="H52" t="n">
         <v>2.164543678531826</v>
@@ -1912,7 +1912,7 @@
         <v>1</v>
       </c>
       <c r="G53" t="n">
-        <v>1</v>
+        <v>9.315567016601562</v>
       </c>
       <c r="H53" t="n">
         <v>2.464650750021215</v>
@@ -1941,7 +1941,7 @@
         <v>1</v>
       </c>
       <c r="G54" t="n">
-        <v>1</v>
+        <v>21.94803619384766</v>
       </c>
       <c r="H54" t="n">
         <v>3.382715588569269</v>
@@ -1970,7 +1970,7 @@
         <v>1</v>
       </c>
       <c r="G55" t="n">
-        <v>1</v>
+        <v>10.43172264099121</v>
       </c>
       <c r="H55" t="n">
         <v>4.914819975131787</v>
@@ -1999,7 +1999,7 @@
         <v>2</v>
       </c>
       <c r="G56" t="n">
-        <v>2</v>
+        <v>26.3037223815918</v>
       </c>
       <c r="H56" t="n">
         <v>5.830471954825193</v>
@@ -2028,7 +2028,7 @@
         <v>2</v>
       </c>
       <c r="G57" t="n">
-        <v>2</v>
+        <v>33.74346923828125</v>
       </c>
       <c r="H57" t="n">
         <v>6.900976133077612</v>
@@ -2057,7 +2057,7 @@
         <v>10</v>
       </c>
       <c r="G58" t="n">
-        <v>10</v>
+        <v>35.59517669677734</v>
       </c>
       <c r="H58" t="n">
         <v>9.132551350533355</v>
@@ -2086,7 +2086,7 @@
         <v>10</v>
       </c>
       <c r="G59" t="n">
-        <v>10</v>
+        <v>28.48172950744629</v>
       </c>
       <c r="H59" t="n">
         <v>4.209557902844931</v>
@@ -2115,7 +2115,7 @@
         <v>10</v>
       </c>
       <c r="G60" t="n">
-        <v>10</v>
+        <v>17.22710037231445</v>
       </c>
       <c r="H60" t="n">
         <v>2.793610518686659</v>
@@ -2144,7 +2144,7 @@
         <v>10</v>
       </c>
       <c r="G61" t="n">
-        <v>10</v>
+        <v>11.27962303161621</v>
       </c>
       <c r="H61" t="n">
         <v>2.035428069511566</v>
@@ -2173,7 +2173,7 @@
         <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>0</v>
+        <v>10.32647228240967</v>
       </c>
       <c r="H62" t="n">
         <v>1.692481677039882</v>
@@ -2202,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="n">
-        <v>0</v>
+        <v>10.86010265350342</v>
       </c>
       <c r="H63" t="n">
         <v>1.704087220363075</v>
@@ -2231,7 +2231,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>0</v>
+        <v>17.46512985229492</v>
       </c>
       <c r="H64" t="n">
         <v>1.971541038015586</v>
@@ -2260,7 +2260,7 @@
         <v>0</v>
       </c>
       <c r="G65" t="n">
-        <v>0</v>
+        <v>27.29384613037109</v>
       </c>
       <c r="H65" t="n">
         <v>1.980543492902473</v>
@@ -2289,7 +2289,7 @@
         <v>1</v>
       </c>
       <c r="G66" t="n">
-        <v>1</v>
+        <v>8.682613372802734</v>
       </c>
       <c r="H66" t="n">
         <v>1.64684452500568</v>
@@ -2318,7 +2318,7 @@
         <v>1</v>
       </c>
       <c r="G67" t="n">
-        <v>1</v>
+        <v>7.110415458679199</v>
       </c>
       <c r="H67" t="n">
         <v>1.866650756768601</v>
@@ -2347,7 +2347,7 @@
         <v>1</v>
       </c>
       <c r="G68" t="n">
-        <v>1</v>
+        <v>9.42103385925293</v>
       </c>
       <c r="H68" t="n">
         <v>2.149802235056419</v>
@@ -2376,7 +2376,7 @@
         <v>1</v>
       </c>
       <c r="G69" t="n">
-        <v>1</v>
+        <v>9.24195671081543</v>
       </c>
       <c r="H69" t="n">
         <v>2.61503014826508</v>
@@ -2405,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="G70" t="n">
-        <v>1</v>
+        <v>12.14538860321045</v>
       </c>
       <c r="H70" t="n">
         <v>2.991192034732157</v>
@@ -2434,7 +2434,7 @@
         <v>2</v>
       </c>
       <c r="G71" t="n">
-        <v>2</v>
+        <v>16.73684501647949</v>
       </c>
       <c r="H71" t="n">
         <v>3.646798496007988</v>
@@ -2463,7 +2463,7 @@
         <v>2</v>
       </c>
       <c r="G72" t="n">
-        <v>2</v>
+        <v>24.93667793273926</v>
       </c>
       <c r="H72" t="n">
         <v>4.815086387087103</v>
@@ -2492,7 +2492,7 @@
         <v>2</v>
       </c>
       <c r="G73" t="n">
-        <v>2</v>
+        <v>31.79803085327148</v>
       </c>
       <c r="H73" t="n">
         <v>7.33873355108866</v>
@@ -2521,7 +2521,7 @@
         <v>2</v>
       </c>
       <c r="G74" t="n">
-        <v>2</v>
+        <v>31.22729301452637</v>
       </c>
       <c r="H74" t="n">
         <v>12.08575316908585</v>
@@ -2550,7 +2550,7 @@
         <v>2</v>
       </c>
       <c r="G75" t="n">
-        <v>2</v>
+        <v>29.28453063964844</v>
       </c>
       <c r="H75" t="n">
         <v>15.92123509167183</v>
@@ -2579,7 +2579,7 @@
         <v>2</v>
       </c>
       <c r="G76" t="n">
-        <v>2</v>
+        <v>23.02219390869141</v>
       </c>
       <c r="H76" t="n">
         <v>25.10920781651108</v>
@@ -2608,7 +2608,7 @@
         <v>100</v>
       </c>
       <c r="G77" t="n">
-        <v>100</v>
+        <v>18.00900268554688</v>
       </c>
       <c r="H77" t="n">
         <v>31.60460890164972</v>
@@ -2637,7 +2637,7 @@
         <v>100</v>
       </c>
       <c r="G78" t="n">
-        <v>100</v>
+        <v>32.1451301574707</v>
       </c>
       <c r="H78" t="n">
         <v>17.28187586265758</v>
@@ -2666,7 +2666,7 @@
         <v>10</v>
       </c>
       <c r="G79" t="n">
-        <v>10</v>
+        <v>38.01406478881836</v>
       </c>
       <c r="H79" t="n">
         <v>5.532867134488765</v>
@@ -2695,7 +2695,7 @@
         <v>10</v>
       </c>
       <c r="G80" t="n">
-        <v>10</v>
+        <v>26.06140899658203</v>
       </c>
       <c r="H80" t="n">
         <v>3.067089080017121</v>
@@ -2724,7 +2724,7 @@
         <v>10</v>
       </c>
       <c r="G81" t="n">
-        <v>10</v>
+        <v>13.72486686706543</v>
       </c>
       <c r="H81" t="n">
         <v>2.275781391937766</v>
@@ -2753,7 +2753,7 @@
         <v>0</v>
       </c>
       <c r="G82" t="n">
-        <v>0</v>
+        <v>9.230171203613281</v>
       </c>
       <c r="H82" t="n">
         <v>1.858165995243492</v>
@@ -2782,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="G83" t="n">
-        <v>0</v>
+        <v>11.65079975128174</v>
       </c>
       <c r="H83" t="n">
         <v>2.05874314328703</v>
@@ -2811,7 +2811,7 @@
         <v>0</v>
       </c>
       <c r="G84" t="n">
-        <v>0</v>
+        <v>25.63359451293945</v>
       </c>
       <c r="H84" t="n">
         <v>2.730694052733707</v>
@@ -2840,7 +2840,7 @@
         <v>0</v>
       </c>
       <c r="G85" t="n">
-        <v>0</v>
+        <v>11.4831485748291</v>
       </c>
       <c r="H85" t="n">
         <v>3.508277880485534</v>
@@ -2869,7 +2869,7 @@
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>0</v>
+        <v>26.21999359130859</v>
       </c>
       <c r="H86" t="n">
         <v>2.436738810518287</v>
@@ -2898,7 +2898,7 @@
         <v>1</v>
       </c>
       <c r="G87" t="n">
-        <v>1</v>
+        <v>6.480991840362549</v>
       </c>
       <c r="H87" t="n">
         <v>1.940353473771524</v>
@@ -2927,7 +2927,7 @@
         <v>1</v>
       </c>
       <c r="G88" t="n">
-        <v>1</v>
+        <v>8.418967247009277</v>
       </c>
       <c r="H88" t="n">
         <v>2.21441577552405</v>
@@ -2956,7 +2956,7 @@
         <v>1</v>
       </c>
       <c r="G89" t="n">
-        <v>1</v>
+        <v>10.94586181640625</v>
       </c>
       <c r="H89" t="n">
         <v>2.579532550278769</v>
@@ -2985,7 +2985,7 @@
         <v>1</v>
       </c>
       <c r="G90" t="n">
-        <v>1</v>
+        <v>14.60520172119141</v>
       </c>
       <c r="H90" t="n">
         <v>3.195460494856385</v>
@@ -3014,7 +3014,7 @@
         <v>2</v>
       </c>
       <c r="G91" t="n">
-        <v>2</v>
+        <v>11.57136058807373</v>
       </c>
       <c r="H91" t="n">
         <v>4.003799301767846</v>
@@ -3043,7 +3043,7 @@
         <v>2</v>
       </c>
       <c r="G92" t="n">
-        <v>2</v>
+        <v>19.02062797546387</v>
       </c>
       <c r="H92" t="n">
         <v>4.621649649853573</v>
@@ -3072,7 +3072,7 @@
         <v>2</v>
       </c>
       <c r="G93" t="n">
-        <v>2</v>
+        <v>15.82343196868896</v>
       </c>
       <c r="H93" t="n">
         <v>5.120527203525829</v>
@@ -3101,7 +3101,7 @@
         <v>2</v>
       </c>
       <c r="G94" t="n">
-        <v>2</v>
+        <v>18.74197578430176</v>
       </c>
       <c r="H94" t="n">
         <v>7.157131980958146</v>
@@ -3130,7 +3130,7 @@
         <v>2</v>
       </c>
       <c r="G95" t="n">
-        <v>2</v>
+        <v>21.20492553710938</v>
       </c>
       <c r="H95" t="n">
         <v>9.756213148143731</v>
@@ -3159,7 +3159,7 @@
         <v>2</v>
       </c>
       <c r="G96" t="n">
-        <v>2</v>
+        <v>31.87858200073242</v>
       </c>
       <c r="H96" t="n">
         <v>15.95754347981189</v>
@@ -3188,7 +3188,7 @@
         <v>100</v>
       </c>
       <c r="G97" t="n">
-        <v>100</v>
+        <v>5.925567626953125</v>
       </c>
       <c r="H97" t="n">
         <v>30.47347070108647</v>
@@ -3217,7 +3217,7 @@
         <v>100</v>
       </c>
       <c r="G98" t="n">
-        <v>100</v>
+        <v>31.30948829650879</v>
       </c>
       <c r="H98" t="n">
         <v>14.01448049539119</v>
@@ -3246,7 +3246,7 @@
         <v>10</v>
       </c>
       <c r="G99" t="n">
-        <v>10</v>
+        <v>33.84295272827148</v>
       </c>
       <c r="H99" t="n">
         <v>5.52027813620713</v>
@@ -3275,7 +3275,7 @@
         <v>10</v>
       </c>
       <c r="G100" t="n">
-        <v>10</v>
+        <v>18.26095771789551</v>
       </c>
       <c r="H100" t="n">
         <v>3.390429873915228</v>
@@ -3304,7 +3304,7 @@
         <v>10</v>
       </c>
       <c r="G101" t="n">
-        <v>10</v>
+        <v>24.55984497070312</v>
       </c>
       <c r="H101" t="n">
         <v>2.90391325460475</v>
@@ -3333,7 +3333,7 @@
         <v>0</v>
       </c>
       <c r="G102" t="n">
-        <v>0</v>
+        <v>12.03707885742188</v>
       </c>
       <c r="H102" t="n">
         <v>2.189337723731022</v>
@@ -3362,7 +3362,7 @@
         <v>0</v>
       </c>
       <c r="G103" t="n">
-        <v>0</v>
+        <v>18.73078155517578</v>
       </c>
       <c r="H103" t="n">
         <v>2.464650750021215</v>
@@ -3391,7 +3391,7 @@
         <v>0</v>
       </c>
       <c r="G104" t="n">
-        <v>0</v>
+        <v>20.89732551574707</v>
       </c>
       <c r="H104" t="n">
         <v>3.224709357887811</v>
@@ -3420,7 +3420,7 @@
         <v>0</v>
       </c>
       <c r="G105" t="n">
-        <v>0</v>
+        <v>28.58622360229492</v>
       </c>
       <c r="H105" t="n">
         <v>3.344406650532939</v>
@@ -3449,7 +3449,7 @@
         <v>0</v>
       </c>
       <c r="G106" t="n">
-        <v>0</v>
+        <v>10.81885814666748</v>
       </c>
       <c r="H106" t="n">
         <v>2.250008380271464</v>
@@ -3478,7 +3478,7 @@
         <v>1</v>
       </c>
       <c r="G107" t="n">
-        <v>1</v>
+        <v>8.836811065673828</v>
       </c>
       <c r="H107" t="n">
         <v>2.130303029348465</v>
@@ -3507,7 +3507,7 @@
         <v>1</v>
       </c>
       <c r="G108" t="n">
-        <v>1</v>
+        <v>13.21036243438721</v>
       </c>
       <c r="H108" t="n">
         <v>2.36563819631443</v>
@@ -3536,7 +3536,7 @@
         <v>1</v>
       </c>
       <c r="G109" t="n">
-        <v>1</v>
+        <v>20.07839584350586</v>
       </c>
       <c r="H109" t="n">
         <v>2.984386139981755</v>
@@ -3565,7 +3565,7 @@
         <v>2</v>
       </c>
       <c r="G110" t="n">
-        <v>2</v>
+        <v>10.28408813476562</v>
       </c>
       <c r="H110" t="n">
         <v>3.398161751694496</v>
@@ -3594,7 +3594,7 @@
         <v>2</v>
       </c>
       <c r="G111" t="n">
-        <v>2</v>
+        <v>13.28550624847412</v>
       </c>
       <c r="H111" t="n">
         <v>4.022081458667099</v>
@@ -3623,7 +3623,7 @@
         <v>2</v>
       </c>
       <c r="G112" t="n">
-        <v>2</v>
+        <v>26.11128044128418</v>
       </c>
       <c r="H112" t="n">
         <v>6.074503319580139</v>
@@ -3652,7 +3652,7 @@
         <v>2</v>
       </c>
       <c r="G113" t="n">
-        <v>2</v>
+        <v>18.9914379119873</v>
       </c>
       <c r="H113" t="n">
         <v>8.020530411659378</v>
@@ -3681,7 +3681,7 @@
         <v>2</v>
       </c>
       <c r="G114" t="n">
-        <v>2</v>
+        <v>16.92643547058105</v>
       </c>
       <c r="H114" t="n">
         <v>7.38905609893065</v>
@@ -3710,7 +3710,7 @@
         <v>2</v>
       </c>
       <c r="G115" t="n">
-        <v>2</v>
+        <v>15.8863000869751</v>
       </c>
       <c r="H115" t="n">
         <v>9.008581981902688</v>
@@ -3739,7 +3739,7 @@
         <v>2</v>
       </c>
       <c r="G116" t="n">
-        <v>2</v>
+        <v>31.45519065856934</v>
       </c>
       <c r="H116" t="n">
         <v>15.24685994048192</v>
@@ -3768,7 +3768,7 @@
         <v>100</v>
       </c>
       <c r="G117" t="n">
-        <v>100</v>
+        <v>19.4771556854248</v>
       </c>
       <c r="H117" t="n">
         <v>29.71938553256001</v>
@@ -3797,7 +3797,7 @@
         <v>100</v>
       </c>
       <c r="G118" t="n">
-        <v>100</v>
+        <v>32.25318908691406</v>
       </c>
       <c r="H118" t="n">
         <v>20.45491579190448</v>
@@ -3826,7 +3826,7 @@
         <v>10</v>
       </c>
       <c r="G119" t="n">
-        <v>10</v>
+        <v>16.1079273223877</v>
       </c>
       <c r="H119" t="n">
         <v>4.209557902844931</v>
@@ -3855,7 +3855,7 @@
         <v>0</v>
       </c>
       <c r="G120" t="n">
-        <v>0</v>
+        <v>12.35540103912354</v>
       </c>
       <c r="H120" t="n">
         <v>2.651016237649828</v>
@@ -3884,7 +3884,7 @@
         <v>0</v>
       </c>
       <c r="G121" t="n">
-        <v>0</v>
+        <v>27.91389274597168</v>
       </c>
       <c r="H121" t="n">
         <v>3.730822436068817</v>
@@ -3913,7 +3913,7 @@
         <v>2</v>
       </c>
       <c r="G122" t="n">
-        <v>2</v>
+        <v>21.25241470336914</v>
       </c>
       <c r="H122" t="n">
         <v>4.590174291905306</v>
@@ -3942,7 +3942,7 @@
         <v>2</v>
       </c>
       <c r="G123" t="n">
-        <v>2</v>
+        <v>18.9649543762207</v>
       </c>
       <c r="H123" t="n">
         <v>3.067089080017121</v>
@@ -3971,7 +3971,7 @@
         <v>2</v>
       </c>
       <c r="G124" t="n">
-        <v>2</v>
+        <v>13.85651302337646</v>
       </c>
       <c r="H124" t="n">
         <v>2.626970904497728</v>
@@ -4000,7 +4000,7 @@
         <v>2</v>
       </c>
       <c r="G125" t="n">
-        <v>2</v>
+        <v>12.88548469543457</v>
       </c>
       <c r="H125" t="n">
         <v>2.78725418350556</v>
@@ -4029,7 +4029,7 @@
         <v>2</v>
       </c>
       <c r="G126" t="n">
-        <v>2</v>
+        <v>15.53585624694824</v>
       </c>
       <c r="H126" t="n">
         <v>3.173698078726824</v>
@@ -4058,7 +4058,7 @@
         <v>2</v>
       </c>
       <c r="G127" t="n">
-        <v>2</v>
+        <v>12.27764129638672</v>
       </c>
       <c r="H127" t="n">
         <v>2.991192034732157</v>
@@ -4087,7 +4087,7 @@
         <v>2</v>
       </c>
       <c r="G128" t="n">
-        <v>2</v>
+        <v>14.9858512878418</v>
       </c>
       <c r="H128" t="n">
         <v>4.257776827668183</v>
@@ -4116,7 +4116,7 @@
         <v>2</v>
       </c>
       <c r="G129" t="n">
-        <v>2</v>
+        <v>21.56575012207031</v>
       </c>
       <c r="H129" t="n">
         <v>4.685249336272087</v>
@@ -4145,7 +4145,7 @@
         <v>2</v>
       </c>
       <c r="G130" t="n">
-        <v>2</v>
+        <v>18.23919486999512</v>
       </c>
       <c r="H130" t="n">
         <v>5.132204569516401</v>
@@ -4174,7 +4174,7 @@
         <v>2</v>
       </c>
       <c r="G131" t="n">
-        <v>2</v>
+        <v>18.27926254272461</v>
       </c>
       <c r="H131" t="n">
         <v>6.59363495933794</v>
@@ -4203,7 +4203,7 @@
         <v>2</v>
       </c>
       <c r="G132" t="n">
-        <v>2</v>
+        <v>17.41238594055176</v>
       </c>
       <c r="H132" t="n">
         <v>10.51786427319245</v>
@@ -4232,7 +4232,7 @@
         <v>2</v>
       </c>
       <c r="G133" t="n">
-        <v>2</v>
+        <v>31.02445220947266</v>
       </c>
       <c r="H133" t="n">
         <v>15.03989219095908</v>
@@ -4261,7 +4261,7 @@
         <v>2</v>
       </c>
       <c r="G134" t="n">
-        <v>2</v>
+        <v>33.7211799621582</v>
       </c>
       <c r="H134" t="n">
         <v>21.8517816909397</v>
@@ -4290,7 +4290,7 @@
         <v>100</v>
       </c>
       <c r="G135" t="n">
-        <v>100</v>
+        <v>27.02102470397949</v>
       </c>
       <c r="H135" t="n">
         <v>30.47347070108647</v>
@@ -4319,7 +4319,7 @@
         <v>10</v>
       </c>
       <c r="G136" t="n">
-        <v>10</v>
+        <v>25.59041404724121</v>
       </c>
       <c r="H136" t="n">
         <v>4.277218697287138</v>
@@ -4348,7 +4348,7 @@
         <v>100</v>
       </c>
       <c r="G137" t="n">
-        <v>100</v>
+        <v>17.88567161560059</v>
       </c>
       <c r="H137" t="n">
         <v>3.359677887303711</v>
@@ -4377,7 +4377,7 @@
         <v>100</v>
       </c>
       <c r="G138" t="n">
-        <v>100</v>
+        <v>27.87400436401367</v>
       </c>
       <c r="H138" t="n">
         <v>4.497028550210074</v>
@@ -4406,7 +4406,7 @@
         <v>2</v>
       </c>
       <c r="G139" t="n">
-        <v>2</v>
+        <v>34.50461196899414</v>
       </c>
       <c r="H139" t="n">
         <v>5.951236950777927</v>
@@ -4435,7 +4435,7 @@
         <v>2</v>
       </c>
       <c r="G140" t="n">
-        <v>2</v>
+        <v>28.03367233276367</v>
       </c>
       <c r="H140" t="n">
         <v>5.085654281771596</v>
@@ -4464,7 +4464,7 @@
         <v>2</v>
       </c>
       <c r="G141" t="n">
-        <v>2</v>
+        <v>17.62350273132324</v>
       </c>
       <c r="H141" t="n">
         <v>3.246821564279982</v>
@@ -4493,7 +4493,7 @@
         <v>2</v>
       </c>
       <c r="G142" t="n">
-        <v>2</v>
+        <v>12.61090564727783</v>
       </c>
       <c r="H142" t="n">
         <v>3.137756244463604</v>
@@ -4522,7 +4522,7 @@
         <v>2</v>
       </c>
       <c r="G143" t="n">
-        <v>2</v>
+        <v>12.23912811279297</v>
       </c>
       <c r="H143" t="n">
         <v>3.931497911153397</v>
@@ -4551,7 +4551,7 @@
         <v>2</v>
       </c>
       <c r="G144" t="n">
-        <v>2</v>
+        <v>22.06994438171387</v>
       </c>
       <c r="H144" t="n">
         <v>3.67180501661647</v>
@@ -4580,7 +4580,7 @@
         <v>2</v>
       </c>
       <c r="G145" t="n">
-        <v>2</v>
+        <v>23.47432327270508</v>
       </c>
       <c r="H145" t="n">
         <v>4.296749342412553</v>
@@ -4609,7 +4609,7 @@
         <v>2</v>
       </c>
       <c r="G146" t="n">
-        <v>2</v>
+        <v>12.90439033508301</v>
       </c>
       <c r="H146" t="n">
         <v>7.173453825616434</v>
@@ -4638,7 +4638,7 @@
         <v>2</v>
       </c>
       <c r="G147" t="n">
-        <v>2</v>
+        <v>15.51296901702881</v>
       </c>
       <c r="H147" t="n">
         <v>5.897257849059788</v>
@@ -4667,7 +4667,7 @@
         <v>2</v>
       </c>
       <c r="G148" t="n">
-        <v>2</v>
+        <v>16.9848461151123</v>
       </c>
       <c r="H148" t="n">
         <v>6.59363495933794</v>
@@ -4696,7 +4696,7 @@
         <v>2</v>
       </c>
       <c r="G149" t="n">
-        <v>2</v>
+        <v>27.34391784667969</v>
       </c>
       <c r="H149" t="n">
         <v>11.26175307041645</v>
@@ -4725,7 +4725,7 @@
         <v>2</v>
       </c>
       <c r="G150" t="n">
-        <v>2</v>
+        <v>34.97518920898438</v>
       </c>
       <c r="H150" t="n">
         <v>21.16590853922112</v>
@@ -4754,7 +4754,7 @@
         <v>2</v>
       </c>
       <c r="G151" t="n">
-        <v>2</v>
+        <v>38.10102844238281</v>
       </c>
       <c r="H151" t="n">
         <v>40.41967327539025</v>
@@ -4783,7 +4783,7 @@
         <v>100</v>
       </c>
       <c r="G152" t="n">
-        <v>100</v>
+        <v>34.84735107421875</v>
       </c>
       <c r="H152" t="n">
         <v>39.06191939043615</v>
@@ -4812,7 +4812,7 @@
         <v>100</v>
       </c>
       <c r="G153" t="n">
-        <v>100</v>
+        <v>27.06534576416016</v>
       </c>
       <c r="H153" t="n">
         <v>6.684371632937881</v>
@@ -4841,7 +4841,7 @@
         <v>100</v>
       </c>
       <c r="G154" t="n">
-        <v>100</v>
+        <v>21.98090362548828</v>
       </c>
       <c r="H154" t="n">
         <v>4.199979845769421</v>
@@ -4870,7 +4870,7 @@
         <v>2</v>
       </c>
       <c r="G155" t="n">
-        <v>2</v>
+        <v>31.75117301940918</v>
       </c>
       <c r="H155" t="n">
         <v>4.84810399337989</v>
@@ -4899,7 +4899,7 @@
         <v>2</v>
       </c>
       <c r="G156" t="n">
-        <v>2</v>
+        <v>28.76050758361816</v>
       </c>
       <c r="H156" t="n">
         <v>5.3836753872296</v>
@@ -4928,7 +4928,7 @@
         <v>2</v>
       </c>
       <c r="G157" t="n">
-        <v>2</v>
+        <v>29.18349838256836</v>
       </c>
       <c r="H157" t="n">
         <v>5.764442404603849</v>
@@ -4957,7 +4957,7 @@
         <v>2</v>
       </c>
       <c r="G158" t="n">
-        <v>2</v>
+        <v>11.77961254119873</v>
       </c>
       <c r="H158" t="n">
         <v>4.05889659372358</v>
@@ -4986,7 +4986,7 @@
         <v>2</v>
       </c>
       <c r="G159" t="n">
-        <v>2</v>
+        <v>27.6462574005127</v>
       </c>
       <c r="H159" t="n">
         <v>6.91671381413957</v>
@@ -5015,7 +5015,7 @@
         <v>2</v>
       </c>
       <c r="G160" t="n">
-        <v>2</v>
+        <v>25.47490692138672</v>
       </c>
       <c r="H160" t="n">
         <v>8.205327177179342</v>
@@ -5044,7 +5044,7 @@
         <v>2</v>
       </c>
       <c r="G161" t="n">
-        <v>2</v>
+        <v>22.93010711669922</v>
       </c>
       <c r="H161" t="n">
         <v>8.186657498833034</v>
@@ -5073,7 +5073,7 @@
         <v>2</v>
       </c>
       <c r="G162" t="n">
-        <v>2</v>
+        <v>24.15179252624512</v>
       </c>
       <c r="H162" t="n">
         <v>11.52122911934112</v>
@@ -5102,7 +5102,7 @@
         <v>2</v>
       </c>
       <c r="G163" t="n">
-        <v>2</v>
+        <v>32.85651397705078</v>
       </c>
       <c r="H163" t="n">
         <v>20.13134200466594</v>
@@ -5131,7 +5131,7 @@
         <v>100</v>
       </c>
       <c r="G164" t="n">
-        <v>100</v>
+        <v>22.44145202636719</v>
       </c>
       <c r="H164" t="n">
         <v>42.11141763309691</v>
@@ -5160,7 +5160,7 @@
         <v>100</v>
       </c>
       <c r="G165" t="n">
-        <v>100</v>
+        <v>29.84837532043457</v>
       </c>
       <c r="H165" t="n">
         <v>42.0156010245766</v>
@@ -5189,7 +5189,7 @@
         <v>100</v>
       </c>
       <c r="G166" t="n">
-        <v>100</v>
+        <v>20.65412139892578</v>
       </c>
       <c r="H166" t="n">
         <v>7.839895557518359</v>
@@ -5218,7 +5218,7 @@
         <v>100</v>
       </c>
       <c r="G167" t="n">
-        <v>100</v>
+        <v>30.85379219055176</v>
       </c>
       <c r="H167" t="n">
         <v>9.19517431525299</v>
@@ -5247,7 +5247,7 @@
         <v>100</v>
       </c>
       <c r="G168" t="n">
-        <v>100</v>
+        <v>32.25296783447266</v>
       </c>
       <c r="H168" t="n">
         <v>7.059977845292225</v>
@@ -5276,7 +5276,7 @@
         <v>2</v>
       </c>
       <c r="G169" t="n">
-        <v>2</v>
+        <v>21.48335647583008</v>
       </c>
       <c r="H169" t="n">
         <v>5.408258337249224</v>
@@ -5305,7 +5305,7 @@
         <v>2</v>
       </c>
       <c r="G170" t="n">
-        <v>2</v>
+        <v>17.94122314453125</v>
       </c>
       <c r="H170" t="n">
         <v>6.401241957091944</v>
@@ -5334,7 +5334,7 @@
         <v>2</v>
       </c>
       <c r="G171" t="n">
-        <v>2</v>
+        <v>27.70295524597168</v>
       </c>
       <c r="H171" t="n">
         <v>9.958290964567235</v>
@@ -5363,7 +5363,7 @@
         <v>2</v>
       </c>
       <c r="G172" t="n">
-        <v>2</v>
+        <v>25.82162666320801</v>
       </c>
       <c r="H172" t="n">
         <v>13.82424161996467</v>
@@ -5392,7 +5392,7 @@
         <v>2</v>
       </c>
       <c r="G173" t="n">
-        <v>2</v>
+        <v>34.22890853881836</v>
       </c>
       <c r="H173" t="n">
         <v>15.10856737871425</v>
@@ -5421,7 +5421,7 @@
         <v>100</v>
       </c>
       <c r="G174" t="n">
-        <v>100</v>
+        <v>27.17200660705566</v>
       </c>
       <c r="H174" t="n">
         <v>27.25505967320341</v>
@@ -5450,7 +5450,7 @@
         <v>100</v>
       </c>
       <c r="G175" t="n">
-        <v>100</v>
+        <v>23.93754577636719</v>
       </c>
       <c r="H175" t="n">
         <v>25.28138456919253</v>
@@ -5479,7 +5479,7 @@
         <v>100</v>
       </c>
       <c r="G176" t="n">
-        <v>100</v>
+        <v>26.03770446777344</v>
       </c>
       <c r="H176" t="n">
         <v>7.965907260886808</v>
@@ -5508,7 +5508,7 @@
         <v>100</v>
       </c>
       <c r="G177" t="n">
-        <v>100</v>
+        <v>34.45971298217773</v>
       </c>
       <c r="H177" t="n">
         <v>10.4700558817256</v>
@@ -5537,7 +5537,7 @@
         <v>100</v>
       </c>
       <c r="G178" t="n">
-        <v>100</v>
+        <v>29.57437896728516</v>
       </c>
       <c r="H178" t="n">
         <v>16.93118479021815</v>
@@ -5566,7 +5566,7 @@
         <v>100</v>
       </c>
       <c r="G179" t="n">
-        <v>100</v>
+        <v>35.53939437866211</v>
       </c>
       <c r="H179" t="n">
         <v>28.26673436747747</v>
@@ -5595,7 +5595,7 @@
         <v>100</v>
       </c>
       <c r="G180" t="n">
-        <v>100</v>
+        <v>26.75092124938965</v>
       </c>
       <c r="H180" t="n">
         <v>27.75628815155564</v>

</xml_diff>

<commit_message>
import age map & fit to dd
</commit_message>
<xml_diff>
--- a/output/xyz_age_eros.xlsx
+++ b/output/xyz_age_eros.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
fixed uncertainty plot and DKW
</commit_message>
<xml_diff>
--- a/output/xyz_age_eros.xlsx
+++ b/output/xyz_age_eros.xlsx
@@ -487,10 +487,10 @@
         <v>743</v>
       </c>
       <c r="D2" t="n">
-        <v>53.13875907512156</v>
+        <v>52.96688797751993</v>
       </c>
       <c r="E2" t="n">
-        <v>15.13692204542046</v>
+        <v>15.93922967451277</v>
       </c>
       <c r="F2" t="n">
         <v>1.998671911465284</v>
@@ -513,10 +513,10 @@
         <v>668</v>
       </c>
       <c r="D3" t="n">
-        <v>51.33917753540972</v>
+        <v>51.2073599644224</v>
       </c>
       <c r="E3" t="n">
-        <v>15.19062547574475</v>
+        <v>15.9379368460668</v>
       </c>
       <c r="F3" t="n">
         <v>1.68478859178372</v>
@@ -539,10 +539,10 @@
         <v>846</v>
       </c>
       <c r="D4" t="n">
-        <v>55.58335777216294</v>
+        <v>55.21920633003464</v>
       </c>
       <c r="E4" t="n">
-        <v>15.4109071185798</v>
+        <v>15.9976841055508</v>
       </c>
       <c r="F4" t="n">
         <v>2.527187593999784</v>
@@ -565,10 +565,10 @@
         <v>710</v>
       </c>
       <c r="D5" t="n">
-        <v>52.55616382561423</v>
+        <v>52.27824588478464</v>
       </c>
       <c r="E5" t="n">
-        <v>15.30681976095904</v>
+        <v>15.87025610126818</v>
       </c>
       <c r="F5" t="n">
         <v>1.853938088092913</v>
@@ -591,10 +591,10 @@
         <v>621</v>
       </c>
       <c r="D6" t="n">
-        <v>50.37316460159224</v>
+        <v>49.4418703539938</v>
       </c>
       <c r="E6" t="n">
-        <v>15.34958347069768</v>
+        <v>15.96094146956005</v>
       </c>
       <c r="F6" t="n">
         <v>1.513732700682522</v>
@@ -617,10 +617,10 @@
         <v>580</v>
       </c>
       <c r="D7" t="n">
-        <v>49.12773779180562</v>
+        <v>48.28757918525302</v>
       </c>
       <c r="E7" t="n">
-        <v>15.50789874795723</v>
+        <v>16.06817599706452</v>
       </c>
       <c r="F7" t="n">
         <v>1.378759952770284</v>
@@ -643,10 +643,10 @@
         <v>521</v>
       </c>
       <c r="D8" t="n">
-        <v>47.39350725691181</v>
+        <v>46.67769849522361</v>
       </c>
       <c r="E8" t="n">
-        <v>15.71429221552933</v>
+        <v>16.20801998008859</v>
       </c>
       <c r="F8" t="n">
         <v>1.205371905865509</v>
@@ -669,10 +669,10 @@
         <v>451</v>
       </c>
       <c r="D9" t="n">
-        <v>45.35862681639751</v>
+        <v>44.79384639341394</v>
       </c>
       <c r="E9" t="n">
-        <v>15.95304955630589</v>
+        <v>16.36756249799924</v>
       </c>
       <c r="F9" t="n">
         <v>1.027711876465111</v>
@@ -695,10 +695,10 @@
         <v>439</v>
       </c>
       <c r="D10" t="n">
-        <v>44.78058677740614</v>
+        <v>39.00603679360908</v>
       </c>
       <c r="E10" t="n">
-        <v>16.13408075554057</v>
+        <v>18.90544612422114</v>
       </c>
       <c r="F10" t="n">
         <v>1</v>
@@ -721,10 +721,10 @@
         <v>951</v>
       </c>
       <c r="D11" t="n">
-        <v>57.94564637402463</v>
+        <v>57.55770363118855</v>
       </c>
       <c r="E11" t="n">
-        <v>15.4829993188284</v>
+        <v>16.07070271705969</v>
       </c>
       <c r="F11" t="n">
         <v>3.210051613373873</v>
@@ -747,10 +747,10 @@
         <v>833</v>
       </c>
       <c r="D12" t="n">
-        <v>55.50252049728901</v>
+        <v>55.16416487159408</v>
       </c>
       <c r="E12" t="n">
-        <v>15.29323247530046</v>
+        <v>15.87858910982343</v>
       </c>
       <c r="F12" t="n">
         <v>2.453447811399311</v>
@@ -773,10 +773,10 @@
         <v>745</v>
       </c>
       <c r="D13" t="n">
-        <v>53.54642720343175</v>
+        <v>53.2516488277639</v>
       </c>
       <c r="E13" t="n">
-        <v>15.21516557420823</v>
+        <v>15.78343648648462</v>
       </c>
       <c r="F13" t="n">
         <v>2.007798251404302</v>
@@ -799,10 +799,10 @@
         <v>661</v>
       </c>
       <c r="D14" t="n">
-        <v>51.54788751374663</v>
+        <v>52.22909871041455</v>
       </c>
       <c r="E14" t="n">
-        <v>15.21050503123888</v>
+        <v>14.82180029500126</v>
       </c>
       <c r="F14" t="n">
         <v>1.658137129079801</v>
@@ -825,10 +825,10 @@
         <v>609</v>
       </c>
       <c r="D15" t="n">
-        <v>50.09954290413283</v>
+        <v>50.01122571737842</v>
       </c>
       <c r="E15" t="n">
-        <v>15.32466924561344</v>
+        <v>15.1645948259662</v>
       </c>
       <c r="F15" t="n">
         <v>1.472915449696967</v>
@@ -851,10 +851,10 @@
         <v>564</v>
       </c>
       <c r="D16" t="n">
-        <v>48.67222256376474</v>
+        <v>48.59673852777667</v>
       </c>
       <c r="E16" t="n">
-        <v>15.53392572369885</v>
+        <v>15.40748418896036</v>
       </c>
       <c r="F16" t="n">
         <v>1.329413730615203</v>
@@ -877,10 +877,10 @@
         <v>515</v>
       </c>
       <c r="D17" t="n">
-        <v>47.00434176567772</v>
+        <v>46.94593616958677</v>
       </c>
       <c r="E17" t="n">
-        <v>15.84772786032831</v>
+        <v>15.75878248043548</v>
       </c>
       <c r="F17" t="n">
         <v>1.189009644280574</v>
@@ -903,10 +903,10 @@
         <v>455</v>
       </c>
       <c r="D18" t="n">
-        <v>44.95267801520868</v>
+        <v>44.91880595932351</v>
       </c>
       <c r="E18" t="n">
-        <v>16.25480371507412</v>
+        <v>16.20803090641053</v>
       </c>
       <c r="F18" t="n">
         <v>1.037118784783609</v>
@@ -929,10 +929,10 @@
         <v>478</v>
       </c>
       <c r="D19" t="n">
-        <v>45.02824279950538</v>
+        <v>44.9945615887159</v>
       </c>
       <c r="E19" t="n">
-        <v>16.5560217881844</v>
+        <v>16.51259435699411</v>
       </c>
       <c r="F19" t="n">
         <v>1.092903885367194</v>
@@ -955,10 +955,10 @@
         <v>540</v>
       </c>
       <c r="D20" t="n">
-        <v>46.56015586597096</v>
+        <v>45.09856829781084</v>
       </c>
       <c r="E20" t="n">
-        <v>16.50410778302064</v>
+        <v>17.34149667501764</v>
       </c>
       <c r="F20" t="n">
         <v>1.258686021980649</v>
@@ -981,10 +981,10 @@
         <v>1317</v>
       </c>
       <c r="D21" t="n">
-        <v>65.45731192138825</v>
+        <v>64.48431215475523</v>
       </c>
       <c r="E21" t="n">
-        <v>16.19161521508609</v>
+        <v>16.81764425099239</v>
       </c>
       <c r="F21" t="n">
         <v>7.38905609893065</v>
@@ -1007,10 +1007,10 @@
         <v>1125</v>
       </c>
       <c r="D22" t="n">
-        <v>61.38077193970329</v>
+        <v>60.94471470246624</v>
       </c>
       <c r="E22" t="n">
-        <v>15.83235823671549</v>
+        <v>16.38815175436252</v>
       </c>
       <c r="F22" t="n">
         <v>4.771412434928934</v>
@@ -1033,10 +1033,10 @@
         <v>960</v>
       </c>
       <c r="D23" t="n">
-        <v>58.18329951451685</v>
+        <v>58.83338921004744</v>
       </c>
       <c r="E23" t="n">
-        <v>15.4670588908404</v>
+        <v>14.96375408163327</v>
       </c>
       <c r="F23" t="n">
         <v>3.276540548249262</v>
@@ -1059,10 +1059,10 @@
         <v>840</v>
       </c>
       <c r="D24" t="n">
-        <v>55.7266214930758</v>
+        <v>56.41144962448659</v>
       </c>
       <c r="E24" t="n">
-        <v>15.25543711943466</v>
+        <v>14.7741132110974</v>
       </c>
       <c r="F24" t="n">
         <v>2.492882410441073</v>
@@ -1085,10 +1085,10 @@
         <v>837</v>
       </c>
       <c r="D25" t="n">
-        <v>55.52789164595391</v>
+        <v>56.16727136753231</v>
       </c>
       <c r="E25" t="n">
-        <v>15.30555424381732</v>
+        <v>14.85075880820212</v>
       </c>
       <c r="F25" t="n">
         <v>2.475904843525316</v>
@@ -1111,10 +1111,10 @@
         <v>707</v>
       </c>
       <c r="D26" t="n">
-        <v>52.61303219477722</v>
+        <v>52.51291117747516</v>
       </c>
       <c r="E26" t="n">
-        <v>15.19973345986776</v>
+        <v>14.9937841406699</v>
       </c>
       <c r="F26" t="n">
         <v>1.841311997982751</v>
@@ -1137,10 +1137,10 @@
         <v>628</v>
       </c>
       <c r="D27" t="n">
-        <v>50.58144052153657</v>
+        <v>50.49650209631368</v>
       </c>
       <c r="E27" t="n">
-        <v>15.27412107861117</v>
+        <v>15.10958751764614</v>
       </c>
       <c r="F27" t="n">
         <v>1.53806313144631</v>
@@ -1163,10 +1163,10 @@
         <v>634</v>
       </c>
       <c r="D28" t="n">
-        <v>50.27670309600741</v>
+        <v>50.19355690630694</v>
       </c>
       <c r="E28" t="n">
-        <v>15.524477649049</v>
+        <v>15.37670764693945</v>
       </c>
       <c r="F28" t="n">
         <v>1.55922880609994</v>
@@ -1189,10 +1189,10 @@
         <v>546</v>
       </c>
       <c r="D29" t="n">
-        <v>47.59744311433016</v>
+        <v>47.53887465734004</v>
       </c>
       <c r="E29" t="n">
-        <v>15.89982377414274</v>
+        <v>15.8076054676225</v>
       </c>
       <c r="F29" t="n">
         <v>1.276007117771601</v>
@@ -1215,10 +1215,10 @@
         <v>470</v>
       </c>
       <c r="D30" t="n">
-        <v>44.82091871716457</v>
+        <v>44.79352267694455</v>
       </c>
       <c r="E30" t="n">
-        <v>16.54680402146714</v>
+        <v>16.51015314310043</v>
       </c>
       <c r="F30" t="n">
         <v>1.073168013320587</v>
@@ -1241,10 +1241,10 @@
         <v>495</v>
       </c>
       <c r="D31" t="n">
-        <v>44.60551466613327</v>
+        <v>44.42829251746996</v>
       </c>
       <c r="E31" t="n">
-        <v>17.39865530253426</v>
+        <v>17.16869656110757</v>
       </c>
       <c r="F31" t="n">
         <v>1.136056031253367</v>
@@ -1267,10 +1267,10 @@
         <v>571</v>
       </c>
       <c r="D32" t="n">
-        <v>46.72768929221765</v>
+        <v>46.53070163393627</v>
       </c>
       <c r="E32" t="n">
-        <v>17.56614676833322</v>
+        <v>16.90435802571212</v>
       </c>
       <c r="F32" t="n">
         <v>1.350781577603365</v>
@@ -1293,10 +1293,10 @@
         <v>688</v>
       </c>
       <c r="D33" t="n">
-        <v>50.53137541865671</v>
+        <v>53.36612482296577</v>
       </c>
       <c r="E33" t="n">
-        <v>17.61575928925073</v>
+        <v>14.13985269648476</v>
       </c>
       <c r="F33" t="n">
         <v>1.763319615489954</v>
@@ -1319,10 +1319,10 @@
         <v>649</v>
       </c>
       <c r="D34" t="n">
-        <v>50.07783711934053</v>
+        <v>51.03795739079624</v>
       </c>
       <c r="E34" t="n">
-        <v>17.28291950960114</v>
+        <v>15.03773801721659</v>
       </c>
       <c r="F34" t="n">
         <v>1.613426065273356</v>
@@ -1345,10 +1345,10 @@
         <v>1518</v>
       </c>
       <c r="D35" t="n">
-        <v>68.85758640242247</v>
+        <v>68.06174947032062</v>
       </c>
       <c r="E35" t="n">
-        <v>16.8054087166531</v>
+        <v>17.29773123021684</v>
       </c>
       <c r="F35" t="n">
         <v>11.6797756589234</v>
@@ -1371,10 +1371,10 @@
         <v>1321</v>
       </c>
       <c r="D36" t="n">
-        <v>65.01081586121543</v>
+        <v>65.4520968327772</v>
       </c>
       <c r="E36" t="n">
-        <v>16.33155818760662</v>
+        <v>15.86574978136692</v>
       </c>
       <c r="F36" t="n">
         <v>7.456690009635234</v>
@@ -1397,10 +1397,10 @@
         <v>1124</v>
       </c>
       <c r="D37" t="n">
-        <v>61.39775191144487</v>
+        <v>61.96696808056258</v>
       </c>
       <c r="E37" t="n">
-        <v>15.81105054236804</v>
+        <v>15.30888898265873</v>
       </c>
       <c r="F37" t="n">
         <v>4.760555983565796</v>
@@ -1423,10 +1423,10 @@
         <v>1025</v>
       </c>
       <c r="D38" t="n">
-        <v>59.51428242056595</v>
+        <v>60.12424626581462</v>
       </c>
       <c r="E38" t="n">
-        <v>15.5714354325175</v>
+        <v>15.06667989256673</v>
       </c>
       <c r="F38" t="n">
         <v>3.799433346301817</v>
@@ -1449,10 +1449,10 @@
         <v>967</v>
       </c>
       <c r="D39" t="n">
-        <v>58.34698051313333</v>
+        <v>58.95920024984652</v>
       </c>
       <c r="E39" t="n">
-        <v>15.45185073690532</v>
+        <v>14.95859116987356</v>
       </c>
       <c r="F39" t="n">
         <v>3.329204828354976</v>
@@ -1475,10 +1475,10 @@
         <v>840</v>
       </c>
       <c r="D40" t="n">
-        <v>55.71276845103699</v>
+        <v>56.35105592666811</v>
       </c>
       <c r="E40" t="n">
-        <v>15.23225183295919</v>
+        <v>14.76862149981654</v>
       </c>
       <c r="F40" t="n">
         <v>2.492882410441073</v>
@@ -1501,10 +1501,10 @@
         <v>721</v>
       </c>
       <c r="D41" t="n">
-        <v>53.05862101459471</v>
+        <v>52.96525740932015</v>
       </c>
       <c r="E41" t="n">
-        <v>15.10940245865141</v>
+        <v>14.89566264633304</v>
       </c>
       <c r="F41" t="n">
         <v>1.900979007363115</v>
@@ -1527,10 +1527,10 @@
         <v>697</v>
       </c>
       <c r="D42" t="n">
-        <v>52.25445889704619</v>
+        <v>52.16732434209097</v>
       </c>
       <c r="E42" t="n">
-        <v>15.20708285966382</v>
+        <v>15.01666135263009</v>
       </c>
       <c r="F42" t="n">
         <v>1.799842779974398</v>
@@ -1553,10 +1553,10 @@
         <v>657</v>
       </c>
       <c r="D43" t="n">
-        <v>50.67314284265827</v>
+        <v>50.88818125310431</v>
       </c>
       <c r="E43" t="n">
-        <v>15.85462186233381</v>
+        <v>15.2230883955334</v>
       </c>
       <c r="F43" t="n">
         <v>1.643097440105306</v>
@@ -1579,10 +1579,10 @@
         <v>574</v>
       </c>
       <c r="D44" t="n">
-        <v>48.25155653076515</v>
+        <v>48.34823216465421</v>
       </c>
       <c r="E44" t="n">
-        <v>15.99215364051541</v>
+        <v>15.64364953241959</v>
       </c>
       <c r="F44" t="n">
         <v>1.360044043680082</v>
@@ -1605,10 +1605,10 @@
         <v>500</v>
       </c>
       <c r="D45" t="n">
-        <v>45.73073215448035</v>
+        <v>45.50625741464484</v>
       </c>
       <c r="E45" t="n">
-        <v>16.80004562629041</v>
+        <v>16.45467886818331</v>
       </c>
       <c r="F45" t="n">
         <v>1.149069131828367</v>
@@ -1631,10 +1631,10 @@
         <v>489</v>
       </c>
       <c r="D46" t="n">
-        <v>43.69129307474174</v>
+        <v>43.592069715692</v>
       </c>
       <c r="E46" t="n">
-        <v>17.72006772515826</v>
+        <v>17.65425572905108</v>
       </c>
       <c r="F46" t="n">
         <v>1.120634694595313</v>
@@ -1657,10 +1657,10 @@
         <v>532</v>
       </c>
       <c r="D47" t="n">
-        <v>45.1682110052599</v>
+        <v>45.03357064187347</v>
       </c>
       <c r="E47" t="n">
-        <v>17.6731739884876</v>
+        <v>17.32731207236272</v>
       </c>
       <c r="F47" t="n">
         <v>1.235956423697341</v>
@@ -1683,10 +1683,10 @@
         <v>572</v>
       </c>
       <c r="D48" t="n">
-        <v>47.5149024236696</v>
+        <v>46.88292074343352</v>
       </c>
       <c r="E48" t="n">
-        <v>17.16509834993037</v>
+        <v>16.63178964823992</v>
       </c>
       <c r="F48" t="n">
         <v>1.353862035967913</v>
@@ -1709,10 +1709,10 @@
         <v>665</v>
       </c>
       <c r="D49" t="n">
-        <v>50.51880571190345</v>
+        <v>51.92925188305506</v>
       </c>
       <c r="E49" t="n">
-        <v>17.26972673555958</v>
+        <v>14.68607857091653</v>
       </c>
       <c r="F49" t="n">
         <v>1.673314480154503</v>
@@ -1735,10 +1735,10 @@
         <v>762</v>
       </c>
       <c r="D50" t="n">
-        <v>53.16341146190675</v>
+        <v>57.00588805143471</v>
       </c>
       <c r="E50" t="n">
-        <v>17.67304196326178</v>
+        <v>12.78618108613156</v>
       </c>
       <c r="F50" t="n">
         <v>2.087074026899868</v>
@@ -1761,10 +1761,10 @@
         <v>748</v>
       </c>
       <c r="D51" t="n">
-        <v>52.66397012040657</v>
+        <v>55.94981387317615</v>
       </c>
       <c r="E51" t="n">
-        <v>17.30184487467596</v>
+        <v>13.20130520331678</v>
       </c>
       <c r="F51" t="n">
         <v>2.021565957079946</v>
@@ -1787,10 +1787,10 @@
         <v>699</v>
       </c>
       <c r="D52" t="n">
-        <v>51.79770799697043</v>
+        <v>53.23683989023291</v>
       </c>
       <c r="E52" t="n">
-        <v>17.12535461915485</v>
+        <v>17.04148006784176</v>
       </c>
       <c r="F52" t="n">
         <v>1.808061225909724</v>
@@ -1813,10 +1813,10 @@
         <v>729</v>
       </c>
       <c r="D53" t="n">
-        <v>52.24310735067523</v>
+        <v>54.6464565822418</v>
       </c>
       <c r="E53" t="n">
-        <v>17.03036624291041</v>
+        <v>19.47030497912526</v>
       </c>
       <c r="F53" t="n">
         <v>1.935938564475256</v>
@@ -1839,10 +1839,10 @@
         <v>1619</v>
       </c>
       <c r="D54" t="n">
-        <v>70.46523367168191</v>
+        <v>70.4331583858345</v>
       </c>
       <c r="E54" t="n">
-        <v>17.15124380259039</v>
+        <v>16.85905961878461</v>
       </c>
       <c r="F54" t="n">
         <v>14.7011703617567</v>
@@ -1865,10 +1865,10 @@
         <v>1494</v>
       </c>
       <c r="D55" t="n">
-        <v>68.09573181633968</v>
+        <v>68.40387306665642</v>
       </c>
       <c r="E55" t="n">
-        <v>16.81873508913862</v>
+        <v>16.41000935898461</v>
       </c>
       <c r="F55" t="n">
         <v>11.05838613157211</v>
@@ -1891,10 +1891,10 @@
         <v>1269</v>
       </c>
       <c r="D56" t="n">
-        <v>64.11195721765083</v>
+        <v>64.58225391995111</v>
       </c>
       <c r="E56" t="n">
-        <v>16.16752282156941</v>
+        <v>15.69059194255127</v>
       </c>
       <c r="F56" t="n">
         <v>6.62374282933277</v>
@@ -1917,10 +1917,10 @@
         <v>1082</v>
       </c>
       <c r="D57" t="n">
-        <v>60.68059979022981</v>
+        <v>61.30832863754874</v>
       </c>
       <c r="E57" t="n">
-        <v>15.66622237704206</v>
+        <v>15.50879953808567</v>
       </c>
       <c r="F57" t="n">
         <v>4.326212651421302</v>
@@ -1943,10 +1943,10 @@
         <v>941</v>
       </c>
       <c r="D58" t="n">
-        <v>57.96232615818173</v>
+        <v>58.64760157711963</v>
       </c>
       <c r="E58" t="n">
-        <v>15.33076710866459</v>
+        <v>15.15939721731263</v>
       </c>
       <c r="F58" t="n">
         <v>3.137756244463604</v>
@@ -1995,10 +1995,10 @@
         <v>760</v>
       </c>
       <c r="D60" t="n">
-        <v>53.64662651447308</v>
+        <v>54.08232956698572</v>
       </c>
       <c r="E60" t="n">
-        <v>15.73554247636985</v>
+        <v>15.02789179340761</v>
       </c>
       <c r="F60" t="n">
         <v>2.07758734314862</v>
@@ -2021,10 +2021,10 @@
         <v>711</v>
       </c>
       <c r="D61" t="n">
-        <v>52.437230302308</v>
+        <v>52.80517028752742</v>
       </c>
       <c r="E61" t="n">
-        <v>15.62124315912084</v>
+        <v>15.02732540511957</v>
       </c>
       <c r="F61" t="n">
         <v>1.858165995243492</v>
@@ -2047,10 +2047,10 @@
         <v>632</v>
       </c>
       <c r="D62" t="n">
-        <v>50.47577894350595</v>
+        <v>50.71923765994121</v>
       </c>
       <c r="E62" t="n">
-        <v>15.47007829512614</v>
+        <v>15.07989790598648</v>
       </c>
       <c r="F62" t="n">
         <v>1.552141414666451</v>
@@ -2255,10 +2255,10 @@
         <v>620</v>
       </c>
       <c r="D70" t="n">
-        <v>50.04913953975233</v>
+        <v>49.00131633929187</v>
       </c>
       <c r="E70" t="n">
-        <v>16.64416455948383</v>
+        <v>16.17512778026231</v>
       </c>
       <c r="F70" t="n">
         <v>1.510288486696439</v>
@@ -2281,10 +2281,10 @@
         <v>654</v>
       </c>
       <c r="D71" t="n">
-        <v>50.79420185729079</v>
+        <v>50.59826880399702</v>
       </c>
       <c r="E71" t="n">
-        <v>16.78156001252828</v>
+        <v>16.42213532531829</v>
       </c>
       <c r="F71" t="n">
         <v>1.631907262573603</v>
@@ -2307,10 +2307,10 @@
         <v>737</v>
       </c>
       <c r="D72" t="n">
-        <v>52.36741253301098</v>
+        <v>54.91898385516136</v>
       </c>
       <c r="E72" t="n">
-        <v>17.03735259531071</v>
+        <v>17.50350642228256</v>
       </c>
       <c r="F72" t="n">
         <v>1.971541038015586</v>
@@ -2333,10 +2333,10 @@
         <v>799</v>
       </c>
       <c r="D73" t="n">
-        <v>53.44040668933646</v>
+        <v>58.16209359664636</v>
       </c>
       <c r="E73" t="n">
-        <v>17.41998285975104</v>
+        <v>18.58565787143118</v>
       </c>
       <c r="F73" t="n">
         <v>2.270603279516831</v>
@@ -2359,10 +2359,10 @@
         <v>778</v>
       </c>
       <c r="D74" t="n">
-        <v>53.1624398040619</v>
+        <v>53.09469706251218</v>
       </c>
       <c r="E74" t="n">
-        <v>17.31707181823908</v>
+        <v>17.91053832422441</v>
       </c>
       <c r="F74" t="n">
         <v>2.164543678531826</v>
@@ -2385,10 +2385,10 @@
         <v>1807</v>
       </c>
       <c r="D75" t="n">
-        <v>73.33982340909634</v>
+        <v>73.32147548564562</v>
       </c>
       <c r="E75" t="n">
-        <v>17.84108501086984</v>
+        <v>17.62538571575201</v>
       </c>
       <c r="F75" t="n">
         <v>22.55988029919262</v>
@@ -2411,10 +2411,10 @@
         <v>1635</v>
       </c>
       <c r="D76" t="n">
-        <v>70.60336185276886</v>
+        <v>70.57904148609464</v>
       </c>
       <c r="E76" t="n">
-        <v>17.249978249968</v>
+        <v>16.98651220505798</v>
       </c>
       <c r="F76" t="n">
         <v>15.24685994048192</v>
@@ -2437,10 +2437,10 @@
         <v>1415</v>
       </c>
       <c r="D77" t="n">
-        <v>66.64071238100071</v>
+        <v>67.04770791755624</v>
       </c>
       <c r="E77" t="n">
-        <v>16.6140405025294</v>
+        <v>16.51011507872386</v>
       </c>
       <c r="F77" t="n">
         <v>9.237161339795705</v>
@@ -2463,10 +2463,10 @@
         <v>1270</v>
       </c>
       <c r="D78" t="n">
-        <v>64.15299006991958</v>
+        <v>64.66528987290629</v>
       </c>
       <c r="E78" t="n">
-        <v>16.1606998109956</v>
+        <v>16.02981196846014</v>
       </c>
       <c r="F78" t="n">
         <v>6.63884827964505</v>
@@ -2489,10 +2489,10 @@
         <v>1102</v>
       </c>
       <c r="D79" t="n">
-        <v>61.14954791665618</v>
+        <v>61.76593496065291</v>
       </c>
       <c r="E79" t="n">
-        <v>15.67502949092539</v>
+        <v>15.51727909188376</v>
       </c>
       <c r="F79" t="n">
         <v>4.527865196995156</v>
@@ -2515,10 +2515,10 @@
         <v>1001</v>
       </c>
       <c r="D80" t="n">
-        <v>59.26737358699999</v>
+        <v>59.92203879271286</v>
       </c>
       <c r="E80" t="n">
-        <v>15.39930126387338</v>
+        <v>15.23112939420251</v>
       </c>
       <c r="F80" t="n">
         <v>3.59729520938842</v>
@@ -2541,10 +2541,10 @@
         <v>849</v>
       </c>
       <c r="D81" t="n">
-        <v>55.73819267232751</v>
+        <v>56.26477812732728</v>
       </c>
       <c r="E81" t="n">
-        <v>15.89641842001553</v>
+        <v>15.04248567793664</v>
       </c>
       <c r="F81" t="n">
         <v>2.544516812688459</v>
@@ -2567,10 +2567,10 @@
         <v>723</v>
       </c>
       <c r="D82" t="n">
-        <v>53.18835803994816</v>
+        <v>53.57816217769724</v>
       </c>
       <c r="E82" t="n">
-        <v>15.42373201544989</v>
+        <v>14.79685652943536</v>
       </c>
       <c r="F82" t="n">
         <v>1.90965926175535</v>
@@ -2905,10 +2905,10 @@
         <v>763</v>
       </c>
       <c r="D95" t="n">
-        <v>52.68805601395244</v>
+        <v>53.41199634497387</v>
       </c>
       <c r="E95" t="n">
-        <v>17.18541674620386</v>
+        <v>16.83356579395518</v>
       </c>
       <c r="F95" t="n">
         <v>2.09183360072749</v>
@@ -2931,10 +2931,10 @@
         <v>829</v>
       </c>
       <c r="D96" t="n">
-        <v>53.46244903244137</v>
+        <v>54.95136488044788</v>
       </c>
       <c r="E96" t="n">
-        <v>17.55382368487939</v>
+        <v>17.08215489431978</v>
       </c>
       <c r="F96" t="n">
         <v>2.431194469771844</v>
@@ -2957,10 +2957,10 @@
         <v>813</v>
       </c>
       <c r="D97" t="n">
-        <v>53.44718860892447</v>
+        <v>53.69773831040796</v>
       </c>
       <c r="E97" t="n">
-        <v>17.57708350190898</v>
+        <v>18.14471873466844</v>
       </c>
       <c r="F97" t="n">
         <v>2.344181308295465</v>
@@ -2983,10 +2983,10 @@
         <v>954</v>
       </c>
       <c r="D98" t="n">
-        <v>54.62085170602591</v>
+        <v>52.34994289682481</v>
       </c>
       <c r="E98" t="n">
-        <v>18.15281579051012</v>
+        <v>19.34949150269448</v>
       </c>
       <c r="F98" t="n">
         <v>3.232063309910436</v>
@@ -3009,10 +3009,10 @@
         <v>1693</v>
       </c>
       <c r="D99" t="n">
-        <v>71.31868988240132</v>
+        <v>71.30429570468623</v>
       </c>
       <c r="E99" t="n">
-        <v>17.52738445377278</v>
+        <v>17.32356033368554</v>
       </c>
       <c r="F99" t="n">
         <v>17.40037969153265</v>
@@ -3061,10 +3061,10 @@
         <v>1407</v>
       </c>
       <c r="D101" t="n">
-        <v>66.47356020976828</v>
+        <v>66.88623337443184</v>
       </c>
       <c r="E101" t="n">
-        <v>16.6015712668771</v>
+        <v>16.4949083909736</v>
       </c>
       <c r="F101" t="n">
         <v>9.070354874271228</v>
@@ -3087,10 +3087,10 @@
         <v>1169</v>
       </c>
       <c r="D102" t="n">
-        <v>62.40584091660743</v>
+        <v>62.99778381628343</v>
       </c>
       <c r="E102" t="n">
-        <v>15.8530295505104</v>
+        <v>15.69955799184115</v>
       </c>
       <c r="F102" t="n">
         <v>5.274427588540518</v>
@@ -3113,10 +3113,10 @@
         <v>1073</v>
       </c>
       <c r="D103" t="n">
-        <v>60.10059254958384</v>
+        <v>61.38159126568696</v>
       </c>
       <c r="E103" t="n">
-        <v>16.59469361473083</v>
+        <v>15.38242297355965</v>
       </c>
       <c r="F103" t="n">
         <v>4.238423330031359</v>
@@ -3139,10 +3139,10 @@
         <v>1003</v>
       </c>
       <c r="D104" t="n">
-        <v>58.84400823816925</v>
+        <v>60.14080143010804</v>
       </c>
       <c r="E104" t="n">
-        <v>16.36161213389667</v>
+        <v>15.15909321333115</v>
       </c>
       <c r="F104" t="n">
         <v>3.613721186435255</v>
@@ -3607,10 +3607,10 @@
         <v>904</v>
       </c>
       <c r="D122" t="n">
-        <v>54.19412086480123</v>
+        <v>54.43409119853735</v>
       </c>
       <c r="E122" t="n">
-        <v>17.97616817139494</v>
+        <v>17.83686467088651</v>
       </c>
       <c r="F122" t="n">
         <v>2.884136396542327</v>
@@ -3633,10 +3633,10 @@
         <v>893</v>
       </c>
       <c r="D123" t="n">
-        <v>54.35351379999352</v>
+        <v>53.19819285544828</v>
       </c>
       <c r="E123" t="n">
-        <v>18.03215568271352</v>
+        <v>18.15625174007817</v>
       </c>
       <c r="F123" t="n">
         <v>2.812766630296358</v>
@@ -3659,10 +3659,10 @@
         <v>975</v>
       </c>
       <c r="D124" t="n">
-        <v>54.75199808062919</v>
+        <v>53.87878134348747</v>
       </c>
       <c r="E124" t="n">
-        <v>18.26505153548855</v>
+        <v>18.40539662813776</v>
       </c>
       <c r="F124" t="n">
         <v>3.390429873915228</v>
@@ -3685,10 +3685,10 @@
         <v>1098</v>
       </c>
       <c r="D125" t="n">
-        <v>55.55071048011287</v>
+        <v>53.8731916107245</v>
       </c>
       <c r="E125" t="n">
-        <v>18.51257762582823</v>
+        <v>18.83865097270531</v>
       </c>
       <c r="F125" t="n">
         <v>4.486796407757537</v>
@@ -3763,10 +3763,10 @@
         <v>1341</v>
       </c>
       <c r="D128" t="n">
-        <v>65.35090014346956</v>
+        <v>65.82117846118918</v>
       </c>
       <c r="E128" t="n">
-        <v>16.39569824870074</v>
+        <v>16.27278677419877</v>
       </c>
       <c r="F128" t="n">
         <v>7.804259730116742</v>
@@ -3789,10 +3789,10 @@
         <v>1210</v>
       </c>
       <c r="D129" t="n">
-        <v>62.5915322508244</v>
+        <v>63.78385132408877</v>
       </c>
       <c r="E129" t="n">
-        <v>16.97030662786552</v>
+        <v>15.79360505016361</v>
       </c>
       <c r="F129" t="n">
         <v>5.79076401378919</v>
@@ -4387,10 +4387,10 @@
         <v>1053</v>
       </c>
       <c r="D152" t="n">
-        <v>55.40780035932431</v>
+        <v>53.66052845410002</v>
       </c>
       <c r="E152" t="n">
-        <v>18.53885667638646</v>
+        <v>18.90971932923981</v>
       </c>
       <c r="F152" t="n">
         <v>4.049661338113483</v>
@@ -4413,10 +4413,10 @@
         <v>1067</v>
       </c>
       <c r="D153" t="n">
-        <v>55.61236740332908</v>
+        <v>53.81973513676296</v>
       </c>
       <c r="E153" t="n">
-        <v>18.57620386970508</v>
+        <v>19.6647344240363</v>
       </c>
       <c r="F153" t="n">
         <v>4.180889061233321</v>
@@ -4439,10 +4439,10 @@
         <v>1067</v>
       </c>
       <c r="D154" t="n">
-        <v>55.08635151477228</v>
+        <v>55.37158396298174</v>
       </c>
       <c r="E154" t="n">
-        <v>19.26268358030456</v>
+        <v>20.11446192305701</v>
       </c>
       <c r="F154" t="n">
         <v>4.180889061233321</v>
@@ -4491,10 +4491,10 @@
         <v>1519</v>
       </c>
       <c r="D156" t="n">
-        <v>68.17927333571851</v>
+        <v>68.5034474401109</v>
       </c>
       <c r="E156" t="n">
-        <v>17.03085461575616</v>
+        <v>16.94565744675715</v>
       </c>
       <c r="F156" t="n">
         <v>11.70641139575985</v>
@@ -5219,10 +5219,10 @@
         <v>1169</v>
       </c>
       <c r="D184" t="n">
-        <v>55.72846402181363</v>
+        <v>56.26035260149518</v>
       </c>
       <c r="E184" t="n">
-        <v>19.31750018957257</v>
+        <v>19.87494918404688</v>
       </c>
       <c r="F184" t="n">
         <v>5.274427588540518</v>
@@ -5245,10 +5245,10 @@
         <v>1213</v>
       </c>
       <c r="D185" t="n">
-        <v>55.89196768399303</v>
+        <v>56.4240534883149</v>
       </c>
       <c r="E185" t="n">
-        <v>19.23665327511029</v>
+        <v>19.68782614239082</v>
       </c>
       <c r="F185" t="n">
         <v>5.830471954825193</v>
@@ -6077,10 +6077,10 @@
         <v>1402</v>
       </c>
       <c r="D217" t="n">
-        <v>56.66567078984173</v>
+        <v>56.8093417150188</v>
       </c>
       <c r="E217" t="n">
-        <v>19.76320387764649</v>
+        <v>19.01885096776954</v>
       </c>
       <c r="F217" t="n">
         <v>8.967633952648329</v>
@@ -6103,10 +6103,10 @@
         <v>1527</v>
       </c>
       <c r="D218" t="n">
-        <v>56.78775016737807</v>
+        <v>56.90067037079318</v>
       </c>
       <c r="E218" t="n">
-        <v>19.4403495481722</v>
+        <v>18.82280973723667</v>
       </c>
       <c r="F218" t="n">
         <v>11.92169570778177</v>
@@ -6129,10 +6129,10 @@
         <v>1610</v>
       </c>
       <c r="D219" t="n">
-        <v>56.9070596159795</v>
+        <v>56.6878629835572</v>
       </c>
       <c r="E219" t="n">
-        <v>18.81453100532503</v>
+        <v>18.85730439797935</v>
       </c>
       <c r="F219" t="n">
         <v>14.40284804760218</v>
@@ -6155,10 +6155,10 @@
         <v>1668</v>
       </c>
       <c r="D220" t="n">
-        <v>56.86786601506155</v>
+        <v>56.65846082204847</v>
       </c>
       <c r="E220" t="n">
-        <v>18.90774637828806</v>
+        <v>18.95571591866298</v>
       </c>
       <c r="F220" t="n">
         <v>16.43715661100289</v>
@@ -6181,10 +6181,10 @@
         <v>1674</v>
       </c>
       <c r="D221" t="n">
-        <v>56.7468217734277</v>
+        <v>56.5448552144188</v>
       </c>
       <c r="E221" t="n">
-        <v>19.07226141823139</v>
+        <v>19.12572261040065</v>
       </c>
       <c r="F221" t="n">
         <v>16.66335246860211</v>
@@ -6207,10 +6207,10 @@
         <v>1731</v>
       </c>
       <c r="D222" t="n">
-        <v>56.7893895611928</v>
+        <v>57.25113162140847</v>
       </c>
       <c r="E222" t="n">
-        <v>19.1777499750668</v>
+        <v>19.92479791859911</v>
       </c>
       <c r="F222" t="n">
         <v>18.97367309652293</v>
@@ -7143,10 +7143,10 @@
         <v>1654</v>
       </c>
       <c r="D258" t="n">
-        <v>56.48215268113484</v>
+        <v>56.28096101962942</v>
       </c>
       <c r="E258" t="n">
-        <v>19.1137758490185</v>
+        <v>19.16317305742793</v>
       </c>
       <c r="F258" t="n">
         <v>15.92123509167183</v>
@@ -7169,10 +7169,10 @@
         <v>1731</v>
       </c>
       <c r="D259" t="n">
-        <v>56.40827582554207</v>
+        <v>56.56191222309833</v>
       </c>
       <c r="E259" t="n">
-        <v>19.32147989796797</v>
+        <v>19.53187825050605</v>
       </c>
       <c r="F259" t="n">
         <v>18.97367309652293</v>
@@ -7195,10 +7195,10 @@
         <v>1854</v>
       </c>
       <c r="D260" t="n">
-        <v>56.83255773352424</v>
+        <v>56.73659176124106</v>
       </c>
       <c r="E260" t="n">
-        <v>19.346108228531</v>
+        <v>19.58582916147679</v>
       </c>
       <c r="F260" t="n">
         <v>25.10920781651108</v>
@@ -7221,10 +7221,10 @@
         <v>1935</v>
       </c>
       <c r="D261" t="n">
-        <v>57.7895698284016</v>
+        <v>57.50467880464831</v>
       </c>
       <c r="E261" t="n">
-        <v>19.16160313931762</v>
+        <v>19.11824439597797</v>
       </c>
       <c r="F261" t="n">
         <v>30.19706924231686</v>
@@ -7247,10 +7247,10 @@
         <v>1955</v>
       </c>
       <c r="D262" t="n">
-        <v>58.57516896871709</v>
+        <v>58.69566530504983</v>
       </c>
       <c r="E262" t="n">
-        <v>18.98025091351528</v>
+        <v>19.24102641041551</v>
       </c>
       <c r="F262" t="n">
         <v>31.60460890164972</v>
@@ -8209,10 +8209,10 @@
         <v>1711</v>
       </c>
       <c r="D299" t="n">
-        <v>55.27617409436274</v>
+        <v>55.39057492816686</v>
       </c>
       <c r="E299" t="n">
-        <v>19.91111763879407</v>
+        <v>20.17122987291349</v>
       </c>
       <c r="F299" t="n">
         <v>18.12866351422814</v>
@@ -8235,10 +8235,10 @@
         <v>1849</v>
       </c>
       <c r="D300" t="n">
-        <v>57.01024125740739</v>
+        <v>56.95233334106908</v>
       </c>
       <c r="E300" t="n">
-        <v>19.53046296262228</v>
+        <v>19.77523453509681</v>
       </c>
       <c r="F300" t="n">
         <v>24.82484838362393</v>
@@ -8261,10 +8261,10 @@
         <v>1942</v>
       </c>
       <c r="D301" t="n">
-        <v>59.39364958893707</v>
+        <v>59.53511734813156</v>
       </c>
       <c r="E301" t="n">
-        <v>18.83519422827724</v>
+        <v>19.02052566279252</v>
       </c>
       <c r="F301" t="n">
         <v>30.68243082705255</v>
@@ -8287,10 +8287,10 @@
         <v>1549</v>
       </c>
       <c r="D302" t="n">
-        <v>68.55629314480717</v>
+        <v>69.61470900576256</v>
       </c>
       <c r="E302" t="n">
-        <v>18.14830162211362</v>
+        <v>16.83994466235523</v>
       </c>
       <c r="F302" t="n">
         <v>12.53436163991697</v>
@@ -9301,10 +9301,10 @@
         <v>1372</v>
       </c>
       <c r="D341" t="n">
-        <v>65.87541191693435</v>
+        <v>67.26109390479373</v>
       </c>
       <c r="E341" t="n">
-        <v>17.6511833540895</v>
+        <v>16.06855382052816</v>
       </c>
       <c r="F341" t="n">
         <v>8.375281910007246</v>
@@ -10263,10 +10263,10 @@
         <v>1942</v>
       </c>
       <c r="D378" t="n">
-        <v>58.82247460907869</v>
+        <v>58.79856777479215</v>
       </c>
       <c r="E378" t="n">
-        <v>18.92424940583336</v>
+        <v>19.01613102161937</v>
       </c>
       <c r="F378" t="n">
         <v>30.68243082705255</v>
@@ -10289,10 +10289,10 @@
         <v>1189</v>
       </c>
       <c r="D379" t="n">
-        <v>63.20540153431254</v>
+        <v>63.70341066242521</v>
       </c>
       <c r="E379" t="n">
-        <v>16.93109438345979</v>
+        <v>16.82620365873095</v>
       </c>
       <c r="F379" t="n">
         <v>5.52027813620713</v>
@@ -11225,10 +11225,10 @@
         <v>1928</v>
       </c>
       <c r="D415" t="n">
-        <v>57.90562601780119</v>
+        <v>57.83880180734964</v>
       </c>
       <c r="E415" t="n">
-        <v>18.98266380895964</v>
+        <v>19.03314545073058</v>
       </c>
       <c r="F415" t="n">
         <v>29.71938553256001</v>
@@ -11251,10 +11251,10 @@
         <v>1201</v>
       </c>
       <c r="D416" t="n">
-        <v>63.42839320279649</v>
+        <v>63.89492087584375</v>
       </c>
       <c r="E416" t="n">
-        <v>17.06672113952433</v>
+        <v>16.96707550110039</v>
       </c>
       <c r="F416" t="n">
         <v>5.673255401970756</v>
@@ -11277,10 +11277,10 @@
         <v>1081</v>
       </c>
       <c r="D417" t="n">
-        <v>61.80549405035499</v>
+        <v>62.3840924500289</v>
       </c>
       <c r="E417" t="n">
-        <v>16.37799229373846</v>
+        <v>16.2459381496813</v>
       </c>
       <c r="F417" t="n">
         <v>4.31636916841134</v>
@@ -12187,10 +12187,10 @@
         <v>1960</v>
       </c>
       <c r="D452" t="n">
-        <v>57.82207373386725</v>
+        <v>57.75328657378921</v>
       </c>
       <c r="E452" t="n">
-        <v>18.81628341617511</v>
+        <v>18.87053759036901</v>
       </c>
       <c r="F452" t="n">
         <v>31.96662797725551</v>
@@ -12213,10 +12213,10 @@
         <v>1163</v>
       </c>
       <c r="D453" t="n">
-        <v>63.70966988338012</v>
+        <v>63.65526654810983</v>
       </c>
       <c r="E453" t="n">
-        <v>17.81059857187437</v>
+        <v>16.76862354780967</v>
       </c>
       <c r="F453" t="n">
         <v>5.202830130947101</v>
@@ -13123,10 +13123,10 @@
         <v>1132</v>
       </c>
       <c r="D488" t="n">
-        <v>62.25088317265448</v>
+        <v>62.92566748900271</v>
       </c>
       <c r="E488" t="n">
-        <v>17.24574397479953</v>
+        <v>16.75786771245271</v>
       </c>
       <c r="F488" t="n">
         <v>4.84810399337989</v>
@@ -14007,10 +14007,10 @@
         <v>1151</v>
       </c>
       <c r="D522" t="n">
-        <v>62.28554212500831</v>
+        <v>63.35635613288849</v>
       </c>
       <c r="E522" t="n">
-        <v>17.66913982919254</v>
+        <v>17.16211549676107</v>
       </c>
       <c r="F522" t="n">
         <v>5.062537711291816</v>
@@ -14033,10 +14033,10 @@
         <v>1077</v>
       </c>
       <c r="D523" t="n">
-        <v>61.63338481910735</v>
+        <v>62.08274056163786</v>
       </c>
       <c r="E523" t="n">
-        <v>17.09609695393247</v>
+        <v>16.77123043291521</v>
       </c>
       <c r="F523" t="n">
         <v>4.277218697287138</v>
@@ -14995,7 +14995,7 @@
         <v>1294</v>
       </c>
       <c r="D560" t="n">
-        <v>61.97777230128749</v>
+        <v>58.98041658335296</v>
       </c>
       <c r="E560" t="n">
         <v>20.19082026778604</v>
@@ -15593,10 +15593,10 @@
         <v>1996</v>
       </c>
       <c r="D583" t="n">
-        <v>58.02801387185088</v>
+        <v>57.89722361698314</v>
       </c>
       <c r="E583" t="n">
-        <v>18.41611116830832</v>
+        <v>18.36812165815569</v>
       </c>
       <c r="F583" t="n">
         <v>34.69852013803012</v>
@@ -15671,10 +15671,10 @@
         <v>1262</v>
       </c>
       <c r="D586" t="n">
-        <v>62.43945666860739</v>
+        <v>59.71515091277792</v>
       </c>
       <c r="E586" t="n">
-        <v>19.65879497563017</v>
+        <v>22.07441794820184</v>
       </c>
       <c r="F586" t="n">
         <v>6.51896265938313</v>
@@ -16165,10 +16165,10 @@
         <v>1512</v>
       </c>
       <c r="D605" t="n">
-        <v>57.41724379013694</v>
+        <v>58.57171488597541</v>
       </c>
       <c r="E605" t="n">
-        <v>19.60974488156421</v>
+        <v>19.27606475575205</v>
       </c>
       <c r="F605" t="n">
         <v>11.52122911934112</v>
@@ -16191,10 +16191,10 @@
         <v>1618</v>
       </c>
       <c r="D606" t="n">
-        <v>57.46354673666112</v>
+        <v>58.2996961446638</v>
       </c>
       <c r="E606" t="n">
-        <v>19.35657346450953</v>
+        <v>19.01300210114766</v>
       </c>
       <c r="F606" t="n">
         <v>14.66772061428879</v>
@@ -16217,10 +16217,10 @@
         <v>1757</v>
       </c>
       <c r="D607" t="n">
-        <v>57.61622830907319</v>
+        <v>58.07297615747071</v>
       </c>
       <c r="E607" t="n">
-        <v>19.07099979115244</v>
+        <v>18.74471546109439</v>
       </c>
       <c r="F607" t="n">
         <v>20.13134200466594</v>
@@ -16243,10 +16243,10 @@
         <v>1971</v>
       </c>
       <c r="D608" t="n">
-        <v>57.80226079987357</v>
+        <v>57.88402339375534</v>
       </c>
       <c r="E608" t="n">
-        <v>18.53719487693752</v>
+        <v>18.3518464237492</v>
       </c>
       <c r="F608" t="n">
         <v>32.7777335776402</v>
@@ -16295,10 +16295,10 @@
         <v>1161</v>
       </c>
       <c r="D610" t="n">
-        <v>55.38595017904587</v>
+        <v>55.66259350305215</v>
       </c>
       <c r="E610" t="n">
-        <v>27.48715136738279</v>
+        <v>27.65985484710795</v>
       </c>
       <c r="F610" t="n">
         <v>5.179180943890193</v>
@@ -16685,10 +16685,10 @@
         <v>1499</v>
       </c>
       <c r="D625" t="n">
-        <v>57.57737767281495</v>
+        <v>58.24947725442809</v>
       </c>
       <c r="E625" t="n">
-        <v>19.59627744351626</v>
+        <v>19.97939436215322</v>
       </c>
       <c r="F625" t="n">
         <v>11.18505584412895</v>
@@ -16711,10 +16711,10 @@
         <v>1481</v>
       </c>
       <c r="D626" t="n">
-        <v>57.4973201749912</v>
+        <v>58.31435159261801</v>
       </c>
       <c r="E626" t="n">
-        <v>19.73311296038194</v>
+        <v>20.19463019487145</v>
       </c>
       <c r="F626" t="n">
         <v>10.73571796432157</v>
@@ -16737,10 +16737,10 @@
         <v>1560</v>
       </c>
       <c r="D627" t="n">
-        <v>57.49674188682766</v>
+        <v>58.48081849812072</v>
       </c>
       <c r="E627" t="n">
-        <v>19.51869536080924</v>
+        <v>19.1526438073553</v>
       </c>
       <c r="F627" t="n">
         <v>12.85240240826506</v>
@@ -16763,10 +16763,10 @@
         <v>1676</v>
       </c>
       <c r="D628" t="n">
-        <v>57.57572241224318</v>
+        <v>58.20819818162575</v>
       </c>
       <c r="E628" t="n">
-        <v>19.2305285727791</v>
+        <v>18.85914363867333</v>
       </c>
       <c r="F628" t="n">
         <v>16.7394407041348</v>
@@ -16789,10 +16789,10 @@
         <v>1829</v>
       </c>
       <c r="D629" t="n">
-        <v>57.75920502743733</v>
+        <v>57.95338406731646</v>
       </c>
       <c r="E629" t="n">
-        <v>18.88012421627396</v>
+        <v>18.52432990235865</v>
       </c>
       <c r="F629" t="n">
         <v>23.71925145168238</v>
@@ -16815,10 +16815,10 @@
         <v>1984</v>
       </c>
       <c r="D630" t="n">
-        <v>57.72827935825426</v>
+        <v>57.80151029624193</v>
       </c>
       <c r="E630" t="n">
-        <v>18.39126904328696</v>
+        <v>18.23124464468165</v>
       </c>
       <c r="F630" t="n">
         <v>33.76288717940884</v>
@@ -16841,10 +16841,10 @@
         <v>1203</v>
       </c>
       <c r="D631" t="n">
-        <v>56.73091404963726</v>
+        <v>56.8183641552979</v>
       </c>
       <c r="E631" t="n">
-        <v>24.91677749602798</v>
+        <v>25.67918840551333</v>
       </c>
       <c r="F631" t="n">
         <v>5.699160632870458</v>
@@ -16867,10 +16867,10 @@
         <v>1257</v>
       </c>
       <c r="D632" t="n">
-        <v>57.20101271276655</v>
+        <v>57.1160308692691</v>
       </c>
       <c r="E632" t="n">
-        <v>23.77228217602386</v>
+        <v>23.72543147373089</v>
       </c>
       <c r="F632" t="n">
         <v>6.445136016249622</v>
@@ -16893,10 +16893,10 @@
         <v>1343</v>
       </c>
       <c r="D633" t="n">
-        <v>57.88634934907101</v>
+        <v>57.19202503577503</v>
       </c>
       <c r="E633" t="n">
-        <v>21.63926859695256</v>
+        <v>22.53305247491419</v>
       </c>
       <c r="F633" t="n">
         <v>7.839895557518359</v>
@@ -16919,10 +16919,10 @@
         <v>1368</v>
       </c>
       <c r="D634" t="n">
-        <v>57.61944829800544</v>
+        <v>57.50721693457161</v>
       </c>
       <c r="E634" t="n">
-        <v>20.79646123675056</v>
+        <v>21.22643690293193</v>
       </c>
       <c r="F634" t="n">
         <v>8.299316157361607</v>
@@ -16945,7 +16945,7 @@
         <v>1413</v>
       </c>
       <c r="D635" t="n">
-        <v>57.69405815682249</v>
+        <v>57.59850741609011</v>
       </c>
       <c r="E635" t="n">
         <v>23.98621527971164</v>
@@ -17127,10 +17127,10 @@
         <v>1342</v>
       </c>
       <c r="D642" t="n">
-        <v>57.79569894494253</v>
+        <v>57.48755219180939</v>
       </c>
       <c r="E642" t="n">
-        <v>18.97547122574302</v>
+        <v>19.54210259894859</v>
       </c>
       <c r="F642" t="n">
         <v>7.822057350074957</v>
@@ -17179,10 +17179,10 @@
         <v>1558</v>
       </c>
       <c r="D644" t="n">
-        <v>57.65469754015997</v>
+        <v>57.99759639416124</v>
       </c>
       <c r="E644" t="n">
-        <v>19.22203784134728</v>
+        <v>19.4185784953834</v>
       </c>
       <c r="F644" t="n">
         <v>12.79398249813273</v>
@@ -17205,10 +17205,10 @@
         <v>1592</v>
       </c>
       <c r="D645" t="n">
-        <v>57.64077226383403</v>
+        <v>57.97578908339293</v>
       </c>
       <c r="E645" t="n">
-        <v>19.24357672294941</v>
+        <v>19.43619694696277</v>
       </c>
       <c r="F645" t="n">
         <v>13.82424161996467</v>
@@ -17231,10 +17231,10 @@
         <v>1552</v>
       </c>
       <c r="D646" t="n">
-        <v>57.5632397682973</v>
+        <v>58.13030104730902</v>
       </c>
       <c r="E646" t="n">
-        <v>19.50324938198656</v>
+        <v>19.82884029374973</v>
       </c>
       <c r="F646" t="n">
         <v>12.62031121267397</v>
@@ -17257,10 +17257,10 @@
         <v>1631</v>
       </c>
       <c r="D647" t="n">
-        <v>57.59205843226643</v>
+        <v>58.30042124583417</v>
       </c>
       <c r="E647" t="n">
-        <v>19.31466695693414</v>
+        <v>18.90172961826898</v>
       </c>
       <c r="F647" t="n">
         <v>15.10856737871425</v>
@@ -17283,10 +17283,10 @@
         <v>1765</v>
       </c>
       <c r="D648" t="n">
-        <v>57.71552830054058</v>
+        <v>58.00538268909375</v>
       </c>
       <c r="E648" t="n">
-        <v>18.97200699706279</v>
+        <v>18.55739941995035</v>
       </c>
       <c r="F648" t="n">
         <v>20.50156324215997</v>
@@ -17309,10 +17309,10 @@
         <v>1890</v>
       </c>
       <c r="D649" t="n">
-        <v>57.67562956087452</v>
+        <v>57.80958659582078</v>
       </c>
       <c r="E649" t="n">
-        <v>18.57335692059062</v>
+        <v>18.29248807573222</v>
       </c>
       <c r="F649" t="n">
         <v>27.25505967320341</v>
@@ -17335,10 +17335,10 @@
         <v>1888</v>
       </c>
       <c r="D650" t="n">
-        <v>57.76536836348087</v>
+        <v>57.90575711311406</v>
       </c>
       <c r="E650" t="n">
-        <v>18.71739553435226</v>
+        <v>18.41940382408047</v>
       </c>
       <c r="F650" t="n">
         <v>27.13117325211409</v>
@@ -17361,10 +17361,10 @@
         <v>1341</v>
       </c>
       <c r="D651" t="n">
-        <v>57.68372719891082</v>
+        <v>57.36068813726115</v>
       </c>
       <c r="E651" t="n">
-        <v>22.2236979054227</v>
+        <v>22.01556856497956</v>
       </c>
       <c r="F651" t="n">
         <v>7.804259730116742</v>
@@ -17387,10 +17387,10 @@
         <v>1451</v>
       </c>
       <c r="D652" t="n">
-        <v>58.11729006966874</v>
+        <v>57.18597677727129</v>
       </c>
       <c r="E652" t="n">
-        <v>20.57827990956909</v>
+        <v>21.01597484166934</v>
       </c>
       <c r="F652" t="n">
         <v>10.02657612167238</v>
@@ -17413,10 +17413,10 @@
         <v>1486</v>
       </c>
       <c r="D653" t="n">
-        <v>57.56455993794844</v>
+        <v>57.36665351867472</v>
       </c>
       <c r="E653" t="n">
-        <v>20.05729417413152</v>
+        <v>19.9009484939824</v>
       </c>
       <c r="F653" t="n">
         <v>10.85869163267173</v>
@@ -17439,10 +17439,10 @@
         <v>1342</v>
       </c>
       <c r="D654" t="n">
-        <v>58.50902311312322</v>
+        <v>58.05033505249033</v>
       </c>
       <c r="E654" t="n">
-        <v>18.68257599796874</v>
+        <v>19.26163784644503</v>
       </c>
       <c r="F654" t="n">
         <v>7.822057350074957</v>
@@ -17491,10 +17491,10 @@
         <v>1293</v>
       </c>
       <c r="D656" t="n">
-        <v>58.16755866503992</v>
+        <v>57.39154235192004</v>
       </c>
       <c r="E656" t="n">
-        <v>18.29621417437932</v>
+        <v>19.00607967495202</v>
       </c>
       <c r="F656" t="n">
         <v>6.995942206081283</v>
@@ -17517,10 +17517,10 @@
         <v>1279</v>
       </c>
       <c r="D657" t="n">
-        <v>58.20814621560186</v>
+        <v>57.29476845741911</v>
       </c>
       <c r="E657" t="n">
-        <v>18.56151679399522</v>
+        <v>19.44125222297057</v>
       </c>
       <c r="F657" t="n">
         <v>6.776356956787151</v>
@@ -17543,10 +17543,10 @@
         <v>1306</v>
       </c>
       <c r="D658" t="n">
-        <v>57.846200760596</v>
+        <v>58.4822154213701</v>
       </c>
       <c r="E658" t="n">
-        <v>19.10611581633344</v>
+        <v>20.34216679880559</v>
       </c>
       <c r="F658" t="n">
         <v>7.206209265753393</v>
@@ -17569,10 +17569,10 @@
         <v>1405</v>
       </c>
       <c r="D659" t="n">
-        <v>57.5664817258535</v>
+        <v>58.34718806932239</v>
       </c>
       <c r="E659" t="n">
-        <v>19.66133471638799</v>
+        <v>20.10421242451155</v>
       </c>
       <c r="F659" t="n">
         <v>9.029126059627012</v>
@@ -17595,10 +17595,10 @@
         <v>1534</v>
       </c>
       <c r="D660" t="n">
-        <v>57.64156188568919</v>
+        <v>58.0684065109042</v>
       </c>
       <c r="E660" t="n">
-        <v>19.33629186768373</v>
+        <v>19.58283304952002</v>
       </c>
       <c r="F660" t="n">
         <v>12.11331473792781</v>
@@ -17621,10 +17621,10 @@
         <v>1670</v>
       </c>
       <c r="D661" t="n">
-        <v>57.72143262860116</v>
+        <v>57.77768639150777</v>
       </c>
       <c r="E661" t="n">
-        <v>18.96766171883933</v>
+        <v>19.00043210213625</v>
       </c>
       <c r="F661" t="n">
         <v>16.51221199052884</v>
@@ -17647,10 +17647,10 @@
         <v>1703</v>
       </c>
       <c r="D662" t="n">
-        <v>57.72029456085991</v>
+        <v>57.7685750923875</v>
       </c>
       <c r="E662" t="n">
-        <v>18.97885546762417</v>
+        <v>19.00705478846246</v>
       </c>
       <c r="F662" t="n">
         <v>17.80129256397061</v>
@@ -17673,10 +17673,10 @@
         <v>1779</v>
       </c>
       <c r="D663" t="n">
-        <v>57.77710663072835</v>
+        <v>57.88767827553526</v>
       </c>
       <c r="E663" t="n">
-        <v>18.82852254780527</v>
+        <v>18.34224662522951</v>
       </c>
       <c r="F663" t="n">
         <v>21.16590853922112</v>
@@ -17699,10 +17699,10 @@
         <v>1898</v>
       </c>
       <c r="D664" t="n">
-        <v>57.53722495755532</v>
+        <v>57.66235604266959</v>
       </c>
       <c r="E664" t="n">
-        <v>18.32396452805774</v>
+        <v>18.06917194546298</v>
       </c>
       <c r="F664" t="n">
         <v>27.75628815155564</v>
@@ -17725,10 +17725,10 @@
         <v>1974</v>
       </c>
       <c r="D665" t="n">
-        <v>57.51178400705584</v>
+        <v>57.58380175225381</v>
       </c>
       <c r="E665" t="n">
-        <v>18.10649091490864</v>
+        <v>17.95837310950051</v>
       </c>
       <c r="F665" t="n">
         <v>33.00249430163028</v>
@@ -17751,10 +17751,10 @@
         <v>1414</v>
       </c>
       <c r="D666" t="n">
-        <v>58.61562313962604</v>
+        <v>58.4035780145998</v>
       </c>
       <c r="E666" t="n">
-        <v>18.59695311179135</v>
+        <v>18.87567873475066</v>
       </c>
       <c r="F666" t="n">
         <v>9.216143916928457</v>
@@ -17777,10 +17777,10 @@
         <v>1392</v>
       </c>
       <c r="D667" t="n">
-        <v>58.40940321698606</v>
+        <v>58.56397318321947</v>
       </c>
       <c r="E667" t="n">
-        <v>18.58506857786704</v>
+        <v>19.21512176105821</v>
       </c>
       <c r="F667" t="n">
         <v>8.765668849608272</v>
@@ -17803,10 +17803,10 @@
         <v>1350</v>
       </c>
       <c r="D668" t="n">
-        <v>58.06372804444833</v>
+        <v>58.24371838125079</v>
       </c>
       <c r="E668" t="n">
-        <v>18.91178574659019</v>
+        <v>19.93011335828557</v>
       </c>
       <c r="F668" t="n">
         <v>7.965907260886808</v>
@@ -17829,10 +17829,10 @@
         <v>1393</v>
       </c>
       <c r="D669" t="n">
-        <v>57.59579662113244</v>
+        <v>58.03118068493935</v>
       </c>
       <c r="E669" t="n">
-        <v>19.59256849883225</v>
+        <v>19.90663332514168</v>
       </c>
       <c r="F669" t="n">
         <v>8.785658963758733</v>
@@ -17855,10 +17855,10 @@
         <v>1470</v>
       </c>
       <c r="D670" t="n">
-        <v>57.62847563558682</v>
+        <v>58.19751172556503</v>
       </c>
       <c r="E670" t="n">
-        <v>19.47715290013103</v>
+        <v>19.80736416268025</v>
       </c>
       <c r="F670" t="n">
         <v>10.4700558817256</v>
@@ -17881,10 +17881,10 @@
         <v>1567</v>
       </c>
       <c r="D671" t="n">
-        <v>57.6773227080633</v>
+        <v>57.99416744025302</v>
       </c>
       <c r="E671" t="n">
-        <v>19.25585291906678</v>
+        <v>19.44207285214464</v>
       </c>
       <c r="F671" t="n">
         <v>13.05898081329102</v>
@@ -17907,10 +17907,10 @@
         <v>1681</v>
       </c>
       <c r="D672" t="n">
-        <v>57.74973618342094</v>
+        <v>57.76134348208351</v>
       </c>
       <c r="E672" t="n">
-        <v>18.95847525785306</v>
+        <v>18.96535063336582</v>
       </c>
       <c r="F672" t="n">
         <v>16.93118479021815</v>
@@ -17933,10 +17933,10 @@
         <v>1823</v>
       </c>
       <c r="D673" t="n">
-        <v>57.87338613874467</v>
+        <v>57.67345964799773</v>
       </c>
       <c r="E673" t="n">
-        <v>18.56645780711894</v>
+        <v>17.99504875741379</v>
       </c>
       <c r="F673" t="n">
         <v>23.39727564076234</v>
@@ -17959,10 +17959,10 @@
         <v>1906</v>
       </c>
       <c r="D674" t="n">
-        <v>57.40935904386188</v>
+        <v>57.52349606289148</v>
       </c>
       <c r="E674" t="n">
-        <v>18.07058479279319</v>
+        <v>17.84225648674823</v>
       </c>
       <c r="F674" t="n">
         <v>28.26673436747747</v>
@@ -17985,10 +17985,10 @@
         <v>1979</v>
       </c>
       <c r="D675" t="n">
-        <v>57.36491429147085</v>
+        <v>57.42574759985252</v>
       </c>
       <c r="E675" t="n">
-        <v>17.85412056555164</v>
+        <v>17.73178968179691</v>
       </c>
       <c r="F675" t="n">
         <v>33.38052563614038</v>
@@ -18011,10 +18011,10 @@
         <v>1479</v>
       </c>
       <c r="D676" t="n">
-        <v>58.00354656095169</v>
+        <v>58.30528368413417</v>
       </c>
       <c r="E676" t="n">
-        <v>18.88911093797135</v>
+        <v>18.9324233069638</v>
       </c>
       <c r="F676" t="n">
         <v>10.68691933051297</v>
@@ -18037,10 +18037,10 @@
         <v>1503</v>
       </c>
       <c r="D677" t="n">
-        <v>57.72749300050626</v>
+        <v>57.57607543294424</v>
       </c>
       <c r="E677" t="n">
-        <v>19.31106977303294</v>
+        <v>19.36273980932637</v>
       </c>
       <c r="F677" t="n">
         <v>11.28743550643752</v>
@@ -18063,10 +18063,10 @@
         <v>1605</v>
       </c>
       <c r="D678" t="n">
-        <v>57.77623764382836</v>
+        <v>57.09673200659764</v>
       </c>
       <c r="E678" t="n">
-        <v>19.03553686761028</v>
+        <v>18.87562949366045</v>
       </c>
       <c r="F678" t="n">
         <v>14.23973713893851</v>
@@ -18089,10 +18089,10 @@
         <v>1702</v>
       </c>
       <c r="D679" t="n">
-        <v>57.82922452092546</v>
+        <v>57.66691527119374</v>
       </c>
       <c r="E679" t="n">
-        <v>18.79240897955089</v>
+        <v>18.69457955348219</v>
       </c>
       <c r="F679" t="n">
         <v>17.76078907164893</v>

</xml_diff>